<commit_message>
Decrease the number of workers and fix the name of one Measure class
</commit_message>
<xml_diff>
--- a/projects/PTool_Full_Analysis.xlsx
+++ b/projects/PTool_Full_Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="5244" windowWidth="22368" windowHeight="5268" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="-12" yWindow="5244" windowWidth="22368" windowHeight="5268" tabRatio="469" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Variables" sheetId="2" r:id="rId3"/>
     <sheet name="Outputs" sheetId="12" r:id="rId4"/>
     <sheet name="Lookups" sheetId="11" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="14" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="645">
   <si>
     <t>type</t>
   </si>
@@ -950,9 +949,6 @@
     <t>in H2O</t>
   </si>
   <si>
-    <t>Add Hot Water Pump Differential Pressure Reset Controls</t>
-  </si>
-  <si>
     <t>Advanced Power Strips</t>
   </si>
   <si>
@@ -1085,9 +1081,6 @@
     <t>occ_threshold</t>
   </si>
   <si>
-    <t>ReplaceDesktopsWithThinClients</t>
-  </si>
-  <si>
     <t>Solar Cogeneration And Daylighting</t>
   </si>
   <si>
@@ -1971,6 +1964,12 @@
   </si>
   <si>
     <t>["ASHRAE 169-2006-2A","ASHRAE 169-2006-3B","ASHRAE 169-2006-4A","ASHRAE 169-2006-5A"]</t>
+  </si>
+  <si>
+    <t>DesktopsToThinClients</t>
+  </si>
+  <si>
+    <t>Hot Water Pump Differential Pressure Reset</t>
   </si>
 </sst>
 </file>
@@ -6708,7 +6707,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6755,7 +6754,7 @@
         <v>81</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>82</v>
@@ -6766,7 +6765,7 @@
         <v>94</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>178</v>
@@ -6777,7 +6776,7 @@
         <v>95</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>97</v>
@@ -6826,7 +6825,7 @@
         <v>83</v>
       </c>
       <c r="B9" s="24">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="31"/>
@@ -6848,7 +6847,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>96</v>
@@ -6954,7 +6953,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="25"/>
       <c r="D23" s="2"/>
     </row>
@@ -7088,7 +7087,7 @@
         <v>198</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>232</v>
@@ -7143,9 +7142,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P5" sqref="P5"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7270,7 +7269,7 @@
         <v>8</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="P3" s="16" t="s">
         <v>100</v>
@@ -7342,7 +7341,7 @@
         <v>263</v>
       </c>
       <c r="P5" s="30" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="R5" s="30" t="s">
         <v>254</v>
@@ -7380,7 +7379,7 @@
         <v>245</v>
       </c>
       <c r="P6" s="30" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="R6" s="30" t="s">
         <v>254</v>
@@ -7418,7 +7417,7 @@
         <v>250</v>
       </c>
       <c r="P7" s="44" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="R7" s="30" t="s">
         <v>254</v>
@@ -7429,13 +7428,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>46</v>
@@ -7488,13 +7487,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>306</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>46</v>
@@ -7759,13 +7758,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>48</v>
@@ -7818,13 +7817,13 @@
         <v>1</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>46</v>
@@ -7879,10 +7878,10 @@
       </c>
       <c r="C26" s="56"/>
       <c r="D26" s="56" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E26" s="56" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="G26" s="56" t="s">
         <v>44</v>
@@ -7901,10 +7900,10 @@
       </c>
       <c r="C27" s="56"/>
       <c r="D27" s="56" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E27" s="56" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="G27" s="56" t="s">
         <v>44</v>
@@ -7921,10 +7920,10 @@
       </c>
       <c r="C28" s="56"/>
       <c r="D28" s="56" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E28" s="56" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="G28" s="56" t="s">
         <v>44</v>
@@ -7939,13 +7938,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>46</v>
@@ -8000,10 +7999,10 @@
       </c>
       <c r="C31" s="56"/>
       <c r="D31" s="56" t="s">
+        <v>307</v>
+      </c>
+      <c r="E31" s="56" t="s">
         <v>308</v>
-      </c>
-      <c r="E31" s="56" t="s">
-        <v>309</v>
       </c>
       <c r="G31" s="56" t="s">
         <v>44</v>
@@ -8020,13 +8019,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>46</v>
@@ -8079,13 +8078,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>310</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>311</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>46</v>
@@ -8138,13 +8137,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>312</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>313</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>46</v>
@@ -8197,13 +8196,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>314</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>315</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>46</v>
@@ -8256,13 +8255,13 @@
         <v>1</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>46</v>
@@ -8315,13 +8314,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>46</v>
@@ -8374,13 +8373,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>48</v>
@@ -8433,13 +8432,13 @@
         <v>1</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>316</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>317</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>46</v>
@@ -8704,13 +8703,13 @@
         <v>1</v>
       </c>
       <c r="B58" s="52" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D58" s="52" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E58" s="52" t="s">
         <v>46</v>
@@ -8765,10 +8764,10 @@
       </c>
       <c r="C60" s="59"/>
       <c r="D60" s="59" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E60" s="59" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G60" s="59" t="s">
         <v>44</v>
@@ -8785,10 +8784,10 @@
       </c>
       <c r="C61" s="59"/>
       <c r="D61" s="59" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E61" s="59" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G61" s="59" t="s">
         <v>44</v>
@@ -8805,10 +8804,10 @@
       </c>
       <c r="C62" s="59"/>
       <c r="D62" s="59" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E62" s="59" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G62" s="59" t="s">
         <v>44</v>
@@ -8823,13 +8822,13 @@
         <v>1</v>
       </c>
       <c r="B63" s="52" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C63" s="52" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D63" s="52" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E63" s="52" t="s">
         <v>46</v>
@@ -8882,13 +8881,13 @@
         <v>1</v>
       </c>
       <c r="B65" s="52" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C65" s="52" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D65" s="52" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E65" s="52" t="s">
         <v>46</v>
@@ -8941,13 +8940,13 @@
         <v>1</v>
       </c>
       <c r="B67" s="52" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C67" s="52" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D67" s="52" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E67" s="52" t="s">
         <v>46</v>
@@ -9000,13 +8999,13 @@
         <v>1</v>
       </c>
       <c r="B69" s="52" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C69" s="52" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D69" s="52" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E69" s="52" t="s">
         <v>46</v>
@@ -9059,13 +9058,13 @@
         <v>1</v>
       </c>
       <c r="B71" s="52" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C71" s="52" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D71" s="52" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E71" s="52" t="s">
         <v>46</v>
@@ -9118,13 +9117,13 @@
         <v>1</v>
       </c>
       <c r="B73" s="52" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C73" s="52" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D73" s="52" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E73" s="52" t="s">
         <v>46</v>
@@ -9177,13 +9176,13 @@
         <v>1</v>
       </c>
       <c r="B75" s="52" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C75" s="52" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D75" s="52" t="s">
-        <v>349</v>
+        <v>643</v>
       </c>
       <c r="E75" s="52" t="s">
         <v>46</v>
@@ -9236,13 +9235,13 @@
         <v>1</v>
       </c>
       <c r="B77" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="C77" s="52" t="s">
+        <v>382</v>
+      </c>
+      <c r="D77" s="52" t="s">
         <v>319</v>
-      </c>
-      <c r="C77" s="52" t="s">
-        <v>384</v>
-      </c>
-      <c r="D77" s="52" t="s">
-        <v>320</v>
       </c>
       <c r="E77" s="52" t="s">
         <v>46</v>
@@ -9507,13 +9506,13 @@
         <v>1</v>
       </c>
       <c r="B89" s="52" t="s">
+        <v>320</v>
+      </c>
+      <c r="C89" s="52" t="s">
+        <v>383</v>
+      </c>
+      <c r="D89" s="52" t="s">
         <v>321</v>
-      </c>
-      <c r="C89" s="52" t="s">
-        <v>385</v>
-      </c>
-      <c r="D89" s="52" t="s">
-        <v>322</v>
       </c>
       <c r="E89" s="52" t="s">
         <v>46</v>
@@ -9778,13 +9777,13 @@
         <v>1</v>
       </c>
       <c r="B101" s="50" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C101" s="50" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D101" s="50" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E101" s="50" t="s">
         <v>46</v>
@@ -9837,13 +9836,13 @@
         <v>1</v>
       </c>
       <c r="B103" s="50" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C103" s="50" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D103" s="50" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E103" s="50" t="s">
         <v>46</v>
@@ -9918,13 +9917,13 @@
         <v>1</v>
       </c>
       <c r="B106" s="50" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C106" s="50" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D106" s="50" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E106" s="50" t="s">
         <v>48</v>
@@ -9977,13 +9976,13 @@
         <v>1</v>
       </c>
       <c r="B108" s="50" t="s">
+        <v>322</v>
+      </c>
+      <c r="C108" s="50" t="s">
+        <v>384</v>
+      </c>
+      <c r="D108" s="50" t="s">
         <v>323</v>
-      </c>
-      <c r="C108" s="50" t="s">
-        <v>386</v>
-      </c>
-      <c r="D108" s="50" t="s">
-        <v>324</v>
       </c>
       <c r="E108" s="50" t="s">
         <v>46</v>
@@ -10036,13 +10035,13 @@
         <v>1</v>
       </c>
       <c r="B110" s="50" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C110" s="50" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D110" s="50" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E110" s="50" t="s">
         <v>46</v>
@@ -10277,13 +10276,13 @@
         <v>1</v>
       </c>
       <c r="B121" s="50" t="s">
+        <v>324</v>
+      </c>
+      <c r="C121" s="50" t="s">
+        <v>385</v>
+      </c>
+      <c r="D121" s="50" t="s">
         <v>325</v>
-      </c>
-      <c r="C121" s="50" t="s">
-        <v>387</v>
-      </c>
-      <c r="D121" s="50" t="s">
-        <v>326</v>
       </c>
       <c r="E121" s="50" t="s">
         <v>46</v>
@@ -10336,13 +10335,13 @@
         <v>1</v>
       </c>
       <c r="B123" s="50" t="s">
+        <v>326</v>
+      </c>
+      <c r="C123" s="50" t="s">
+        <v>386</v>
+      </c>
+      <c r="D123" s="50" t="s">
         <v>327</v>
-      </c>
-      <c r="C123" s="50" t="s">
-        <v>388</v>
-      </c>
-      <c r="D123" s="50" t="s">
-        <v>328</v>
       </c>
       <c r="E123" s="50" t="s">
         <v>46</v>
@@ -10395,13 +10394,13 @@
         <v>1</v>
       </c>
       <c r="B125" s="50" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C125" s="50" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D125" s="50" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E125" s="50" t="s">
         <v>48</v>
@@ -10454,13 +10453,13 @@
         <v>1</v>
       </c>
       <c r="B127" s="50" t="s">
-        <v>304</v>
+        <v>644</v>
       </c>
       <c r="C127" s="50" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D127" s="50" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E127" s="50" t="s">
         <v>46</v>
@@ -10475,7 +10474,7 @@
       <c r="C128" s="61"/>
       <c r="D128" s="61" t="str">
         <f>"Run Measure " &amp; B127</f>
-        <v>Run Measure Add Hot Water Pump Differential Pressure Reset Controls</v>
+        <v>Run Measure Hot Water Pump Differential Pressure Reset</v>
       </c>
       <c r="E128" s="61" t="s">
         <v>257</v>
@@ -10513,13 +10512,13 @@
         <v>1</v>
       </c>
       <c r="B129" s="50" t="s">
+        <v>328</v>
+      </c>
+      <c r="C129" s="50" t="s">
+        <v>406</v>
+      </c>
+      <c r="D129" s="50" t="s">
         <v>329</v>
-      </c>
-      <c r="C129" s="50" t="s">
-        <v>408</v>
-      </c>
-      <c r="D129" s="50" t="s">
-        <v>330</v>
       </c>
       <c r="E129" s="50" t="s">
         <v>46</v>
@@ -10572,13 +10571,13 @@
         <v>1</v>
       </c>
       <c r="B131" s="50" t="s">
+        <v>330</v>
+      </c>
+      <c r="C131" s="50" t="s">
+        <v>407</v>
+      </c>
+      <c r="D131" s="50" t="s">
         <v>331</v>
-      </c>
-      <c r="C131" s="50" t="s">
-        <v>409</v>
-      </c>
-      <c r="D131" s="50" t="s">
-        <v>332</v>
       </c>
       <c r="E131" s="50" t="s">
         <v>46</v>
@@ -10633,10 +10632,10 @@
       </c>
       <c r="C133" s="61"/>
       <c r="D133" s="61" t="s">
+        <v>332</v>
+      </c>
+      <c r="E133" s="61" t="s">
         <v>333</v>
-      </c>
-      <c r="E133" s="61" t="s">
-        <v>334</v>
       </c>
       <c r="G133" s="61" t="s">
         <v>44</v>
@@ -10653,13 +10652,13 @@
         <v>1</v>
       </c>
       <c r="B134" s="50" t="s">
+        <v>334</v>
+      </c>
+      <c r="C134" s="50" t="s">
+        <v>408</v>
+      </c>
+      <c r="D134" s="50" t="s">
         <v>335</v>
-      </c>
-      <c r="C134" s="50" t="s">
-        <v>410</v>
-      </c>
-      <c r="D134" s="50" t="s">
-        <v>336</v>
       </c>
       <c r="E134" s="50" t="s">
         <v>46</v>
@@ -10714,16 +10713,16 @@
       </c>
       <c r="C136" s="61"/>
       <c r="D136" s="61" t="s">
+        <v>336</v>
+      </c>
+      <c r="E136" s="61" t="s">
         <v>337</v>
-      </c>
-      <c r="E136" s="61" t="s">
-        <v>338</v>
       </c>
       <c r="G136" s="61" t="s">
         <v>44</v>
       </c>
       <c r="H136" s="61" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I136" s="61">
         <v>0.5</v>
@@ -10734,13 +10733,13 @@
         <v>1</v>
       </c>
       <c r="B137" s="50" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C137" s="50" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D137" s="50" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E137" s="50" t="s">
         <v>48</v>
@@ -10793,13 +10792,13 @@
         <v>1</v>
       </c>
       <c r="B139" s="50" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C139" s="50" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D139" s="50" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E139" s="50" t="s">
         <v>48</v>
@@ -10852,13 +10851,13 @@
         <v>1</v>
       </c>
       <c r="B141" s="58" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C141" s="58" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="D141" s="58" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E141" s="58" t="s">
         <v>46</v>
@@ -10911,13 +10910,13 @@
         <v>1</v>
       </c>
       <c r="B143" s="58" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C143" s="58" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D143" s="58" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E143" s="58" t="s">
         <v>48</v>
@@ -10970,13 +10969,13 @@
         <v>1</v>
       </c>
       <c r="B145" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="C145" s="58" t="s">
+        <v>409</v>
+      </c>
+      <c r="D145" s="58" t="s">
         <v>340</v>
-      </c>
-      <c r="C145" s="58" t="s">
-        <v>411</v>
-      </c>
-      <c r="D145" s="58" t="s">
-        <v>341</v>
       </c>
       <c r="E145" s="58" t="s">
         <v>46</v>
@@ -11241,13 +11240,13 @@
         <v>1</v>
       </c>
       <c r="B157" s="58" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C157" s="58" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D157" s="58" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E157" s="58" t="s">
         <v>48</v>
@@ -11300,13 +11299,13 @@
         <v>1</v>
       </c>
       <c r="B159" s="58" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C159" s="58" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D159" s="58" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E159" s="58" t="s">
         <v>46</v>
@@ -11570,13 +11569,13 @@
         <v>1</v>
       </c>
       <c r="B171" s="58" t="s">
+        <v>342</v>
+      </c>
+      <c r="C171" s="58" t="s">
+        <v>411</v>
+      </c>
+      <c r="D171" s="58" t="s">
         <v>343</v>
-      </c>
-      <c r="C171" s="58" t="s">
-        <v>413</v>
-      </c>
-      <c r="D171" s="58" t="s">
-        <v>344</v>
       </c>
       <c r="E171" s="58" t="s">
         <v>46</v>
@@ -11629,13 +11628,13 @@
         <v>1</v>
       </c>
       <c r="B173" s="58" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C173" s="58" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D173" s="58" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E173" s="58" t="s">
         <v>46</v>
@@ -11690,10 +11689,10 @@
       </c>
       <c r="C175" s="62"/>
       <c r="D175" s="62" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E175" s="62" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="G175" s="62" t="s">
         <v>44</v>
@@ -11710,10 +11709,10 @@
       </c>
       <c r="C176" s="62"/>
       <c r="D176" s="62" t="s">
+        <v>576</v>
+      </c>
+      <c r="E176" s="62" t="s">
         <v>578</v>
-      </c>
-      <c r="E176" s="62" t="s">
-        <v>580</v>
       </c>
       <c r="G176" s="62" t="s">
         <v>44</v>
@@ -11750,7 +11749,7 @@
       </c>
       <c r="C178" s="62"/>
       <c r="D178" s="62" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E178" s="62" t="s">
         <v>51</v>
@@ -11772,7 +11771,7 @@
       </c>
       <c r="C179" s="62"/>
       <c r="D179" s="62" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E179" s="62" t="s">
         <v>52</v>
@@ -11814,7 +11813,7 @@
       </c>
       <c r="C181" s="62"/>
       <c r="D181" s="62" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E181" s="62" t="s">
         <v>54</v>
@@ -11836,7 +11835,7 @@
       </c>
       <c r="C182" s="62"/>
       <c r="D182" s="62" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E182" s="62" t="s">
         <v>55</v>
@@ -11878,7 +11877,7 @@
       </c>
       <c r="C184" s="62"/>
       <c r="D184" s="62" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E184" s="62" t="s">
         <v>57</v>
@@ -11900,7 +11899,7 @@
       </c>
       <c r="C185" s="62"/>
       <c r="D185" s="62" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E185" s="62" t="s">
         <v>58</v>
@@ -11920,13 +11919,13 @@
         <v>1</v>
       </c>
       <c r="B186" s="58" t="s">
+        <v>344</v>
+      </c>
+      <c r="C186" s="58" t="s">
+        <v>423</v>
+      </c>
+      <c r="D186" s="58" t="s">
         <v>345</v>
-      </c>
-      <c r="C186" s="58" t="s">
-        <v>425</v>
-      </c>
-      <c r="D186" s="58" t="s">
-        <v>346</v>
       </c>
       <c r="E186" s="58" t="s">
         <v>46</v>
@@ -11981,10 +11980,10 @@
       </c>
       <c r="C188" s="62"/>
       <c r="D188" s="62" t="s">
+        <v>346</v>
+      </c>
+      <c r="E188" s="62" t="s">
         <v>347</v>
-      </c>
-      <c r="E188" s="62" t="s">
-        <v>348</v>
       </c>
       <c r="G188" s="62" t="s">
         <v>44</v>
@@ -12001,13 +12000,13 @@
         <v>1</v>
       </c>
       <c r="B189" s="58" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C189" s="58" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D189" s="58" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E189" s="58" t="s">
         <v>46</v>
@@ -12060,13 +12059,13 @@
         <v>1</v>
       </c>
       <c r="B191" s="58" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C191" s="58" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D191" s="58" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E191" s="58" t="s">
         <v>46</v>
@@ -12124,7 +12123,7 @@
         <v>287</v>
       </c>
       <c r="E193" s="62" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="G193" s="62" t="s">
         <v>44</v>
@@ -12141,13 +12140,13 @@
         <v>1</v>
       </c>
       <c r="B194" s="58" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C194" s="58" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D194" s="58" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E194" s="58" t="s">
         <v>48</v>
@@ -12200,13 +12199,13 @@
         <v>1</v>
       </c>
       <c r="B196" s="58" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C196" s="58" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D196" s="58" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E196" s="58" t="s">
         <v>46</v>
@@ -12261,10 +12260,10 @@
       </c>
       <c r="C198" s="62"/>
       <c r="D198" s="62" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E198" s="62" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G198" s="62" t="s">
         <v>44</v>
@@ -12281,10 +12280,10 @@
       </c>
       <c r="C199" s="62"/>
       <c r="D199" s="62" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E199" s="62" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G199" s="62" t="s">
         <v>44</v>
@@ -12303,10 +12302,10 @@
       </c>
       <c r="C200" s="62"/>
       <c r="D200" s="62" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E200" s="62" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G200" s="62" t="s">
         <v>44</v>
@@ -12323,13 +12322,13 @@
         <v>1</v>
       </c>
       <c r="B201" s="58" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C201" s="58" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D201" s="58" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E201" s="58" t="s">
         <v>46</v>
@@ -12384,7 +12383,7 @@
       </c>
       <c r="C203" s="62"/>
       <c r="D203" s="62" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E203" s="62" t="s">
         <v>41</v>
@@ -12404,13 +12403,13 @@
         <v>1</v>
       </c>
       <c r="B204" s="58" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C204" s="58" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D204" s="58" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E204" s="58" t="s">
         <v>48</v>
@@ -12463,13 +12462,13 @@
         <v>1</v>
       </c>
       <c r="B206" s="58" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C206" s="58" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D206" s="58" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E206" s="58" t="s">
         <v>46</v>
@@ -12522,13 +12521,13 @@
         <v>1</v>
       </c>
       <c r="B208" s="58" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C208" s="58" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D208" s="58" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E208" s="58" t="s">
         <v>46</v>
@@ -12581,13 +12580,13 @@
         <v>1</v>
       </c>
       <c r="B210" s="58" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C210" s="58" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D210" s="58" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E210" s="58" t="s">
         <v>46</v>
@@ -12640,13 +12639,13 @@
         <v>1</v>
       </c>
       <c r="B212" s="58" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C212" s="58" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D212" s="58" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E212" s="58" t="s">
         <v>46</v>
@@ -12699,13 +12698,13 @@
         <v>1</v>
       </c>
       <c r="B214" s="58" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C214" s="58" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D214" s="58" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E214" s="58" t="s">
         <v>46</v>
@@ -12758,13 +12757,13 @@
         <v>1</v>
       </c>
       <c r="B216" s="58" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C216" s="58" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D216" s="58" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E216" s="58" t="s">
         <v>46</v>
@@ -12819,10 +12818,10 @@
       </c>
       <c r="C218" s="62"/>
       <c r="D218" s="62" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E218" s="62" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G218" s="62" t="s">
         <v>44</v>
@@ -13491,13 +13490,13 @@
     </row>
     <row r="22" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F22" s="47" t="s">
         <v>43</v>
@@ -13514,13 +13513,13 @@
     </row>
     <row r="23" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F23" s="47" t="s">
         <v>43</v>
@@ -13537,13 +13536,13 @@
     </row>
     <row r="24" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F24" s="47" t="s">
         <v>43</v>
@@ -13560,13 +13559,13 @@
     </row>
     <row r="25" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F25" s="47" t="s">
         <v>43</v>
@@ -13583,13 +13582,13 @@
     </row>
     <row r="26" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F26" s="47" t="s">
         <v>43</v>
@@ -13606,13 +13605,13 @@
     </row>
     <row r="27" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F27" s="47" t="s">
         <v>43</v>
@@ -13629,13 +13628,13 @@
     </row>
     <row r="28" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F28" s="47" t="s">
         <v>43</v>
@@ -13652,13 +13651,13 @@
     </row>
     <row r="29" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F29" s="47" t="s">
         <v>43</v>
@@ -13675,13 +13674,13 @@
     </row>
     <row r="30" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F30" s="47" t="s">
         <v>43</v>
@@ -13698,13 +13697,13 @@
     </row>
     <row r="31" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F31" s="47" t="s">
         <v>43</v>
@@ -13721,13 +13720,13 @@
     </row>
     <row r="32" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F32" s="47" t="s">
         <v>43</v>
@@ -13744,13 +13743,13 @@
     </row>
     <row r="33" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F33" s="47" t="s">
         <v>43</v>
@@ -13767,13 +13766,13 @@
     </row>
     <row r="34" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F34" s="47" t="s">
         <v>43</v>
@@ -13790,13 +13789,13 @@
     </row>
     <row r="35" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="52" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B35" s="52" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F35" s="55" t="s">
         <v>43</v>
@@ -13813,13 +13812,13 @@
     </row>
     <row r="36" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="52" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B36" s="52" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D36" s="52" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F36" s="55" t="s">
         <v>43</v>
@@ -13836,13 +13835,13 @@
     </row>
     <row r="37" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="52" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B37" s="52" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D37" s="52" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F37" s="55" t="s">
         <v>43</v>
@@ -13859,13 +13858,13 @@
     </row>
     <row r="38" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="52" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B38" s="52" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="F38" s="55" t="s">
         <v>43</v>
@@ -13882,13 +13881,13 @@
     </row>
     <row r="39" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="52" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B39" s="52" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D39" s="52" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F39" s="55" t="s">
         <v>43</v>
@@ -13905,13 +13904,13 @@
     </row>
     <row r="40" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="52" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B40" s="52" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D40" s="52" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F40" s="55" t="s">
         <v>43</v>
@@ -13928,13 +13927,13 @@
     </row>
     <row r="41" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="52" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B41" s="52" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F41" s="55" t="s">
         <v>43</v>
@@ -13951,13 +13950,13 @@
     </row>
     <row r="42" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="52" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B42" s="52" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D42" s="52" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F42" s="55" t="s">
         <v>43</v>
@@ -13974,13 +13973,13 @@
     </row>
     <row r="43" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="52" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B43" s="52" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D43" s="52" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F43" s="55" t="s">
         <v>43</v>
@@ -13997,13 +13996,13 @@
     </row>
     <row r="44" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="52" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B44" s="52" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D44" s="52" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F44" s="55" t="s">
         <v>43</v>
@@ -14020,13 +14019,13 @@
     </row>
     <row r="45" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="52" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B45" s="52" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D45" s="52" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F45" s="55" t="s">
         <v>43</v>
@@ -14043,13 +14042,13 @@
     </row>
     <row r="46" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="50" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D46" s="50" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F46" s="54" t="s">
         <v>43</v>
@@ -14066,13 +14065,13 @@
     </row>
     <row r="47" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="50" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B47" s="50" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D47" s="50" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="F47" s="54" t="s">
         <v>43</v>
@@ -14089,13 +14088,13 @@
     </row>
     <row r="48" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="50" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D48" s="50" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F48" s="54" t="s">
         <v>43</v>
@@ -14112,13 +14111,13 @@
     </row>
     <row r="49" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="50" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B49" s="50" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D49" s="50" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F49" s="54" t="s">
         <v>43</v>
@@ -14135,13 +14134,13 @@
     </row>
     <row r="50" spans="1:9" s="50" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="50" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B50" s="50" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D50" s="50" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F50" s="54" t="s">
         <v>43</v>
@@ -14158,13 +14157,13 @@
     </row>
     <row r="51" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="50" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D51" s="50" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F51" s="54" t="s">
         <v>43</v>
@@ -14181,13 +14180,13 @@
     </row>
     <row r="52" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="50" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B52" s="50" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D52" s="50" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F52" s="54" t="s">
         <v>43</v>
@@ -14204,13 +14203,13 @@
     </row>
     <row r="53" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="50" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D53" s="50" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F53" s="54" t="s">
         <v>43</v>
@@ -14227,13 +14226,13 @@
     </row>
     <row r="54" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="50" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D54" s="50" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F54" s="54" t="s">
         <v>43</v>
@@ -14250,13 +14249,13 @@
     </row>
     <row r="55" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="50" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B55" s="50" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D55" s="50" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="F55" s="54" t="s">
         <v>43</v>
@@ -14273,13 +14272,13 @@
     </row>
     <row r="56" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="50" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B56" s="50" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D56" s="50" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F56" s="54" t="s">
         <v>43</v>
@@ -14296,13 +14295,13 @@
     </row>
     <row r="57" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="50" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B57" s="50" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D57" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F57" s="54" t="s">
         <v>43</v>
@@ -14319,13 +14318,13 @@
     </row>
     <row r="58" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="50" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B58" s="50" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D58" s="50" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F58" s="54" t="s">
         <v>43</v>
@@ -14342,13 +14341,13 @@
     </row>
     <row r="59" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="50" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B59" s="50" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D59" s="50" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F59" s="54" t="s">
         <v>43</v>
@@ -14365,13 +14364,13 @@
     </row>
     <row r="60" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="50" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B60" s="50" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D60" s="50" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F60" s="54" t="s">
         <v>43</v>
@@ -14388,13 +14387,13 @@
     </row>
     <row r="61" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="50" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D61" s="50" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F61" s="54" t="s">
         <v>43</v>
@@ -14411,13 +14410,13 @@
     </row>
     <row r="62" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="58" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B62" s="58" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D62" s="58" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="F62" s="60" t="s">
         <v>43</v>
@@ -14434,13 +14433,13 @@
     </row>
     <row r="63" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="58" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B63" s="58" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D63" s="58" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F63" s="60" t="s">
         <v>43</v>
@@ -14457,13 +14456,13 @@
     </row>
     <row r="64" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="58" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B64" s="58" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D64" s="58" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F64" s="60" t="s">
         <v>43</v>
@@ -14480,13 +14479,13 @@
     </row>
     <row r="65" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="58" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B65" s="58" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D65" s="58" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="F65" s="60" t="s">
         <v>43</v>
@@ -14503,13 +14502,13 @@
     </row>
     <row r="66" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="58" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B66" s="58" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D66" s="58" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F66" s="60" t="s">
         <v>43</v>
@@ -14526,13 +14525,13 @@
     </row>
     <row r="67" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="58" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B67" s="58" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D67" s="58" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F67" s="60" t="s">
         <v>43</v>
@@ -14549,13 +14548,13 @@
     </row>
     <row r="68" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="58" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B68" s="58" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D68" s="58" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F68" s="60" t="s">
         <v>43</v>
@@ -14572,13 +14571,13 @@
     </row>
     <row r="69" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="58" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B69" s="58" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D69" s="58" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F69" s="60" t="s">
         <v>43</v>
@@ -14595,13 +14594,13 @@
     </row>
     <row r="70" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="58" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B70" s="58" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D70" s="58" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F70" s="60" t="s">
         <v>43</v>
@@ -14618,13 +14617,13 @@
     </row>
     <row r="71" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="58" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B71" s="58" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D71" s="58" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F71" s="60" t="s">
         <v>43</v>
@@ -14641,13 +14640,13 @@
     </row>
     <row r="72" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="58" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B72" s="58" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D72" s="58" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="F72" s="60" t="s">
         <v>43</v>
@@ -14664,13 +14663,13 @@
     </row>
     <row r="73" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="58" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B73" s="58" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D73" s="58" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="F73" s="60" t="s">
         <v>43</v>
@@ -14687,13 +14686,13 @@
     </row>
     <row r="74" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="58" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B74" s="58" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D74" s="58" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F74" s="60" t="s">
         <v>43</v>
@@ -14710,13 +14709,13 @@
     </row>
     <row r="75" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="58" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B75" s="58" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D75" s="58" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F75" s="60" t="s">
         <v>43</v>
@@ -14733,13 +14732,13 @@
     </row>
     <row r="76" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="58" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B76" s="58" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D76" s="58" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="F76" s="60" t="s">
         <v>43</v>
@@ -14756,13 +14755,13 @@
     </row>
     <row r="77" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="58" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B77" s="58" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D77" s="58" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F77" s="60" t="s">
         <v>43</v>
@@ -14779,13 +14778,13 @@
     </row>
     <row r="78" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="58" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B78" s="58" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D78" s="58" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F78" s="60" t="s">
         <v>43</v>
@@ -14802,13 +14801,13 @@
     </row>
     <row r="79" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="58" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B79" s="58" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D79" s="58" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F79" s="60" t="s">
         <v>43</v>
@@ -14825,13 +14824,13 @@
     </row>
     <row r="80" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="58" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B80" s="58" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D80" s="58" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F80" s="60" t="s">
         <v>43</v>
@@ -14848,13 +14847,13 @@
     </row>
     <row r="81" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="58" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B81" s="58" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D81" s="58" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F81" s="60" t="s">
         <v>43</v>
@@ -14871,13 +14870,13 @@
     </row>
     <row r="82" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="58" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B82" s="58" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D82" s="58" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F82" s="60" t="s">
         <v>43</v>
@@ -15399,966 +15398,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A213"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A213"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30"/>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="56" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="56" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="56" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="56" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="56" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="56" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="56" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="56" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="56" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="56" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="56" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="56" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="56" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="56" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="56" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="56" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="56" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="56" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="56" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="56" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="56" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="56" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="56" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="56" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="52"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="59" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="59" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="59" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="59" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="52"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="59" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="52"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="59" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="52"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="59" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="52"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="59" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="52"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="59" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="52"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="59" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="52"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="59" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="52"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="59" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="59" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="59" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="59" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="59" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="59" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="59" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="59" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="59" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="59" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="59" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="52"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="59" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="59" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="59" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="59" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="59" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="59" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="59" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="59" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="59" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="59" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="59" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="50"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="50"/>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="61" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="50"/>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="50"/>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="50"/>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" s="61" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="61" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" s="61" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="61" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="61" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" s="61" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" s="61" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="61" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" s="61" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" s="50"/>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="50"/>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" s="50"/>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" s="50"/>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" s="50"/>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" s="50"/>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" s="61" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" s="50"/>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" s="61" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" s="50"/>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134" s="50"/>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135" s="61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136" s="58"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138" s="58"/>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" s="58"/>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142" s="62" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143" s="62" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144" s="62" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145" s="62" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146" s="62" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147" s="62" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" s="62" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149" s="62" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150" s="62" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151" s="62" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152" s="58"/>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A154" s="58"/>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156" s="62" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157" s="62" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A158" s="62" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A159" s="62" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A160" s="62" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A161" s="62" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A162" s="62" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A163" s="62" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A164" s="62" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A165" s="62" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A166" s="58"/>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A167" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A168" s="58"/>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A169" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A170" s="62" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A171" s="62" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A172" s="62" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A173" s="62" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A174" s="62" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A175" s="62" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A176" s="62" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A177" s="62" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A178" s="62" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A179" s="62" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A180" s="62" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A181" s="58"/>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A182" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A183" s="62" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A184" s="58"/>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A185" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A186" s="58"/>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A187" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A188" s="62" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A189" s="58"/>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A190" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A191" s="58"/>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A192" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A193" s="62" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A194" s="62" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A195" s="62" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A196" s="58"/>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A197" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A198" s="62" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A199" s="58"/>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A200" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A201" s="58"/>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A202" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A203" s="58"/>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A204" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A205" s="58"/>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A206" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A207" s="58"/>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A208" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A209" s="58"/>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A210" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A211" s="58"/>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A212" s="62" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A213" s="62" t="s">
-        <v>369</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Removes the measure_name.applicable outputs from the objective function
</commit_message>
<xml_diff>
--- a/projects/PTool_Full_Analysis.xlsx
+++ b/projects/PTool_Full_Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="5244" windowWidth="22368" windowHeight="5268" tabRatio="469" activeTab="2"/>
+    <workbookView xWindow="-12" yWindow="5244" windowWidth="22368" windowHeight="5268" tabRatio="469" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -826,9 +826,6 @@
     <t>../../OpenStudio-PTool/weather/*</t>
   </si>
   <si>
-    <t>|LargeOffice,SmallOffice,MediumOffice,RetailStandalone,SecondarySchool,LargeHotel,SmallHotel|</t>
-  </si>
-  <si>
     <t>../../openstudio-standards/measures</t>
   </si>
   <si>
@@ -1372,9 +1369,6 @@
     <t>Ptool_Full_Analysis</t>
   </si>
   <si>
-    <t>cluster6</t>
-  </si>
-  <si>
     <t>AdvancedHybridRTUs</t>
   </si>
   <si>
@@ -1957,9 +1951,6 @@
     <t>delta_x</t>
   </si>
   <si>
-    <t>["LargeOffice","SmallOffice","MediumOffice","RetailStandalone","SecondarySchool","LargeHotel","SmallHotel"]</t>
-  </si>
-  <si>
     <t>["DOE Ref Pre-1980","DOE Ref 1980-2004","90.1-2010"]</t>
   </si>
   <si>
@@ -1970,6 +1961,15 @@
   </si>
   <si>
     <t>Hot Water Pump Differential Pressure Reset</t>
+  </si>
+  <si>
+    <t>["SecondarySchool","PrimarySchool","SmallOffice","MediumOffice","SmallHotel","LargeHotel","RetailStandalone","RetailStripmall","QuickServiceRestaurant","FullServiceRestaurant"]</t>
+  </si>
+  <si>
+    <t>|SecondarySchool,PrimarySchool,SmallOffice,MediumOffice,SmallHotel,LargeHotel,RetailStandalone,RetailStripmall,QuickServiceRestaurant,FullServiceRestaurant|</t>
+  </si>
+  <si>
+    <t>PToolFullCluster</t>
   </si>
 </sst>
 </file>
@@ -6754,7 +6754,7 @@
         <v>81</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>82</v>
@@ -6765,7 +6765,7 @@
         <v>94</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>178</v>
@@ -6776,7 +6776,7 @@
         <v>95</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>445</v>
+        <v>644</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>97</v>
@@ -6787,15 +6787,15 @@
         <v>67</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C7" s="31" t="str">
         <f>VLOOKUP($B7,instance_defs,2,FALSE)&amp;VLOOKUP($B7,instance_defs,4,FALSE)</f>
-        <v>16 Cores - Worker Only - Recommended for Worker</v>
+        <v>8 Cores - Recommended for Server</v>
       </c>
       <c r="D7" s="31" t="str">
         <f>VLOOKUP($B7,instance_defs,3,FALSE)</f>
-        <v>$1.68/hour</v>
+        <v>$0.56/hour</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>171</v>
@@ -6825,7 +6825,7 @@
         <v>83</v>
       </c>
       <c r="B9" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="31"/>
@@ -6847,7 +6847,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>96</v>
@@ -6858,7 +6858,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="30" t="s">
@@ -7087,7 +7087,7 @@
         <v>198</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>232</v>
@@ -7142,7 +7142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z218"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
@@ -7269,7 +7269,7 @@
         <v>8</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="P3" s="16" t="s">
         <v>100</v>
@@ -7338,10 +7338,10 @@
         <v>255</v>
       </c>
       <c r="J5" s="30" t="s">
-        <v>263</v>
+        <v>643</v>
       </c>
       <c r="P5" s="30" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="R5" s="30" t="s">
         <v>254</v>
@@ -7355,7 +7355,7 @@
         <v>246</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G6" s="30" t="s">
         <v>243</v>
@@ -7379,7 +7379,7 @@
         <v>245</v>
       </c>
       <c r="P6" s="30" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="R6" s="30" t="s">
         <v>254</v>
@@ -7417,7 +7417,7 @@
         <v>250</v>
       </c>
       <c r="P7" s="44" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="R7" s="30" t="s">
         <v>254</v>
@@ -7428,13 +7428,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>46</v>
@@ -7487,13 +7487,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>305</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>46</v>
@@ -7568,7 +7568,7 @@
       </c>
       <c r="C13" s="56"/>
       <c r="D13" s="56" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E13" s="56" t="s">
         <v>50</v>
@@ -7588,7 +7588,7 @@
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="56" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E14" s="56" t="s">
         <v>51</v>
@@ -7597,7 +7597,7 @@
         <v>44</v>
       </c>
       <c r="H14" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I14" s="56">
         <v>18</v>
@@ -7610,7 +7610,7 @@
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="56" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E15" s="56" t="s">
         <v>52</v>
@@ -7619,7 +7619,7 @@
         <v>44</v>
       </c>
       <c r="H15" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I15" s="56">
         <v>9</v>
@@ -7632,7 +7632,7 @@
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="56" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E16" s="56" t="s">
         <v>53</v>
@@ -7652,7 +7652,7 @@
       </c>
       <c r="C17" s="56"/>
       <c r="D17" s="56" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E17" s="56" t="s">
         <v>54</v>
@@ -7661,7 +7661,7 @@
         <v>44</v>
       </c>
       <c r="H17" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I17" s="56">
         <v>18</v>
@@ -7674,7 +7674,7 @@
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="56" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E18" s="56" t="s">
         <v>55</v>
@@ -7683,7 +7683,7 @@
         <v>44</v>
       </c>
       <c r="H18" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I18" s="56">
         <v>9</v>
@@ -7696,7 +7696,7 @@
       </c>
       <c r="C19" s="56"/>
       <c r="D19" s="56" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E19" s="56" t="s">
         <v>56</v>
@@ -7716,7 +7716,7 @@
       </c>
       <c r="C20" s="56"/>
       <c r="D20" s="56" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E20" s="56" t="s">
         <v>57</v>
@@ -7725,7 +7725,7 @@
         <v>44</v>
       </c>
       <c r="H20" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I20" s="56">
         <v>18</v>
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C21" s="56"/>
       <c r="D21" s="56" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E21" s="56" t="s">
         <v>58</v>
@@ -7747,7 +7747,7 @@
         <v>44</v>
       </c>
       <c r="H21" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I21" s="56">
         <v>9</v>
@@ -7758,13 +7758,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>48</v>
@@ -7817,13 +7817,13 @@
         <v>1</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>46</v>
@@ -7878,16 +7878,16 @@
       </c>
       <c r="C26" s="56"/>
       <c r="D26" s="56" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E26" s="56" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G26" s="56" t="s">
         <v>44</v>
       </c>
       <c r="H26" s="56" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I26" s="56">
         <v>10</v>
@@ -7900,10 +7900,10 @@
       </c>
       <c r="C27" s="56"/>
       <c r="D27" s="56" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E27" s="56" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="G27" s="56" t="s">
         <v>44</v>
@@ -7920,10 +7920,10 @@
       </c>
       <c r="C28" s="56"/>
       <c r="D28" s="56" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E28" s="56" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="G28" s="56" t="s">
         <v>44</v>
@@ -7938,13 +7938,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>46</v>
@@ -7999,16 +7999,16 @@
       </c>
       <c r="C31" s="56"/>
       <c r="D31" s="56" t="s">
+        <v>306</v>
+      </c>
+      <c r="E31" s="56" t="s">
         <v>307</v>
-      </c>
-      <c r="E31" s="56" t="s">
-        <v>308</v>
       </c>
       <c r="G31" s="56" t="s">
         <v>44</v>
       </c>
       <c r="H31" s="56" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I31" s="56">
         <v>2</v>
@@ -8019,13 +8019,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>46</v>
@@ -8078,13 +8078,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>310</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>46</v>
@@ -8137,13 +8137,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>311</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>312</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>46</v>
@@ -8196,13 +8196,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>313</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>314</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>46</v>
@@ -8255,13 +8255,13 @@
         <v>1</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>46</v>
@@ -8314,13 +8314,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>46</v>
@@ -8373,13 +8373,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>48</v>
@@ -8432,13 +8432,13 @@
         <v>1</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>315</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>316</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>46</v>
@@ -8513,7 +8513,7 @@
       </c>
       <c r="C49" s="56"/>
       <c r="D49" s="56" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E49" s="56" t="s">
         <v>50</v>
@@ -8533,7 +8533,7 @@
       </c>
       <c r="C50" s="56"/>
       <c r="D50" s="56" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E50" s="56" t="s">
         <v>51</v>
@@ -8542,7 +8542,7 @@
         <v>44</v>
       </c>
       <c r="H50" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I50" s="56">
         <v>18</v>
@@ -8555,7 +8555,7 @@
       </c>
       <c r="C51" s="56"/>
       <c r="D51" s="56" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E51" s="56" t="s">
         <v>52</v>
@@ -8564,7 +8564,7 @@
         <v>44</v>
       </c>
       <c r="H51" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I51" s="56">
         <v>9</v>
@@ -8577,7 +8577,7 @@
       </c>
       <c r="C52" s="56"/>
       <c r="D52" s="56" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E52" s="56" t="s">
         <v>53</v>
@@ -8597,7 +8597,7 @@
       </c>
       <c r="C53" s="56"/>
       <c r="D53" s="56" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E53" s="56" t="s">
         <v>54</v>
@@ -8606,7 +8606,7 @@
         <v>44</v>
       </c>
       <c r="H53" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I53" s="56">
         <v>18</v>
@@ -8619,7 +8619,7 @@
       </c>
       <c r="C54" s="56"/>
       <c r="D54" s="56" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E54" s="56" t="s">
         <v>55</v>
@@ -8628,7 +8628,7 @@
         <v>44</v>
       </c>
       <c r="H54" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I54" s="56">
         <v>9</v>
@@ -8641,7 +8641,7 @@
       </c>
       <c r="C55" s="56"/>
       <c r="D55" s="56" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E55" s="56" t="s">
         <v>56</v>
@@ -8661,7 +8661,7 @@
       </c>
       <c r="C56" s="56"/>
       <c r="D56" s="56" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E56" s="56" t="s">
         <v>57</v>
@@ -8670,7 +8670,7 @@
         <v>44</v>
       </c>
       <c r="H56" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I56" s="56">
         <v>18</v>
@@ -8683,7 +8683,7 @@
       </c>
       <c r="C57" s="56"/>
       <c r="D57" s="56" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E57" s="56" t="s">
         <v>58</v>
@@ -8692,7 +8692,7 @@
         <v>44</v>
       </c>
       <c r="H57" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I57" s="56">
         <v>9</v>
@@ -8703,13 +8703,13 @@
         <v>1</v>
       </c>
       <c r="B58" s="52" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D58" s="52" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E58" s="52" t="s">
         <v>46</v>
@@ -8764,10 +8764,10 @@
       </c>
       <c r="C60" s="59"/>
       <c r="D60" s="59" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E60" s="59" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="G60" s="59" t="s">
         <v>44</v>
@@ -8784,10 +8784,10 @@
       </c>
       <c r="C61" s="59"/>
       <c r="D61" s="59" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E61" s="59" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G61" s="59" t="s">
         <v>44</v>
@@ -8804,10 +8804,10 @@
       </c>
       <c r="C62" s="59"/>
       <c r="D62" s="59" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E62" s="59" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G62" s="59" t="s">
         <v>44</v>
@@ -8822,13 +8822,13 @@
         <v>1</v>
       </c>
       <c r="B63" s="52" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C63" s="52" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D63" s="52" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E63" s="52" t="s">
         <v>46</v>
@@ -8881,13 +8881,13 @@
         <v>1</v>
       </c>
       <c r="B65" s="52" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C65" s="52" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D65" s="52" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E65" s="52" t="s">
         <v>46</v>
@@ -8940,13 +8940,13 @@
         <v>1</v>
       </c>
       <c r="B67" s="52" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C67" s="52" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D67" s="52" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E67" s="52" t="s">
         <v>46</v>
@@ -8999,13 +8999,13 @@
         <v>1</v>
       </c>
       <c r="B69" s="52" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C69" s="52" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D69" s="52" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E69" s="52" t="s">
         <v>46</v>
@@ -9058,13 +9058,13 @@
         <v>1</v>
       </c>
       <c r="B71" s="52" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C71" s="52" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D71" s="52" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E71" s="52" t="s">
         <v>46</v>
@@ -9117,13 +9117,13 @@
         <v>1</v>
       </c>
       <c r="B73" s="52" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C73" s="52" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D73" s="52" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E73" s="52" t="s">
         <v>46</v>
@@ -9176,13 +9176,13 @@
         <v>1</v>
       </c>
       <c r="B75" s="52" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C75" s="52" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D75" s="52" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E75" s="52" t="s">
         <v>46</v>
@@ -9235,13 +9235,13 @@
         <v>1</v>
       </c>
       <c r="B77" s="52" t="s">
+        <v>317</v>
+      </c>
+      <c r="C77" s="52" t="s">
+        <v>381</v>
+      </c>
+      <c r="D77" s="52" t="s">
         <v>318</v>
-      </c>
-      <c r="C77" s="52" t="s">
-        <v>382</v>
-      </c>
-      <c r="D77" s="52" t="s">
-        <v>319</v>
       </c>
       <c r="E77" s="52" t="s">
         <v>46</v>
@@ -9316,7 +9316,7 @@
       </c>
       <c r="C80" s="59"/>
       <c r="D80" s="59" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E80" s="59" t="s">
         <v>50</v>
@@ -9336,7 +9336,7 @@
       </c>
       <c r="C81" s="59"/>
       <c r="D81" s="59" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E81" s="59" t="s">
         <v>51</v>
@@ -9345,7 +9345,7 @@
         <v>44</v>
       </c>
       <c r="H81" s="59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I81" s="59">
         <v>18</v>
@@ -9358,7 +9358,7 @@
       </c>
       <c r="C82" s="59"/>
       <c r="D82" s="59" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E82" s="59" t="s">
         <v>52</v>
@@ -9367,7 +9367,7 @@
         <v>44</v>
       </c>
       <c r="H82" s="59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I82" s="59">
         <v>9</v>
@@ -9380,7 +9380,7 @@
       </c>
       <c r="C83" s="59"/>
       <c r="D83" s="59" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E83" s="59" t="s">
         <v>53</v>
@@ -9400,7 +9400,7 @@
       </c>
       <c r="C84" s="59"/>
       <c r="D84" s="59" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E84" s="59" t="s">
         <v>54</v>
@@ -9409,7 +9409,7 @@
         <v>44</v>
       </c>
       <c r="H84" s="59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I84" s="59">
         <v>18</v>
@@ -9422,7 +9422,7 @@
       </c>
       <c r="C85" s="59"/>
       <c r="D85" s="59" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E85" s="59" t="s">
         <v>55</v>
@@ -9431,7 +9431,7 @@
         <v>44</v>
       </c>
       <c r="H85" s="59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I85" s="59">
         <v>9</v>
@@ -9444,7 +9444,7 @@
       </c>
       <c r="C86" s="59"/>
       <c r="D86" s="59" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E86" s="59" t="s">
         <v>56</v>
@@ -9464,7 +9464,7 @@
       </c>
       <c r="C87" s="59"/>
       <c r="D87" s="59" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E87" s="59" t="s">
         <v>57</v>
@@ -9473,7 +9473,7 @@
         <v>44</v>
       </c>
       <c r="H87" s="59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I87" s="59">
         <v>18</v>
@@ -9486,7 +9486,7 @@
       </c>
       <c r="C88" s="59"/>
       <c r="D88" s="59" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E88" s="59" t="s">
         <v>58</v>
@@ -9495,7 +9495,7 @@
         <v>44</v>
       </c>
       <c r="H88" s="59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I88" s="59">
         <v>9</v>
@@ -9506,13 +9506,13 @@
         <v>1</v>
       </c>
       <c r="B89" s="52" t="s">
+        <v>319</v>
+      </c>
+      <c r="C89" s="52" t="s">
+        <v>382</v>
+      </c>
+      <c r="D89" s="52" t="s">
         <v>320</v>
-      </c>
-      <c r="C89" s="52" t="s">
-        <v>383</v>
-      </c>
-      <c r="D89" s="52" t="s">
-        <v>321</v>
       </c>
       <c r="E89" s="52" t="s">
         <v>46</v>
@@ -9587,7 +9587,7 @@
       </c>
       <c r="C92" s="59"/>
       <c r="D92" s="59" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E92" s="59" t="s">
         <v>50</v>
@@ -9607,7 +9607,7 @@
       </c>
       <c r="C93" s="59"/>
       <c r="D93" s="59" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E93" s="59" t="s">
         <v>51</v>
@@ -9616,7 +9616,7 @@
         <v>44</v>
       </c>
       <c r="H93" s="59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I93" s="59">
         <v>18</v>
@@ -9629,7 +9629,7 @@
       </c>
       <c r="C94" s="59"/>
       <c r="D94" s="59" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E94" s="59" t="s">
         <v>52</v>
@@ -9638,7 +9638,7 @@
         <v>44</v>
       </c>
       <c r="H94" s="59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I94" s="59">
         <v>9</v>
@@ -9651,7 +9651,7 @@
       </c>
       <c r="C95" s="59"/>
       <c r="D95" s="59" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E95" s="59" t="s">
         <v>53</v>
@@ -9671,7 +9671,7 @@
       </c>
       <c r="C96" s="59"/>
       <c r="D96" s="59" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E96" s="59" t="s">
         <v>54</v>
@@ -9680,7 +9680,7 @@
         <v>44</v>
       </c>
       <c r="H96" s="59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I96" s="59">
         <v>18</v>
@@ -9693,7 +9693,7 @@
       </c>
       <c r="C97" s="59"/>
       <c r="D97" s="59" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E97" s="59" t="s">
         <v>55</v>
@@ -9702,7 +9702,7 @@
         <v>44</v>
       </c>
       <c r="H97" s="59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I97" s="59">
         <v>9</v>
@@ -9715,7 +9715,7 @@
       </c>
       <c r="C98" s="59"/>
       <c r="D98" s="59" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E98" s="59" t="s">
         <v>56</v>
@@ -9735,7 +9735,7 @@
       </c>
       <c r="C99" s="59"/>
       <c r="D99" s="59" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E99" s="59" t="s">
         <v>57</v>
@@ -9744,7 +9744,7 @@
         <v>44</v>
       </c>
       <c r="H99" s="59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I99" s="59">
         <v>18</v>
@@ -9757,7 +9757,7 @@
       </c>
       <c r="C100" s="59"/>
       <c r="D100" s="59" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E100" s="59" t="s">
         <v>58</v>
@@ -9766,7 +9766,7 @@
         <v>44</v>
       </c>
       <c r="H100" s="59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I100" s="59">
         <v>9</v>
@@ -9777,13 +9777,13 @@
         <v>1</v>
       </c>
       <c r="B101" s="50" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C101" s="50" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D101" s="50" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E101" s="50" t="s">
         <v>46</v>
@@ -9836,13 +9836,13 @@
         <v>1</v>
       </c>
       <c r="B103" s="50" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C103" s="50" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D103" s="50" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E103" s="50" t="s">
         <v>46</v>
@@ -9897,16 +9897,16 @@
       </c>
       <c r="C105" s="61"/>
       <c r="D105" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E105" s="61" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G105" s="61" t="s">
         <v>44</v>
       </c>
       <c r="H105" s="61" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I105" s="61">
         <v>30</v>
@@ -9917,13 +9917,13 @@
         <v>1</v>
       </c>
       <c r="B106" s="50" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C106" s="50" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D106" s="50" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E106" s="50" t="s">
         <v>48</v>
@@ -9976,13 +9976,13 @@
         <v>1</v>
       </c>
       <c r="B108" s="50" t="s">
+        <v>321</v>
+      </c>
+      <c r="C108" s="50" t="s">
+        <v>383</v>
+      </c>
+      <c r="D108" s="50" t="s">
         <v>322</v>
-      </c>
-      <c r="C108" s="50" t="s">
-        <v>384</v>
-      </c>
-      <c r="D108" s="50" t="s">
-        <v>323</v>
       </c>
       <c r="E108" s="50" t="s">
         <v>46</v>
@@ -10035,13 +10035,13 @@
         <v>1</v>
       </c>
       <c r="B110" s="50" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C110" s="50" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D110" s="50" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E110" s="50" t="s">
         <v>46</v>
@@ -10096,16 +10096,16 @@
       </c>
       <c r="C112" s="61"/>
       <c r="D112" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="E112" s="61" t="s">
         <v>301</v>
-      </c>
-      <c r="E112" s="61" t="s">
-        <v>302</v>
       </c>
       <c r="G112" s="61" t="s">
         <v>44</v>
       </c>
       <c r="H112" s="61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I112" s="61">
         <v>1</v>
@@ -10118,10 +10118,10 @@
       </c>
       <c r="C113" s="61"/>
       <c r="D113" s="61" t="s">
+        <v>270</v>
+      </c>
+      <c r="E113" s="61" t="s">
         <v>271</v>
-      </c>
-      <c r="E113" s="61" t="s">
-        <v>272</v>
       </c>
       <c r="G113" s="61" t="s">
         <v>44</v>
@@ -10138,10 +10138,10 @@
       </c>
       <c r="C114" s="61"/>
       <c r="D114" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="E114" s="61" t="s">
         <v>273</v>
-      </c>
-      <c r="E114" s="61" t="s">
-        <v>274</v>
       </c>
       <c r="G114" s="61" t="s">
         <v>44</v>
@@ -10158,10 +10158,10 @@
       </c>
       <c r="C115" s="61"/>
       <c r="D115" s="61" t="s">
+        <v>274</v>
+      </c>
+      <c r="E115" s="61" t="s">
         <v>275</v>
-      </c>
-      <c r="E115" s="61" t="s">
-        <v>276</v>
       </c>
       <c r="G115" s="61" t="s">
         <v>44</v>
@@ -10178,10 +10178,10 @@
       </c>
       <c r="C116" s="61"/>
       <c r="D116" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="E116" s="61" t="s">
         <v>277</v>
-      </c>
-      <c r="E116" s="61" t="s">
-        <v>278</v>
       </c>
       <c r="G116" s="61" t="s">
         <v>44</v>
@@ -10198,10 +10198,10 @@
       </c>
       <c r="C117" s="61"/>
       <c r="D117" s="61" t="s">
+        <v>278</v>
+      </c>
+      <c r="E117" s="61" t="s">
         <v>279</v>
-      </c>
-      <c r="E117" s="61" t="s">
-        <v>280</v>
       </c>
       <c r="G117" s="61" t="s">
         <v>44</v>
@@ -10218,10 +10218,10 @@
       </c>
       <c r="C118" s="61"/>
       <c r="D118" s="61" t="s">
+        <v>280</v>
+      </c>
+      <c r="E118" s="61" t="s">
         <v>281</v>
-      </c>
-      <c r="E118" s="61" t="s">
-        <v>282</v>
       </c>
       <c r="G118" s="61" t="s">
         <v>44</v>
@@ -10238,10 +10238,10 @@
       </c>
       <c r="C119" s="61"/>
       <c r="D119" s="61" t="s">
+        <v>282</v>
+      </c>
+      <c r="E119" s="61" t="s">
         <v>283</v>
-      </c>
-      <c r="E119" s="61" t="s">
-        <v>284</v>
       </c>
       <c r="G119" s="61" t="s">
         <v>44</v>
@@ -10258,10 +10258,10 @@
       </c>
       <c r="C120" s="61"/>
       <c r="D120" s="61" t="s">
+        <v>284</v>
+      </c>
+      <c r="E120" s="61" t="s">
         <v>285</v>
-      </c>
-      <c r="E120" s="61" t="s">
-        <v>286</v>
       </c>
       <c r="G120" s="61" t="s">
         <v>44</v>
@@ -10276,13 +10276,13 @@
         <v>1</v>
       </c>
       <c r="B121" s="50" t="s">
+        <v>323</v>
+      </c>
+      <c r="C121" s="50" t="s">
+        <v>384</v>
+      </c>
+      <c r="D121" s="50" t="s">
         <v>324</v>
-      </c>
-      <c r="C121" s="50" t="s">
-        <v>385</v>
-      </c>
-      <c r="D121" s="50" t="s">
-        <v>325</v>
       </c>
       <c r="E121" s="50" t="s">
         <v>46</v>
@@ -10335,13 +10335,13 @@
         <v>1</v>
       </c>
       <c r="B123" s="50" t="s">
+        <v>325</v>
+      </c>
+      <c r="C123" s="50" t="s">
+        <v>385</v>
+      </c>
+      <c r="D123" s="50" t="s">
         <v>326</v>
-      </c>
-      <c r="C123" s="50" t="s">
-        <v>386</v>
-      </c>
-      <c r="D123" s="50" t="s">
-        <v>327</v>
       </c>
       <c r="E123" s="50" t="s">
         <v>46</v>
@@ -10394,13 +10394,13 @@
         <v>1</v>
       </c>
       <c r="B125" s="50" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C125" s="50" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D125" s="50" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E125" s="50" t="s">
         <v>48</v>
@@ -10453,13 +10453,13 @@
         <v>1</v>
       </c>
       <c r="B127" s="50" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C127" s="50" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D127" s="50" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E127" s="50" t="s">
         <v>46</v>
@@ -10512,13 +10512,13 @@
         <v>1</v>
       </c>
       <c r="B129" s="50" t="s">
+        <v>327</v>
+      </c>
+      <c r="C129" s="50" t="s">
+        <v>405</v>
+      </c>
+      <c r="D129" s="50" t="s">
         <v>328</v>
-      </c>
-      <c r="C129" s="50" t="s">
-        <v>406</v>
-      </c>
-      <c r="D129" s="50" t="s">
-        <v>329</v>
       </c>
       <c r="E129" s="50" t="s">
         <v>46</v>
@@ -10571,13 +10571,13 @@
         <v>1</v>
       </c>
       <c r="B131" s="50" t="s">
+        <v>329</v>
+      </c>
+      <c r="C131" s="50" t="s">
+        <v>406</v>
+      </c>
+      <c r="D131" s="50" t="s">
         <v>330</v>
-      </c>
-      <c r="C131" s="50" t="s">
-        <v>407</v>
-      </c>
-      <c r="D131" s="50" t="s">
-        <v>331</v>
       </c>
       <c r="E131" s="50" t="s">
         <v>46</v>
@@ -10632,16 +10632,16 @@
       </c>
       <c r="C133" s="61"/>
       <c r="D133" s="61" t="s">
+        <v>331</v>
+      </c>
+      <c r="E133" s="61" t="s">
         <v>332</v>
-      </c>
-      <c r="E133" s="61" t="s">
-        <v>333</v>
       </c>
       <c r="G133" s="61" t="s">
         <v>44</v>
       </c>
       <c r="H133" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I133" s="61">
         <v>10</v>
@@ -10652,13 +10652,13 @@
         <v>1</v>
       </c>
       <c r="B134" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="C134" s="50" t="s">
+        <v>407</v>
+      </c>
+      <c r="D134" s="50" t="s">
         <v>334</v>
-      </c>
-      <c r="C134" s="50" t="s">
-        <v>408</v>
-      </c>
-      <c r="D134" s="50" t="s">
-        <v>335</v>
       </c>
       <c r="E134" s="50" t="s">
         <v>46</v>
@@ -10713,16 +10713,16 @@
       </c>
       <c r="C136" s="61"/>
       <c r="D136" s="61" t="s">
+        <v>335</v>
+      </c>
+      <c r="E136" s="61" t="s">
         <v>336</v>
-      </c>
-      <c r="E136" s="61" t="s">
-        <v>337</v>
       </c>
       <c r="G136" s="61" t="s">
         <v>44</v>
       </c>
       <c r="H136" s="61" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I136" s="61">
         <v>0.5</v>
@@ -10733,13 +10733,13 @@
         <v>1</v>
       </c>
       <c r="B137" s="50" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C137" s="50" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D137" s="50" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E137" s="50" t="s">
         <v>48</v>
@@ -10792,13 +10792,13 @@
         <v>1</v>
       </c>
       <c r="B139" s="50" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C139" s="50" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D139" s="50" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E139" s="50" t="s">
         <v>48</v>
@@ -10851,13 +10851,13 @@
         <v>1</v>
       </c>
       <c r="B141" s="58" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C141" s="58" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D141" s="58" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E141" s="58" t="s">
         <v>46</v>
@@ -10910,13 +10910,13 @@
         <v>1</v>
       </c>
       <c r="B143" s="58" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C143" s="58" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D143" s="58" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E143" s="58" t="s">
         <v>48</v>
@@ -10969,13 +10969,13 @@
         <v>1</v>
       </c>
       <c r="B145" s="58" t="s">
+        <v>338</v>
+      </c>
+      <c r="C145" s="58" t="s">
+        <v>408</v>
+      </c>
+      <c r="D145" s="58" t="s">
         <v>339</v>
-      </c>
-      <c r="C145" s="58" t="s">
-        <v>409</v>
-      </c>
-      <c r="D145" s="58" t="s">
-        <v>340</v>
       </c>
       <c r="E145" s="58" t="s">
         <v>46</v>
@@ -11050,7 +11050,7 @@
       </c>
       <c r="C148" s="62"/>
       <c r="D148" s="62" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E148" s="62" t="s">
         <v>50</v>
@@ -11070,7 +11070,7 @@
       </c>
       <c r="C149" s="62"/>
       <c r="D149" s="62" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E149" s="62" t="s">
         <v>51</v>
@@ -11079,7 +11079,7 @@
         <v>44</v>
       </c>
       <c r="H149" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I149" s="62">
         <v>18</v>
@@ -11092,7 +11092,7 @@
       </c>
       <c r="C150" s="62"/>
       <c r="D150" s="62" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E150" s="62" t="s">
         <v>52</v>
@@ -11101,7 +11101,7 @@
         <v>44</v>
       </c>
       <c r="H150" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I150" s="62">
         <v>9</v>
@@ -11114,7 +11114,7 @@
       </c>
       <c r="C151" s="62"/>
       <c r="D151" s="62" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E151" s="62" t="s">
         <v>53</v>
@@ -11134,7 +11134,7 @@
       </c>
       <c r="C152" s="62"/>
       <c r="D152" s="62" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E152" s="62" t="s">
         <v>54</v>
@@ -11143,7 +11143,7 @@
         <v>44</v>
       </c>
       <c r="H152" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I152" s="62">
         <v>18</v>
@@ -11156,7 +11156,7 @@
       </c>
       <c r="C153" s="62"/>
       <c r="D153" s="62" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E153" s="62" t="s">
         <v>55</v>
@@ -11165,7 +11165,7 @@
         <v>44</v>
       </c>
       <c r="H153" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I153" s="62">
         <v>9</v>
@@ -11178,7 +11178,7 @@
       </c>
       <c r="C154" s="62"/>
       <c r="D154" s="62" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E154" s="62" t="s">
         <v>56</v>
@@ -11198,7 +11198,7 @@
       </c>
       <c r="C155" s="62"/>
       <c r="D155" s="62" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E155" s="62" t="s">
         <v>57</v>
@@ -11207,7 +11207,7 @@
         <v>44</v>
       </c>
       <c r="H155" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I155" s="62">
         <v>18</v>
@@ -11220,7 +11220,7 @@
       </c>
       <c r="C156" s="62"/>
       <c r="D156" s="62" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E156" s="62" t="s">
         <v>58</v>
@@ -11229,7 +11229,7 @@
         <v>44</v>
       </c>
       <c r="H156" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I156" s="62">
         <v>9</v>
@@ -11240,13 +11240,13 @@
         <v>1</v>
       </c>
       <c r="B157" s="58" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C157" s="58" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="D157" s="58" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E157" s="58" t="s">
         <v>48</v>
@@ -11299,13 +11299,13 @@
         <v>1</v>
       </c>
       <c r="B159" s="58" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C159" s="58" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D159" s="58" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E159" s="58" t="s">
         <v>46</v>
@@ -11319,7 +11319,7 @@
       </c>
       <c r="C160" s="62"/>
       <c r="D160" s="62" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E160" s="62" t="s">
         <v>257</v>
@@ -11379,7 +11379,7 @@
       </c>
       <c r="C162" s="62"/>
       <c r="D162" s="62" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E162" s="62" t="s">
         <v>50</v>
@@ -11399,7 +11399,7 @@
       </c>
       <c r="C163" s="62"/>
       <c r="D163" s="62" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E163" s="62" t="s">
         <v>51</v>
@@ -11408,7 +11408,7 @@
         <v>44</v>
       </c>
       <c r="H163" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I163" s="62">
         <v>18</v>
@@ -11421,7 +11421,7 @@
       </c>
       <c r="C164" s="62"/>
       <c r="D164" s="62" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E164" s="62" t="s">
         <v>52</v>
@@ -11430,7 +11430,7 @@
         <v>44</v>
       </c>
       <c r="H164" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I164" s="62">
         <v>9</v>
@@ -11443,7 +11443,7 @@
       </c>
       <c r="C165" s="62"/>
       <c r="D165" s="62" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E165" s="62" t="s">
         <v>53</v>
@@ -11463,7 +11463,7 @@
       </c>
       <c r="C166" s="62"/>
       <c r="D166" s="62" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E166" s="62" t="s">
         <v>54</v>
@@ -11472,7 +11472,7 @@
         <v>44</v>
       </c>
       <c r="H166" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I166" s="62">
         <v>18</v>
@@ -11485,7 +11485,7 @@
       </c>
       <c r="C167" s="62"/>
       <c r="D167" s="62" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E167" s="62" t="s">
         <v>55</v>
@@ -11494,7 +11494,7 @@
         <v>44</v>
       </c>
       <c r="H167" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I167" s="62">
         <v>9</v>
@@ -11507,7 +11507,7 @@
       </c>
       <c r="C168" s="62"/>
       <c r="D168" s="62" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E168" s="62" t="s">
         <v>56</v>
@@ -11527,7 +11527,7 @@
       </c>
       <c r="C169" s="62"/>
       <c r="D169" s="62" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E169" s="62" t="s">
         <v>57</v>
@@ -11536,7 +11536,7 @@
         <v>44</v>
       </c>
       <c r="H169" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I169" s="62">
         <v>18</v>
@@ -11549,7 +11549,7 @@
       </c>
       <c r="C170" s="62"/>
       <c r="D170" s="62" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E170" s="62" t="s">
         <v>58</v>
@@ -11558,7 +11558,7 @@
         <v>44</v>
       </c>
       <c r="H170" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I170" s="62">
         <v>9</v>
@@ -11569,13 +11569,13 @@
         <v>1</v>
       </c>
       <c r="B171" s="58" t="s">
+        <v>341</v>
+      </c>
+      <c r="C171" s="58" t="s">
+        <v>410</v>
+      </c>
+      <c r="D171" s="58" t="s">
         <v>342</v>
-      </c>
-      <c r="C171" s="58" t="s">
-        <v>411</v>
-      </c>
-      <c r="D171" s="58" t="s">
-        <v>343</v>
       </c>
       <c r="E171" s="58" t="s">
         <v>46</v>
@@ -11628,13 +11628,13 @@
         <v>1</v>
       </c>
       <c r="B173" s="58" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C173" s="58" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D173" s="58" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E173" s="58" t="s">
         <v>46</v>
@@ -11689,10 +11689,10 @@
       </c>
       <c r="C175" s="62"/>
       <c r="D175" s="62" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E175" s="62" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="G175" s="62" t="s">
         <v>44</v>
@@ -11709,10 +11709,10 @@
       </c>
       <c r="C176" s="62"/>
       <c r="D176" s="62" t="s">
+        <v>574</v>
+      </c>
+      <c r="E176" s="62" t="s">
         <v>576</v>
-      </c>
-      <c r="E176" s="62" t="s">
-        <v>578</v>
       </c>
       <c r="G176" s="62" t="s">
         <v>44</v>
@@ -11729,7 +11729,7 @@
       </c>
       <c r="C177" s="62"/>
       <c r="D177" s="62" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E177" s="62" t="s">
         <v>50</v>
@@ -11749,7 +11749,7 @@
       </c>
       <c r="C178" s="62"/>
       <c r="D178" s="62" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E178" s="62" t="s">
         <v>51</v>
@@ -11758,7 +11758,7 @@
         <v>44</v>
       </c>
       <c r="H178" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I178" s="62">
         <v>18</v>
@@ -11771,7 +11771,7 @@
       </c>
       <c r="C179" s="62"/>
       <c r="D179" s="62" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E179" s="62" t="s">
         <v>52</v>
@@ -11780,7 +11780,7 @@
         <v>44</v>
       </c>
       <c r="H179" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I179" s="62">
         <v>9</v>
@@ -11793,7 +11793,7 @@
       </c>
       <c r="C180" s="62"/>
       <c r="D180" s="62" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E180" s="62" t="s">
         <v>53</v>
@@ -11813,7 +11813,7 @@
       </c>
       <c r="C181" s="62"/>
       <c r="D181" s="62" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E181" s="62" t="s">
         <v>54</v>
@@ -11822,7 +11822,7 @@
         <v>44</v>
       </c>
       <c r="H181" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I181" s="62">
         <v>18</v>
@@ -11835,7 +11835,7 @@
       </c>
       <c r="C182" s="62"/>
       <c r="D182" s="62" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E182" s="62" t="s">
         <v>55</v>
@@ -11844,7 +11844,7 @@
         <v>44</v>
       </c>
       <c r="H182" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I182" s="62">
         <v>9</v>
@@ -11857,7 +11857,7 @@
       </c>
       <c r="C183" s="62"/>
       <c r="D183" s="62" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E183" s="62" t="s">
         <v>56</v>
@@ -11877,7 +11877,7 @@
       </c>
       <c r="C184" s="62"/>
       <c r="D184" s="62" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E184" s="62" t="s">
         <v>57</v>
@@ -11886,7 +11886,7 @@
         <v>44</v>
       </c>
       <c r="H184" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I184" s="62">
         <v>18</v>
@@ -11899,7 +11899,7 @@
       </c>
       <c r="C185" s="62"/>
       <c r="D185" s="62" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E185" s="62" t="s">
         <v>58</v>
@@ -11908,7 +11908,7 @@
         <v>44</v>
       </c>
       <c r="H185" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I185" s="62">
         <v>9</v>
@@ -11919,13 +11919,13 @@
         <v>1</v>
       </c>
       <c r="B186" s="58" t="s">
+        <v>343</v>
+      </c>
+      <c r="C186" s="58" t="s">
+        <v>422</v>
+      </c>
+      <c r="D186" s="58" t="s">
         <v>344</v>
-      </c>
-      <c r="C186" s="58" t="s">
-        <v>423</v>
-      </c>
-      <c r="D186" s="58" t="s">
-        <v>345</v>
       </c>
       <c r="E186" s="58" t="s">
         <v>46</v>
@@ -11980,16 +11980,16 @@
       </c>
       <c r="C188" s="62"/>
       <c r="D188" s="62" t="s">
+        <v>345</v>
+      </c>
+      <c r="E188" s="62" t="s">
         <v>346</v>
-      </c>
-      <c r="E188" s="62" t="s">
-        <v>347</v>
       </c>
       <c r="G188" s="62" t="s">
         <v>44</v>
       </c>
       <c r="H188" s="62" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I188" s="62">
         <v>10</v>
@@ -12000,13 +12000,13 @@
         <v>1</v>
       </c>
       <c r="B189" s="58" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C189" s="58" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D189" s="58" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E189" s="58" t="s">
         <v>46</v>
@@ -12059,13 +12059,13 @@
         <v>1</v>
       </c>
       <c r="B191" s="58" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C191" s="58" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D191" s="58" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E191" s="58" t="s">
         <v>46</v>
@@ -12120,16 +12120,16 @@
       </c>
       <c r="C193" s="62"/>
       <c r="D193" s="62" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E193" s="62" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G193" s="62" t="s">
         <v>44</v>
       </c>
       <c r="H193" s="62" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I193" s="62">
         <v>30</v>
@@ -12140,13 +12140,13 @@
         <v>1</v>
       </c>
       <c r="B194" s="58" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C194" s="58" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D194" s="58" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E194" s="58" t="s">
         <v>48</v>
@@ -12199,13 +12199,13 @@
         <v>1</v>
       </c>
       <c r="B196" s="58" t="s">
+        <v>347</v>
+      </c>
+      <c r="C196" s="58" t="s">
+        <v>423</v>
+      </c>
+      <c r="D196" s="58" t="s">
         <v>348</v>
-      </c>
-      <c r="C196" s="58" t="s">
-        <v>424</v>
-      </c>
-      <c r="D196" s="58" t="s">
-        <v>349</v>
       </c>
       <c r="E196" s="58" t="s">
         <v>46</v>
@@ -12260,10 +12260,10 @@
       </c>
       <c r="C198" s="62"/>
       <c r="D198" s="62" t="s">
+        <v>349</v>
+      </c>
+      <c r="E198" s="62" t="s">
         <v>350</v>
-      </c>
-      <c r="E198" s="62" t="s">
-        <v>351</v>
       </c>
       <c r="G198" s="62" t="s">
         <v>44</v>
@@ -12280,16 +12280,16 @@
       </c>
       <c r="C199" s="62"/>
       <c r="D199" s="62" t="s">
+        <v>351</v>
+      </c>
+      <c r="E199" s="62" t="s">
         <v>352</v>
-      </c>
-      <c r="E199" s="62" t="s">
-        <v>353</v>
       </c>
       <c r="G199" s="62" t="s">
         <v>44</v>
       </c>
       <c r="H199" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I199" s="62">
         <v>9</v>
@@ -12302,16 +12302,16 @@
       </c>
       <c r="C200" s="62"/>
       <c r="D200" s="62" t="s">
+        <v>353</v>
+      </c>
+      <c r="E200" s="62" t="s">
         <v>354</v>
-      </c>
-      <c r="E200" s="62" t="s">
-        <v>355</v>
       </c>
       <c r="G200" s="62" t="s">
         <v>44</v>
       </c>
       <c r="H200" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I200" s="62">
         <v>16</v>
@@ -12322,13 +12322,13 @@
         <v>1</v>
       </c>
       <c r="B201" s="58" t="s">
+        <v>355</v>
+      </c>
+      <c r="C201" s="58" t="s">
+        <v>424</v>
+      </c>
+      <c r="D201" s="58" t="s">
         <v>356</v>
-      </c>
-      <c r="C201" s="58" t="s">
-        <v>425</v>
-      </c>
-      <c r="D201" s="58" t="s">
-        <v>357</v>
       </c>
       <c r="E201" s="58" t="s">
         <v>46</v>
@@ -12383,7 +12383,7 @@
       </c>
       <c r="C203" s="62"/>
       <c r="D203" s="62" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E203" s="62" t="s">
         <v>41</v>
@@ -12392,7 +12392,7 @@
         <v>44</v>
       </c>
       <c r="H203" s="62" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I203" s="62">
         <v>20</v>
@@ -12403,13 +12403,13 @@
         <v>1</v>
       </c>
       <c r="B204" s="58" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C204" s="58" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D204" s="58" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E204" s="58" t="s">
         <v>48</v>
@@ -12462,13 +12462,13 @@
         <v>1</v>
       </c>
       <c r="B206" s="58" t="s">
+        <v>358</v>
+      </c>
+      <c r="C206" s="58" t="s">
+        <v>425</v>
+      </c>
+      <c r="D206" s="58" t="s">
         <v>359</v>
-      </c>
-      <c r="C206" s="58" t="s">
-        <v>426</v>
-      </c>
-      <c r="D206" s="58" t="s">
-        <v>360</v>
       </c>
       <c r="E206" s="58" t="s">
         <v>46</v>
@@ -12521,13 +12521,13 @@
         <v>1</v>
       </c>
       <c r="B208" s="58" t="s">
+        <v>360</v>
+      </c>
+      <c r="C208" s="58" t="s">
+        <v>426</v>
+      </c>
+      <c r="D208" s="58" t="s">
         <v>361</v>
-      </c>
-      <c r="C208" s="58" t="s">
-        <v>427</v>
-      </c>
-      <c r="D208" s="58" t="s">
-        <v>362</v>
       </c>
       <c r="E208" s="58" t="s">
         <v>46</v>
@@ -12580,13 +12580,13 @@
         <v>1</v>
       </c>
       <c r="B210" s="58" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C210" s="58" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D210" s="58" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E210" s="58" t="s">
         <v>46</v>
@@ -12639,13 +12639,13 @@
         <v>1</v>
       </c>
       <c r="B212" s="58" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C212" s="58" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D212" s="58" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E212" s="58" t="s">
         <v>46</v>
@@ -12698,13 +12698,13 @@
         <v>1</v>
       </c>
       <c r="B214" s="58" t="s">
+        <v>362</v>
+      </c>
+      <c r="C214" s="58" t="s">
+        <v>427</v>
+      </c>
+      <c r="D214" s="58" t="s">
         <v>363</v>
-      </c>
-      <c r="C214" s="58" t="s">
-        <v>428</v>
-      </c>
-      <c r="D214" s="58" t="s">
-        <v>364</v>
       </c>
       <c r="E214" s="58" t="s">
         <v>46</v>
@@ -12757,13 +12757,13 @@
         <v>1</v>
       </c>
       <c r="B216" s="58" t="s">
+        <v>364</v>
+      </c>
+      <c r="C216" s="58" t="s">
+        <v>428</v>
+      </c>
+      <c r="D216" s="58" t="s">
         <v>365</v>
-      </c>
-      <c r="C216" s="58" t="s">
-        <v>429</v>
-      </c>
-      <c r="D216" s="58" t="s">
-        <v>366</v>
       </c>
       <c r="E216" s="58" t="s">
         <v>46</v>
@@ -12818,16 +12818,16 @@
       </c>
       <c r="C218" s="62"/>
       <c r="D218" s="62" t="s">
+        <v>366</v>
+      </c>
+      <c r="E218" s="62" t="s">
         <v>367</v>
-      </c>
-      <c r="E218" s="62" t="s">
-        <v>368</v>
       </c>
       <c r="G218" s="62" t="s">
         <v>44</v>
       </c>
       <c r="H218" s="62" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I218" s="62">
         <v>15</v>
@@ -12847,7 +12847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
@@ -13055,12 +13055,12 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="35"/>
       <c r="D7" s="35" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>93</v>
@@ -13461,14 +13461,14 @@
     </row>
     <row r="21" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="46" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C21" s="46"/>
       <c r="D21" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E21" s="46"/>
       <c r="F21" s="46" t="s">
@@ -13480,8 +13480,8 @@
       <c r="H21" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="I21" s="46" t="b">
-        <v>1</v>
+      <c r="I21" s="35" t="b">
+        <v>0</v>
       </c>
       <c r="J21" s="46"/>
       <c r="K21" s="46"/>
@@ -13490,13 +13490,13 @@
     </row>
     <row r="22" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F22" s="47" t="s">
         <v>43</v>
@@ -13507,19 +13507,19 @@
       <c r="H22" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I22" s="47" t="b">
-        <v>1</v>
+      <c r="I22" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>374</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>375</v>
       </c>
       <c r="F23" s="47" t="s">
         <v>43</v>
@@ -13530,19 +13530,19 @@
       <c r="H23" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I23" s="47" t="b">
-        <v>1</v>
+      <c r="I23" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="F24" s="47" t="s">
         <v>43</v>
@@ -13553,19 +13553,19 @@
       <c r="H24" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I24" s="47" t="b">
-        <v>1</v>
+      <c r="I24" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F25" s="47" t="s">
         <v>43</v>
@@ -13576,19 +13576,19 @@
       <c r="H25" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I25" s="47" t="b">
-        <v>1</v>
+      <c r="I25" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F26" s="47" t="s">
         <v>43</v>
@@ -13599,19 +13599,19 @@
       <c r="H26" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I26" s="47" t="b">
-        <v>1</v>
+      <c r="I26" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F27" s="47" t="s">
         <v>43</v>
@@ -13622,19 +13622,19 @@
       <c r="H27" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I27" s="47" t="b">
-        <v>1</v>
+      <c r="I27" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>387</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>388</v>
       </c>
       <c r="F28" s="47" t="s">
         <v>43</v>
@@ -13645,19 +13645,19 @@
       <c r="H28" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I28" s="47" t="b">
-        <v>1</v>
+      <c r="I28" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>389</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>390</v>
       </c>
       <c r="F29" s="47" t="s">
         <v>43</v>
@@ -13668,19 +13668,19 @@
       <c r="H29" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I29" s="47" t="b">
-        <v>1</v>
+      <c r="I29" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>391</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>392</v>
       </c>
       <c r="F30" s="47" t="s">
         <v>43</v>
@@ -13691,19 +13691,19 @@
       <c r="H30" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I30" s="47" t="b">
-        <v>1</v>
+      <c r="I30" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F31" s="47" t="s">
         <v>43</v>
@@ -13714,19 +13714,19 @@
       <c r="H31" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I31" s="47" t="b">
-        <v>1</v>
+      <c r="I31" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F32" s="47" t="s">
         <v>43</v>
@@ -13737,19 +13737,19 @@
       <c r="H32" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I32" s="47" t="b">
-        <v>1</v>
+      <c r="I32" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F33" s="47" t="s">
         <v>43</v>
@@ -13760,19 +13760,19 @@
       <c r="H33" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I33" s="47" t="b">
-        <v>1</v>
+      <c r="I33" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>393</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>394</v>
       </c>
       <c r="F34" s="47" t="s">
         <v>43</v>
@@ -13783,19 +13783,19 @@
       <c r="H34" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="I34" s="47" t="b">
-        <v>1</v>
+      <c r="I34" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="52" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B35" s="52" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="F35" s="55" t="s">
         <v>43</v>
@@ -13806,19 +13806,19 @@
       <c r="H35" s="55" t="b">
         <v>1</v>
       </c>
-      <c r="I35" s="55" t="b">
-        <v>1</v>
+      <c r="I35" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="52" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B36" s="52" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D36" s="52" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F36" s="55" t="s">
         <v>43</v>
@@ -13829,19 +13829,19 @@
       <c r="H36" s="55" t="b">
         <v>1</v>
       </c>
-      <c r="I36" s="55" t="b">
-        <v>1</v>
+      <c r="I36" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="52" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B37" s="52" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D37" s="52" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F37" s="55" t="s">
         <v>43</v>
@@ -13852,19 +13852,19 @@
       <c r="H37" s="55" t="b">
         <v>1</v>
       </c>
-      <c r="I37" s="55" t="b">
-        <v>1</v>
+      <c r="I37" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="52" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B38" s="52" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="F38" s="55" t="s">
         <v>43</v>
@@ -13875,19 +13875,19 @@
       <c r="H38" s="55" t="b">
         <v>1</v>
       </c>
-      <c r="I38" s="55" t="b">
-        <v>1</v>
+      <c r="I38" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="52" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B39" s="52" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D39" s="52" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F39" s="55" t="s">
         <v>43</v>
@@ -13898,19 +13898,19 @@
       <c r="H39" s="55" t="b">
         <v>1</v>
       </c>
-      <c r="I39" s="55" t="b">
-        <v>1</v>
+      <c r="I39" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="52" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B40" s="52" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D40" s="52" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F40" s="55" t="s">
         <v>43</v>
@@ -13921,19 +13921,19 @@
       <c r="H40" s="55" t="b">
         <v>1</v>
       </c>
-      <c r="I40" s="55" t="b">
-        <v>1</v>
+      <c r="I40" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="52" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B41" s="52" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F41" s="55" t="s">
         <v>43</v>
@@ -13944,19 +13944,19 @@
       <c r="H41" s="55" t="b">
         <v>1</v>
       </c>
-      <c r="I41" s="55" t="b">
-        <v>1</v>
+      <c r="I41" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="52" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B42" s="52" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D42" s="52" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F42" s="55" t="s">
         <v>43</v>
@@ -13967,19 +13967,19 @@
       <c r="H42" s="55" t="b">
         <v>1</v>
       </c>
-      <c r="I42" s="55" t="b">
-        <v>1</v>
+      <c r="I42" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="52" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B43" s="52" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D43" s="52" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F43" s="55" t="s">
         <v>43</v>
@@ -13990,19 +13990,19 @@
       <c r="H43" s="55" t="b">
         <v>1</v>
       </c>
-      <c r="I43" s="55" t="b">
-        <v>1</v>
+      <c r="I43" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="52" t="s">
+        <v>395</v>
+      </c>
+      <c r="B44" s="52" t="s">
+        <v>395</v>
+      </c>
+      <c r="D44" s="52" t="s">
         <v>396</v>
-      </c>
-      <c r="B44" s="52" t="s">
-        <v>396</v>
-      </c>
-      <c r="D44" s="52" t="s">
-        <v>397</v>
       </c>
       <c r="F44" s="55" t="s">
         <v>43</v>
@@ -14013,19 +14013,19 @@
       <c r="H44" s="55" t="b">
         <v>1</v>
       </c>
-      <c r="I44" s="55" t="b">
-        <v>1</v>
+      <c r="I44" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="52" t="s">
+        <v>397</v>
+      </c>
+      <c r="B45" s="52" t="s">
+        <v>397</v>
+      </c>
+      <c r="D45" s="52" t="s">
         <v>398</v>
-      </c>
-      <c r="B45" s="52" t="s">
-        <v>398</v>
-      </c>
-      <c r="D45" s="52" t="s">
-        <v>399</v>
       </c>
       <c r="F45" s="55" t="s">
         <v>43</v>
@@ -14036,19 +14036,19 @@
       <c r="H45" s="55" t="b">
         <v>1</v>
       </c>
-      <c r="I45" s="55" t="b">
-        <v>1</v>
+      <c r="I45" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="50" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D46" s="50" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F46" s="54" t="s">
         <v>43</v>
@@ -14059,19 +14059,19 @@
       <c r="H46" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I46" s="54" t="b">
-        <v>1</v>
+      <c r="I46" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="50" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B47" s="50" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D47" s="50" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F47" s="54" t="s">
         <v>43</v>
@@ -14082,19 +14082,19 @@
       <c r="H47" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I47" s="54" t="b">
-        <v>1</v>
+      <c r="I47" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="50" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D48" s="50" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F48" s="54" t="s">
         <v>43</v>
@@ -14105,19 +14105,19 @@
       <c r="H48" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I48" s="54" t="b">
-        <v>1</v>
+      <c r="I48" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="50" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B49" s="50" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D49" s="50" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F49" s="54" t="s">
         <v>43</v>
@@ -14128,19 +14128,19 @@
       <c r="H49" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I49" s="54" t="b">
-        <v>1</v>
+      <c r="I49" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="50" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="50" t="s">
+        <v>399</v>
+      </c>
+      <c r="B50" s="50" t="s">
+        <v>399</v>
+      </c>
+      <c r="D50" s="50" t="s">
         <v>400</v>
-      </c>
-      <c r="B50" s="50" t="s">
-        <v>400</v>
-      </c>
-      <c r="D50" s="50" t="s">
-        <v>401</v>
       </c>
       <c r="F50" s="54" t="s">
         <v>43</v>
@@ -14151,19 +14151,19 @@
       <c r="H50" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I50" s="54" t="b">
-        <v>1</v>
+      <c r="I50" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="50" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D51" s="50" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F51" s="54" t="s">
         <v>43</v>
@@ -14174,19 +14174,19 @@
       <c r="H51" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I51" s="54" t="b">
-        <v>1</v>
+      <c r="I51" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="50" t="s">
+        <v>401</v>
+      </c>
+      <c r="B52" s="50" t="s">
+        <v>401</v>
+      </c>
+      <c r="D52" s="50" t="s">
         <v>402</v>
-      </c>
-      <c r="B52" s="50" t="s">
-        <v>402</v>
-      </c>
-      <c r="D52" s="50" t="s">
-        <v>403</v>
       </c>
       <c r="F52" s="54" t="s">
         <v>43</v>
@@ -14197,19 +14197,19 @@
       <c r="H52" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I52" s="54" t="b">
-        <v>1</v>
+      <c r="I52" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="50" t="s">
+        <v>403</v>
+      </c>
+      <c r="B53" s="50" t="s">
+        <v>403</v>
+      </c>
+      <c r="D53" s="50" t="s">
         <v>404</v>
-      </c>
-      <c r="B53" s="50" t="s">
-        <v>404</v>
-      </c>
-      <c r="D53" s="50" t="s">
-        <v>405</v>
       </c>
       <c r="F53" s="54" t="s">
         <v>43</v>
@@ -14220,19 +14220,19 @@
       <c r="H53" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I53" s="54" t="b">
-        <v>1</v>
+      <c r="I53" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="50" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D54" s="50" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F54" s="54" t="s">
         <v>43</v>
@@ -14243,19 +14243,19 @@
       <c r="H54" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I54" s="54" t="b">
-        <v>1</v>
+      <c r="I54" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="50" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B55" s="50" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D55" s="50" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="F55" s="54" t="s">
         <v>43</v>
@@ -14266,19 +14266,19 @@
       <c r="H55" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I55" s="54" t="b">
-        <v>1</v>
+      <c r="I55" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="50" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B56" s="50" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D56" s="50" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F56" s="54" t="s">
         <v>43</v>
@@ -14289,19 +14289,19 @@
       <c r="H56" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I56" s="54" t="b">
-        <v>1</v>
+      <c r="I56" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="50" t="s">
+        <v>411</v>
+      </c>
+      <c r="B57" s="50" t="s">
+        <v>411</v>
+      </c>
+      <c r="D57" s="50" t="s">
         <v>412</v>
-      </c>
-      <c r="B57" s="50" t="s">
-        <v>412</v>
-      </c>
-      <c r="D57" s="50" t="s">
-        <v>413</v>
       </c>
       <c r="F57" s="54" t="s">
         <v>43</v>
@@ -14312,19 +14312,19 @@
       <c r="H57" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I57" s="54" t="b">
-        <v>1</v>
+      <c r="I57" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="50" t="s">
+        <v>413</v>
+      </c>
+      <c r="B58" s="50" t="s">
+        <v>413</v>
+      </c>
+      <c r="D58" s="50" t="s">
         <v>414</v>
-      </c>
-      <c r="B58" s="50" t="s">
-        <v>414</v>
-      </c>
-      <c r="D58" s="50" t="s">
-        <v>415</v>
       </c>
       <c r="F58" s="54" t="s">
         <v>43</v>
@@ -14335,19 +14335,19 @@
       <c r="H58" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I58" s="54" t="b">
-        <v>1</v>
+      <c r="I58" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="50" t="s">
+        <v>415</v>
+      </c>
+      <c r="B59" s="50" t="s">
+        <v>415</v>
+      </c>
+      <c r="D59" s="50" t="s">
         <v>416</v>
-      </c>
-      <c r="B59" s="50" t="s">
-        <v>416</v>
-      </c>
-      <c r="D59" s="50" t="s">
-        <v>417</v>
       </c>
       <c r="F59" s="54" t="s">
         <v>43</v>
@@ -14358,19 +14358,19 @@
       <c r="H59" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I59" s="54" t="b">
-        <v>1</v>
+      <c r="I59" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="50" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B60" s="50" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D60" s="50" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F60" s="54" t="s">
         <v>43</v>
@@ -14381,19 +14381,19 @@
       <c r="H60" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I60" s="54" t="b">
-        <v>1</v>
+      <c r="I60" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="50" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D61" s="50" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F61" s="54" t="s">
         <v>43</v>
@@ -14404,19 +14404,19 @@
       <c r="H61" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I61" s="54" t="b">
-        <v>1</v>
+      <c r="I61" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="58" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B62" s="58" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D62" s="58" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="F62" s="60" t="s">
         <v>43</v>
@@ -14427,19 +14427,19 @@
       <c r="H62" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I62" s="60" t="b">
-        <v>1</v>
+      <c r="I62" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="58" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B63" s="58" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D63" s="58" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="F63" s="60" t="s">
         <v>43</v>
@@ -14450,19 +14450,19 @@
       <c r="H63" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I63" s="60" t="b">
-        <v>1</v>
+      <c r="I63" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="58" t="s">
+        <v>417</v>
+      </c>
+      <c r="B64" s="58" t="s">
+        <v>417</v>
+      </c>
+      <c r="D64" s="58" t="s">
         <v>418</v>
-      </c>
-      <c r="B64" s="58" t="s">
-        <v>418</v>
-      </c>
-      <c r="D64" s="58" t="s">
-        <v>419</v>
       </c>
       <c r="F64" s="60" t="s">
         <v>43</v>
@@ -14473,19 +14473,19 @@
       <c r="H64" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I64" s="60" t="b">
-        <v>1</v>
+      <c r="I64" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="58" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B65" s="58" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D65" s="58" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="F65" s="60" t="s">
         <v>43</v>
@@ -14496,19 +14496,19 @@
       <c r="H65" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I65" s="60" t="b">
-        <v>1</v>
+      <c r="I65" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="58" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B66" s="58" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D66" s="58" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F66" s="60" t="s">
         <v>43</v>
@@ -14519,19 +14519,19 @@
       <c r="H66" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I66" s="60" t="b">
-        <v>1</v>
+      <c r="I66" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="58" t="s">
+        <v>420</v>
+      </c>
+      <c r="B67" s="58" t="s">
+        <v>420</v>
+      </c>
+      <c r="D67" s="58" t="s">
         <v>421</v>
-      </c>
-      <c r="B67" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="D67" s="58" t="s">
-        <v>422</v>
       </c>
       <c r="F67" s="60" t="s">
         <v>43</v>
@@ -14542,19 +14542,19 @@
       <c r="H67" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I67" s="60" t="b">
-        <v>1</v>
+      <c r="I67" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="58" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B68" s="58" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D68" s="58" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F68" s="60" t="s">
         <v>43</v>
@@ -14565,19 +14565,19 @@
       <c r="H68" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I68" s="60" t="b">
-        <v>1</v>
+      <c r="I68" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="58" t="s">
+        <v>429</v>
+      </c>
+      <c r="B69" s="58" t="s">
+        <v>429</v>
+      </c>
+      <c r="D69" s="58" t="s">
         <v>430</v>
-      </c>
-      <c r="B69" s="58" t="s">
-        <v>430</v>
-      </c>
-      <c r="D69" s="58" t="s">
-        <v>431</v>
       </c>
       <c r="F69" s="60" t="s">
         <v>43</v>
@@ -14588,19 +14588,19 @@
       <c r="H69" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I69" s="60" t="b">
-        <v>1</v>
+      <c r="I69" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="58" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B70" s="58" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D70" s="58" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="F70" s="60" t="s">
         <v>43</v>
@@ -14611,19 +14611,19 @@
       <c r="H70" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I70" s="60" t="b">
-        <v>1</v>
+      <c r="I70" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="58" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B71" s="58" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D71" s="58" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F71" s="60" t="s">
         <v>43</v>
@@ -14634,19 +14634,19 @@
       <c r="H71" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I71" s="60" t="b">
-        <v>1</v>
+      <c r="I71" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="58" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B72" s="58" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D72" s="58" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F72" s="60" t="s">
         <v>43</v>
@@ -14657,19 +14657,19 @@
       <c r="H72" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I72" s="60" t="b">
-        <v>1</v>
+      <c r="I72" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="58" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B73" s="58" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D73" s="58" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="F73" s="60" t="s">
         <v>43</v>
@@ -14680,19 +14680,19 @@
       <c r="H73" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I73" s="60" t="b">
-        <v>1</v>
+      <c r="I73" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="58" t="s">
+        <v>431</v>
+      </c>
+      <c r="B74" s="58" t="s">
+        <v>431</v>
+      </c>
+      <c r="D74" s="58" t="s">
         <v>432</v>
-      </c>
-      <c r="B74" s="58" t="s">
-        <v>432</v>
-      </c>
-      <c r="D74" s="58" t="s">
-        <v>433</v>
       </c>
       <c r="F74" s="60" t="s">
         <v>43</v>
@@ -14703,19 +14703,19 @@
       <c r="H74" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I74" s="60" t="b">
-        <v>1</v>
+      <c r="I74" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="58" t="s">
+        <v>433</v>
+      </c>
+      <c r="B75" s="58" t="s">
+        <v>433</v>
+      </c>
+      <c r="D75" s="58" t="s">
         <v>434</v>
-      </c>
-      <c r="B75" s="58" t="s">
-        <v>434</v>
-      </c>
-      <c r="D75" s="58" t="s">
-        <v>435</v>
       </c>
       <c r="F75" s="60" t="s">
         <v>43</v>
@@ -14726,19 +14726,19 @@
       <c r="H75" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I75" s="60" t="b">
-        <v>1</v>
+      <c r="I75" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="58" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B76" s="58" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D76" s="58" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F76" s="60" t="s">
         <v>43</v>
@@ -14749,19 +14749,19 @@
       <c r="H76" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I76" s="60" t="b">
-        <v>1</v>
+      <c r="I76" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="58" t="s">
+        <v>435</v>
+      </c>
+      <c r="B77" s="58" t="s">
+        <v>435</v>
+      </c>
+      <c r="D77" s="58" t="s">
         <v>436</v>
-      </c>
-      <c r="B77" s="58" t="s">
-        <v>436</v>
-      </c>
-      <c r="D77" s="58" t="s">
-        <v>437</v>
       </c>
       <c r="F77" s="60" t="s">
         <v>43</v>
@@ -14772,19 +14772,19 @@
       <c r="H77" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I77" s="60" t="b">
-        <v>1</v>
+      <c r="I77" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="58" t="s">
+        <v>437</v>
+      </c>
+      <c r="B78" s="58" t="s">
+        <v>437</v>
+      </c>
+      <c r="D78" s="58" t="s">
         <v>438</v>
-      </c>
-      <c r="B78" s="58" t="s">
-        <v>438</v>
-      </c>
-      <c r="D78" s="58" t="s">
-        <v>439</v>
       </c>
       <c r="F78" s="60" t="s">
         <v>43</v>
@@ -14795,19 +14795,19 @@
       <c r="H78" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I78" s="60" t="b">
-        <v>1</v>
+      <c r="I78" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="58" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B79" s="58" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D79" s="58" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="F79" s="60" t="s">
         <v>43</v>
@@ -14818,19 +14818,19 @@
       <c r="H79" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I79" s="60" t="b">
-        <v>1</v>
+      <c r="I79" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="58" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B80" s="58" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D80" s="58" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="F80" s="60" t="s">
         <v>43</v>
@@ -14841,19 +14841,19 @@
       <c r="H80" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I80" s="60" t="b">
-        <v>1</v>
+      <c r="I80" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="58" t="s">
+        <v>439</v>
+      </c>
+      <c r="B81" s="58" t="s">
+        <v>439</v>
+      </c>
+      <c r="D81" s="58" t="s">
         <v>440</v>
-      </c>
-      <c r="B81" s="58" t="s">
-        <v>440</v>
-      </c>
-      <c r="D81" s="58" t="s">
-        <v>441</v>
       </c>
       <c r="F81" s="60" t="s">
         <v>43</v>
@@ -14864,19 +14864,19 @@
       <c r="H81" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I81" s="60" t="b">
-        <v>1</v>
+      <c r="I81" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="58" t="s">
+        <v>441</v>
+      </c>
+      <c r="B82" s="58" t="s">
+        <v>441</v>
+      </c>
+      <c r="D82" s="58" t="s">
         <v>442</v>
-      </c>
-      <c r="B82" s="58" t="s">
-        <v>442</v>
-      </c>
-      <c r="D82" s="58" t="s">
-        <v>443</v>
       </c>
       <c r="F82" s="60" t="s">
         <v>43</v>
@@ -14887,8 +14887,8 @@
       <c r="H82" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I82" s="60" t="b">
-        <v>1</v>
+      <c r="I82" s="35" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated server version to 1.15.0 per Ry
</commit_message>
<xml_diff>
--- a/projects/PTool_Full_Analysis.xlsx
+++ b/projects/PTool_Full_Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="5244" windowWidth="22368" windowHeight="5268" tabRatio="469" activeTab="3"/>
+    <workbookView xWindow="-12" yWindow="5244" windowWidth="22368" windowHeight="5268" tabRatio="469" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -1144,9 +1144,6 @@
     <t>aparker</t>
   </si>
   <si>
-    <t>1.14.7</t>
-  </si>
-  <si>
     <t>advanced_power_strips</t>
   </si>
   <si>
@@ -1970,6 +1967,9 @@
   </si>
   <si>
     <t>PToolFullCluster</t>
+  </si>
+  <si>
+    <t>1.15.0</t>
   </si>
 </sst>
 </file>
@@ -6706,8 +6706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6765,7 +6765,7 @@
         <v>94</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>369</v>
+        <v>644</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>178</v>
@@ -6776,7 +6776,7 @@
         <v>95</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>97</v>
@@ -6847,7 +6847,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>96</v>
@@ -7087,7 +7087,7 @@
         <v>198</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>232</v>
@@ -7269,7 +7269,7 @@
         <v>8</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="P3" s="16" t="s">
         <v>100</v>
@@ -7338,10 +7338,10 @@
         <v>255</v>
       </c>
       <c r="J5" s="30" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="P5" s="30" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="R5" s="30" t="s">
         <v>254</v>
@@ -7379,7 +7379,7 @@
         <v>245</v>
       </c>
       <c r="P6" s="30" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="R6" s="30" t="s">
         <v>254</v>
@@ -7417,7 +7417,7 @@
         <v>250</v>
       </c>
       <c r="P7" s="44" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="R7" s="30" t="s">
         <v>254</v>
@@ -7428,13 +7428,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>46</v>
@@ -7490,7 +7490,7 @@
         <v>303</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>304</v>
@@ -7758,13 +7758,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>48</v>
@@ -7817,13 +7817,13 @@
         <v>1</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>446</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>447</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>46</v>
@@ -7878,10 +7878,10 @@
       </c>
       <c r="C26" s="56"/>
       <c r="D26" s="56" t="s">
+        <v>447</v>
+      </c>
+      <c r="E26" s="56" t="s">
         <v>448</v>
-      </c>
-      <c r="E26" s="56" t="s">
-        <v>449</v>
       </c>
       <c r="G26" s="56" t="s">
         <v>44</v>
@@ -7900,10 +7900,10 @@
       </c>
       <c r="C27" s="56"/>
       <c r="D27" s="56" t="s">
+        <v>449</v>
+      </c>
+      <c r="E27" s="56" t="s">
         <v>450</v>
-      </c>
-      <c r="E27" s="56" t="s">
-        <v>451</v>
       </c>
       <c r="G27" s="56" t="s">
         <v>44</v>
@@ -7920,10 +7920,10 @@
       </c>
       <c r="C28" s="56"/>
       <c r="D28" s="56" t="s">
+        <v>451</v>
+      </c>
+      <c r="E28" s="56" t="s">
         <v>452</v>
-      </c>
-      <c r="E28" s="56" t="s">
-        <v>453</v>
       </c>
       <c r="G28" s="56" t="s">
         <v>44</v>
@@ -7938,10 +7938,10 @@
         <v>1</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>305</v>
@@ -8019,13 +8019,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>454</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>463</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>455</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>46</v>
@@ -8081,7 +8081,7 @@
         <v>308</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>309</v>
@@ -8140,7 +8140,7 @@
         <v>310</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>311</v>
@@ -8199,7 +8199,7 @@
         <v>312</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>313</v>
@@ -8255,13 +8255,13 @@
         <v>1</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>46</v>
@@ -8314,13 +8314,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>46</v>
@@ -8373,13 +8373,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>458</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>459</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>48</v>
@@ -8435,7 +8435,7 @@
         <v>314</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>315</v>
@@ -8703,13 +8703,13 @@
         <v>1</v>
       </c>
       <c r="B58" s="52" t="s">
+        <v>486</v>
+      </c>
+      <c r="C58" s="52" t="s">
+        <v>505</v>
+      </c>
+      <c r="D58" s="52" t="s">
         <v>487</v>
-      </c>
-      <c r="C58" s="52" t="s">
-        <v>506</v>
-      </c>
-      <c r="D58" s="52" t="s">
-        <v>488</v>
       </c>
       <c r="E58" s="52" t="s">
         <v>46</v>
@@ -8764,10 +8764,10 @@
       </c>
       <c r="C60" s="59"/>
       <c r="D60" s="59" t="s">
+        <v>488</v>
+      </c>
+      <c r="E60" s="59" t="s">
         <v>489</v>
-      </c>
-      <c r="E60" s="59" t="s">
-        <v>490</v>
       </c>
       <c r="G60" s="59" t="s">
         <v>44</v>
@@ -8784,10 +8784,10 @@
       </c>
       <c r="C61" s="59"/>
       <c r="D61" s="59" t="s">
+        <v>490</v>
+      </c>
+      <c r="E61" s="59" t="s">
         <v>491</v>
-      </c>
-      <c r="E61" s="59" t="s">
-        <v>492</v>
       </c>
       <c r="G61" s="59" t="s">
         <v>44</v>
@@ -8804,10 +8804,10 @@
       </c>
       <c r="C62" s="59"/>
       <c r="D62" s="59" t="s">
+        <v>492</v>
+      </c>
+      <c r="E62" s="59" t="s">
         <v>493</v>
-      </c>
-      <c r="E62" s="59" t="s">
-        <v>494</v>
       </c>
       <c r="G62" s="59" t="s">
         <v>44</v>
@@ -8822,10 +8822,10 @@
         <v>1</v>
       </c>
       <c r="B63" s="52" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C63" s="52" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D63" s="52" t="s">
         <v>316</v>
@@ -8881,13 +8881,13 @@
         <v>1</v>
       </c>
       <c r="B65" s="52" t="s">
+        <v>494</v>
+      </c>
+      <c r="C65" s="52" t="s">
+        <v>506</v>
+      </c>
+      <c r="D65" s="52" t="s">
         <v>495</v>
-      </c>
-      <c r="C65" s="52" t="s">
-        <v>507</v>
-      </c>
-      <c r="D65" s="52" t="s">
-        <v>496</v>
       </c>
       <c r="E65" s="52" t="s">
         <v>46</v>
@@ -8940,13 +8940,13 @@
         <v>1</v>
       </c>
       <c r="B67" s="52" t="s">
+        <v>496</v>
+      </c>
+      <c r="C67" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="D67" s="52" t="s">
         <v>497</v>
-      </c>
-      <c r="C67" s="52" t="s">
-        <v>508</v>
-      </c>
-      <c r="D67" s="52" t="s">
-        <v>498</v>
       </c>
       <c r="E67" s="52" t="s">
         <v>46</v>
@@ -8999,13 +8999,13 @@
         <v>1</v>
       </c>
       <c r="B69" s="52" t="s">
+        <v>498</v>
+      </c>
+      <c r="C69" s="52" t="s">
+        <v>508</v>
+      </c>
+      <c r="D69" s="52" t="s">
         <v>499</v>
-      </c>
-      <c r="C69" s="52" t="s">
-        <v>509</v>
-      </c>
-      <c r="D69" s="52" t="s">
-        <v>500</v>
       </c>
       <c r="E69" s="52" t="s">
         <v>46</v>
@@ -9058,13 +9058,13 @@
         <v>1</v>
       </c>
       <c r="B71" s="52" t="s">
+        <v>500</v>
+      </c>
+      <c r="C71" s="52" t="s">
+        <v>509</v>
+      </c>
+      <c r="D71" s="52" t="s">
         <v>501</v>
-      </c>
-      <c r="C71" s="52" t="s">
-        <v>510</v>
-      </c>
-      <c r="D71" s="52" t="s">
-        <v>502</v>
       </c>
       <c r="E71" s="52" t="s">
         <v>46</v>
@@ -9117,13 +9117,13 @@
         <v>1</v>
       </c>
       <c r="B73" s="52" t="s">
+        <v>502</v>
+      </c>
+      <c r="C73" s="52" t="s">
+        <v>510</v>
+      </c>
+      <c r="D73" s="52" t="s">
         <v>503</v>
-      </c>
-      <c r="C73" s="52" t="s">
-        <v>511</v>
-      </c>
-      <c r="D73" s="52" t="s">
-        <v>504</v>
       </c>
       <c r="E73" s="52" t="s">
         <v>46</v>
@@ -9176,13 +9176,13 @@
         <v>1</v>
       </c>
       <c r="B75" s="52" t="s">
+        <v>511</v>
+      </c>
+      <c r="C75" s="52" t="s">
         <v>512</v>
       </c>
-      <c r="C75" s="52" t="s">
-        <v>513</v>
-      </c>
       <c r="D75" s="52" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E75" s="52" t="s">
         <v>46</v>
@@ -9238,7 +9238,7 @@
         <v>317</v>
       </c>
       <c r="C77" s="52" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D77" s="52" t="s">
         <v>318</v>
@@ -9509,7 +9509,7 @@
         <v>319</v>
       </c>
       <c r="C89" s="52" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D89" s="52" t="s">
         <v>320</v>
@@ -9777,13 +9777,13 @@
         <v>1</v>
       </c>
       <c r="B101" s="50" t="s">
+        <v>528</v>
+      </c>
+      <c r="C101" s="50" t="s">
+        <v>547</v>
+      </c>
+      <c r="D101" s="50" t="s">
         <v>529</v>
-      </c>
-      <c r="C101" s="50" t="s">
-        <v>548</v>
-      </c>
-      <c r="D101" s="50" t="s">
-        <v>530</v>
       </c>
       <c r="E101" s="50" t="s">
         <v>46</v>
@@ -9836,13 +9836,13 @@
         <v>1</v>
       </c>
       <c r="B103" s="50" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C103" s="50" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D103" s="50" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E103" s="50" t="s">
         <v>46</v>
@@ -9917,13 +9917,13 @@
         <v>1</v>
       </c>
       <c r="B106" s="50" t="s">
+        <v>531</v>
+      </c>
+      <c r="C106" s="50" t="s">
+        <v>550</v>
+      </c>
+      <c r="D106" s="50" t="s">
         <v>532</v>
-      </c>
-      <c r="C106" s="50" t="s">
-        <v>551</v>
-      </c>
-      <c r="D106" s="50" t="s">
-        <v>533</v>
       </c>
       <c r="E106" s="50" t="s">
         <v>48</v>
@@ -9979,7 +9979,7 @@
         <v>321</v>
       </c>
       <c r="C108" s="50" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D108" s="50" t="s">
         <v>322</v>
@@ -10035,13 +10035,13 @@
         <v>1</v>
       </c>
       <c r="B110" s="50" t="s">
+        <v>533</v>
+      </c>
+      <c r="C110" s="50" t="s">
+        <v>551</v>
+      </c>
+      <c r="D110" s="50" t="s">
         <v>534</v>
-      </c>
-      <c r="C110" s="50" t="s">
-        <v>552</v>
-      </c>
-      <c r="D110" s="50" t="s">
-        <v>535</v>
       </c>
       <c r="E110" s="50" t="s">
         <v>46</v>
@@ -10279,7 +10279,7 @@
         <v>323</v>
       </c>
       <c r="C121" s="50" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D121" s="50" t="s">
         <v>324</v>
@@ -10338,7 +10338,7 @@
         <v>325</v>
       </c>
       <c r="C123" s="50" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D123" s="50" t="s">
         <v>326</v>
@@ -10394,13 +10394,13 @@
         <v>1</v>
       </c>
       <c r="B125" s="50" t="s">
+        <v>535</v>
+      </c>
+      <c r="C125" s="50" t="s">
+        <v>552</v>
+      </c>
+      <c r="D125" s="50" t="s">
         <v>536</v>
-      </c>
-      <c r="C125" s="50" t="s">
-        <v>553</v>
-      </c>
-      <c r="D125" s="50" t="s">
-        <v>537</v>
       </c>
       <c r="E125" s="50" t="s">
         <v>48</v>
@@ -10453,13 +10453,13 @@
         <v>1</v>
       </c>
       <c r="B127" s="50" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C127" s="50" t="s">
+        <v>553</v>
+      </c>
+      <c r="D127" s="50" t="s">
         <v>554</v>
-      </c>
-      <c r="D127" s="50" t="s">
-        <v>555</v>
       </c>
       <c r="E127" s="50" t="s">
         <v>46</v>
@@ -10515,7 +10515,7 @@
         <v>327</v>
       </c>
       <c r="C129" s="50" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D129" s="50" t="s">
         <v>328</v>
@@ -10574,7 +10574,7 @@
         <v>329</v>
       </c>
       <c r="C131" s="50" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D131" s="50" t="s">
         <v>330</v>
@@ -10655,7 +10655,7 @@
         <v>333</v>
       </c>
       <c r="C134" s="50" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D134" s="50" t="s">
         <v>334</v>
@@ -10733,13 +10733,13 @@
         <v>1</v>
       </c>
       <c r="B137" s="50" t="s">
+        <v>537</v>
+      </c>
+      <c r="C137" s="50" t="s">
+        <v>555</v>
+      </c>
+      <c r="D137" s="50" t="s">
         <v>538</v>
-      </c>
-      <c r="C137" s="50" t="s">
-        <v>556</v>
-      </c>
-      <c r="D137" s="50" t="s">
-        <v>539</v>
       </c>
       <c r="E137" s="50" t="s">
         <v>48</v>
@@ -10792,13 +10792,13 @@
         <v>1</v>
       </c>
       <c r="B139" s="50" t="s">
+        <v>539</v>
+      </c>
+      <c r="C139" s="50" t="s">
+        <v>556</v>
+      </c>
+      <c r="D139" s="50" t="s">
         <v>540</v>
-      </c>
-      <c r="C139" s="50" t="s">
-        <v>557</v>
-      </c>
-      <c r="D139" s="50" t="s">
-        <v>541</v>
       </c>
       <c r="E139" s="50" t="s">
         <v>48</v>
@@ -10851,13 +10851,13 @@
         <v>1</v>
       </c>
       <c r="B141" s="58" t="s">
+        <v>565</v>
+      </c>
+      <c r="C141" s="58" t="s">
+        <v>596</v>
+      </c>
+      <c r="D141" s="58" t="s">
         <v>566</v>
-      </c>
-      <c r="C141" s="58" t="s">
-        <v>597</v>
-      </c>
-      <c r="D141" s="58" t="s">
-        <v>567</v>
       </c>
       <c r="E141" s="58" t="s">
         <v>46</v>
@@ -10910,13 +10910,13 @@
         <v>1</v>
       </c>
       <c r="B143" s="58" t="s">
+        <v>567</v>
+      </c>
+      <c r="C143" s="58" t="s">
+        <v>597</v>
+      </c>
+      <c r="D143" s="58" t="s">
         <v>568</v>
-      </c>
-      <c r="C143" s="58" t="s">
-        <v>598</v>
-      </c>
-      <c r="D143" s="58" t="s">
-        <v>569</v>
       </c>
       <c r="E143" s="58" t="s">
         <v>48</v>
@@ -10972,7 +10972,7 @@
         <v>338</v>
       </c>
       <c r="C145" s="58" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D145" s="58" t="s">
         <v>339</v>
@@ -11240,13 +11240,13 @@
         <v>1</v>
       </c>
       <c r="B157" s="58" t="s">
+        <v>569</v>
+      </c>
+      <c r="C157" s="58" t="s">
+        <v>598</v>
+      </c>
+      <c r="D157" s="58" t="s">
         <v>570</v>
-      </c>
-      <c r="C157" s="58" t="s">
-        <v>599</v>
-      </c>
-      <c r="D157" s="58" t="s">
-        <v>571</v>
       </c>
       <c r="E157" s="58" t="s">
         <v>48</v>
@@ -11299,10 +11299,10 @@
         <v>1</v>
       </c>
       <c r="B159" s="58" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C159" s="58" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D159" s="58" t="s">
         <v>340</v>
@@ -11572,7 +11572,7 @@
         <v>341</v>
       </c>
       <c r="C171" s="58" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D171" s="58" t="s">
         <v>342</v>
@@ -11628,13 +11628,13 @@
         <v>1</v>
       </c>
       <c r="B173" s="58" t="s">
+        <v>571</v>
+      </c>
+      <c r="C173" s="58" t="s">
+        <v>599</v>
+      </c>
+      <c r="D173" s="58" t="s">
         <v>572</v>
-      </c>
-      <c r="C173" s="58" t="s">
-        <v>600</v>
-      </c>
-      <c r="D173" s="58" t="s">
-        <v>573</v>
       </c>
       <c r="E173" s="58" t="s">
         <v>46</v>
@@ -11689,10 +11689,10 @@
       </c>
       <c r="C175" s="62"/>
       <c r="D175" s="62" t="s">
+        <v>573</v>
+      </c>
+      <c r="E175" s="62" t="s">
         <v>574</v>
-      </c>
-      <c r="E175" s="62" t="s">
-        <v>575</v>
       </c>
       <c r="G175" s="62" t="s">
         <v>44</v>
@@ -11709,10 +11709,10 @@
       </c>
       <c r="C176" s="62"/>
       <c r="D176" s="62" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E176" s="62" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G176" s="62" t="s">
         <v>44</v>
@@ -11749,7 +11749,7 @@
       </c>
       <c r="C178" s="62"/>
       <c r="D178" s="62" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E178" s="62" t="s">
         <v>51</v>
@@ -11771,7 +11771,7 @@
       </c>
       <c r="C179" s="62"/>
       <c r="D179" s="62" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E179" s="62" t="s">
         <v>52</v>
@@ -11813,7 +11813,7 @@
       </c>
       <c r="C181" s="62"/>
       <c r="D181" s="62" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E181" s="62" t="s">
         <v>54</v>
@@ -11835,7 +11835,7 @@
       </c>
       <c r="C182" s="62"/>
       <c r="D182" s="62" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E182" s="62" t="s">
         <v>55</v>
@@ -11877,7 +11877,7 @@
       </c>
       <c r="C184" s="62"/>
       <c r="D184" s="62" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E184" s="62" t="s">
         <v>57</v>
@@ -11899,7 +11899,7 @@
       </c>
       <c r="C185" s="62"/>
       <c r="D185" s="62" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E185" s="62" t="s">
         <v>58</v>
@@ -11922,7 +11922,7 @@
         <v>343</v>
       </c>
       <c r="C186" s="58" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D186" s="58" t="s">
         <v>344</v>
@@ -12000,13 +12000,13 @@
         <v>1</v>
       </c>
       <c r="B189" s="58" t="s">
+        <v>582</v>
+      </c>
+      <c r="C189" s="58" t="s">
+        <v>600</v>
+      </c>
+      <c r="D189" s="58" t="s">
         <v>583</v>
-      </c>
-      <c r="C189" s="58" t="s">
-        <v>601</v>
-      </c>
-      <c r="D189" s="58" t="s">
-        <v>584</v>
       </c>
       <c r="E189" s="58" t="s">
         <v>46</v>
@@ -12059,13 +12059,13 @@
         <v>1</v>
       </c>
       <c r="B191" s="58" t="s">
+        <v>584</v>
+      </c>
+      <c r="C191" s="58" t="s">
+        <v>601</v>
+      </c>
+      <c r="D191" s="58" t="s">
         <v>585</v>
-      </c>
-      <c r="C191" s="58" t="s">
-        <v>602</v>
-      </c>
-      <c r="D191" s="58" t="s">
-        <v>586</v>
       </c>
       <c r="E191" s="58" t="s">
         <v>46</v>
@@ -12123,7 +12123,7 @@
         <v>286</v>
       </c>
       <c r="E193" s="62" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G193" s="62" t="s">
         <v>44</v>
@@ -12140,13 +12140,13 @@
         <v>1</v>
       </c>
       <c r="B194" s="58" t="s">
+        <v>587</v>
+      </c>
+      <c r="C194" s="58" t="s">
+        <v>602</v>
+      </c>
+      <c r="D194" s="58" t="s">
         <v>588</v>
-      </c>
-      <c r="C194" s="58" t="s">
-        <v>603</v>
-      </c>
-      <c r="D194" s="58" t="s">
-        <v>589</v>
       </c>
       <c r="E194" s="58" t="s">
         <v>48</v>
@@ -12202,7 +12202,7 @@
         <v>347</v>
       </c>
       <c r="C196" s="58" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D196" s="58" t="s">
         <v>348</v>
@@ -12325,7 +12325,7 @@
         <v>355</v>
       </c>
       <c r="C201" s="58" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D201" s="58" t="s">
         <v>356</v>
@@ -12403,13 +12403,13 @@
         <v>1</v>
       </c>
       <c r="B204" s="58" t="s">
+        <v>589</v>
+      </c>
+      <c r="C204" s="58" t="s">
+        <v>603</v>
+      </c>
+      <c r="D204" s="58" t="s">
         <v>590</v>
-      </c>
-      <c r="C204" s="58" t="s">
-        <v>604</v>
-      </c>
-      <c r="D204" s="58" t="s">
-        <v>591</v>
       </c>
       <c r="E204" s="58" t="s">
         <v>48</v>
@@ -12465,7 +12465,7 @@
         <v>358</v>
       </c>
       <c r="C206" s="58" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D206" s="58" t="s">
         <v>359</v>
@@ -12524,7 +12524,7 @@
         <v>360</v>
       </c>
       <c r="C208" s="58" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D208" s="58" t="s">
         <v>361</v>
@@ -12580,13 +12580,13 @@
         <v>1</v>
       </c>
       <c r="B210" s="58" t="s">
+        <v>591</v>
+      </c>
+      <c r="C210" s="58" t="s">
+        <v>604</v>
+      </c>
+      <c r="D210" s="58" t="s">
         <v>592</v>
-      </c>
-      <c r="C210" s="58" t="s">
-        <v>605</v>
-      </c>
-      <c r="D210" s="58" t="s">
-        <v>593</v>
       </c>
       <c r="E210" s="58" t="s">
         <v>46</v>
@@ -12639,13 +12639,13 @@
         <v>1</v>
       </c>
       <c r="B212" s="58" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C212" s="58" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D212" s="58" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E212" s="58" t="s">
         <v>46</v>
@@ -12701,7 +12701,7 @@
         <v>362</v>
       </c>
       <c r="C214" s="58" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D214" s="58" t="s">
         <v>363</v>
@@ -12760,7 +12760,7 @@
         <v>364</v>
       </c>
       <c r="C216" s="58" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D216" s="58" t="s">
         <v>365</v>
@@ -12847,7 +12847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
@@ -13490,13 +13490,13 @@
     </row>
     <row r="22" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F22" s="47" t="s">
         <v>43</v>
@@ -13513,13 +13513,13 @@
     </row>
     <row r="23" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>373</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>374</v>
       </c>
       <c r="F23" s="47" t="s">
         <v>43</v>
@@ -13536,13 +13536,13 @@
     </row>
     <row r="24" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F24" s="47" t="s">
         <v>43</v>
@@ -13559,13 +13559,13 @@
     </row>
     <row r="25" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F25" s="47" t="s">
         <v>43</v>
@@ -13582,13 +13582,13 @@
     </row>
     <row r="26" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F26" s="47" t="s">
         <v>43</v>
@@ -13605,13 +13605,13 @@
     </row>
     <row r="27" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F27" s="47" t="s">
         <v>43</v>
@@ -13628,13 +13628,13 @@
     </row>
     <row r="28" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>386</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>387</v>
       </c>
       <c r="F28" s="47" t="s">
         <v>43</v>
@@ -13651,13 +13651,13 @@
     </row>
     <row r="29" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>388</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>389</v>
       </c>
       <c r="F29" s="47" t="s">
         <v>43</v>
@@ -13674,13 +13674,13 @@
     </row>
     <row r="30" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>390</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>391</v>
       </c>
       <c r="F30" s="47" t="s">
         <v>43</v>
@@ -13697,13 +13697,13 @@
     </row>
     <row r="31" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F31" s="47" t="s">
         <v>43</v>
@@ -13720,13 +13720,13 @@
     </row>
     <row r="32" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F32" s="47" t="s">
         <v>43</v>
@@ -13743,13 +13743,13 @@
     </row>
     <row r="33" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F33" s="47" t="s">
         <v>43</v>
@@ -13766,13 +13766,13 @@
     </row>
     <row r="34" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>392</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>393</v>
       </c>
       <c r="F34" s="47" t="s">
         <v>43</v>
@@ -13789,13 +13789,13 @@
     </row>
     <row r="35" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="52" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B35" s="52" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F35" s="55" t="s">
         <v>43</v>
@@ -13812,13 +13812,13 @@
     </row>
     <row r="36" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="52" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B36" s="52" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D36" s="52" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F36" s="55" t="s">
         <v>43</v>
@@ -13835,13 +13835,13 @@
     </row>
     <row r="37" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="52" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B37" s="52" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D37" s="52" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F37" s="55" t="s">
         <v>43</v>
@@ -13858,13 +13858,13 @@
     </row>
     <row r="38" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="52" t="s">
+        <v>629</v>
+      </c>
+      <c r="B38" s="52" t="s">
+        <v>629</v>
+      </c>
+      <c r="D38" s="52" t="s">
         <v>630</v>
-      </c>
-      <c r="B38" s="52" t="s">
-        <v>630</v>
-      </c>
-      <c r="D38" s="52" t="s">
-        <v>631</v>
       </c>
       <c r="F38" s="55" t="s">
         <v>43</v>
@@ -13881,13 +13881,13 @@
     </row>
     <row r="39" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="52" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B39" s="52" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D39" s="52" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F39" s="55" t="s">
         <v>43</v>
@@ -13904,13 +13904,13 @@
     </row>
     <row r="40" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="52" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B40" s="52" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D40" s="52" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F40" s="55" t="s">
         <v>43</v>
@@ -13927,13 +13927,13 @@
     </row>
     <row r="41" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="52" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B41" s="52" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F41" s="55" t="s">
         <v>43</v>
@@ -13950,13 +13950,13 @@
     </row>
     <row r="42" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="52" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B42" s="52" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D42" s="52" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F42" s="55" t="s">
         <v>43</v>
@@ -13973,13 +13973,13 @@
     </row>
     <row r="43" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="52" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B43" s="52" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D43" s="52" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F43" s="55" t="s">
         <v>43</v>
@@ -13996,13 +13996,13 @@
     </row>
     <row r="44" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="52" t="s">
+        <v>394</v>
+      </c>
+      <c r="B44" s="52" t="s">
+        <v>394</v>
+      </c>
+      <c r="D44" s="52" t="s">
         <v>395</v>
-      </c>
-      <c r="B44" s="52" t="s">
-        <v>395</v>
-      </c>
-      <c r="D44" s="52" t="s">
-        <v>396</v>
       </c>
       <c r="F44" s="55" t="s">
         <v>43</v>
@@ -14019,13 +14019,13 @@
     </row>
     <row r="45" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="52" t="s">
+        <v>396</v>
+      </c>
+      <c r="B45" s="52" t="s">
+        <v>396</v>
+      </c>
+      <c r="D45" s="52" t="s">
         <v>397</v>
-      </c>
-      <c r="B45" s="52" t="s">
-        <v>397</v>
-      </c>
-      <c r="D45" s="52" t="s">
-        <v>398</v>
       </c>
       <c r="F45" s="55" t="s">
         <v>43</v>
@@ -14042,13 +14042,13 @@
     </row>
     <row r="46" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="50" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D46" s="50" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F46" s="54" t="s">
         <v>43</v>
@@ -14065,13 +14065,13 @@
     </row>
     <row r="47" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="50" t="s">
+        <v>627</v>
+      </c>
+      <c r="B47" s="50" t="s">
+        <v>627</v>
+      </c>
+      <c r="D47" s="50" t="s">
         <v>628</v>
-      </c>
-      <c r="B47" s="50" t="s">
-        <v>628</v>
-      </c>
-      <c r="D47" s="50" t="s">
-        <v>629</v>
       </c>
       <c r="F47" s="54" t="s">
         <v>43</v>
@@ -14088,13 +14088,13 @@
     </row>
     <row r="48" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="50" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D48" s="50" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F48" s="54" t="s">
         <v>43</v>
@@ -14111,13 +14111,13 @@
     </row>
     <row r="49" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="50" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B49" s="50" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D49" s="50" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F49" s="54" t="s">
         <v>43</v>
@@ -14134,13 +14134,13 @@
     </row>
     <row r="50" spans="1:9" s="50" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="50" t="s">
+        <v>398</v>
+      </c>
+      <c r="B50" s="50" t="s">
+        <v>398</v>
+      </c>
+      <c r="D50" s="50" t="s">
         <v>399</v>
-      </c>
-      <c r="B50" s="50" t="s">
-        <v>399</v>
-      </c>
-      <c r="D50" s="50" t="s">
-        <v>400</v>
       </c>
       <c r="F50" s="54" t="s">
         <v>43</v>
@@ -14157,13 +14157,13 @@
     </row>
     <row r="51" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="50" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D51" s="50" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F51" s="54" t="s">
         <v>43</v>
@@ -14180,13 +14180,13 @@
     </row>
     <row r="52" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="50" t="s">
+        <v>400</v>
+      </c>
+      <c r="B52" s="50" t="s">
+        <v>400</v>
+      </c>
+      <c r="D52" s="50" t="s">
         <v>401</v>
-      </c>
-      <c r="B52" s="50" t="s">
-        <v>401</v>
-      </c>
-      <c r="D52" s="50" t="s">
-        <v>402</v>
       </c>
       <c r="F52" s="54" t="s">
         <v>43</v>
@@ -14203,13 +14203,13 @@
     </row>
     <row r="53" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="50" t="s">
+        <v>402</v>
+      </c>
+      <c r="B53" s="50" t="s">
+        <v>402</v>
+      </c>
+      <c r="D53" s="50" t="s">
         <v>403</v>
-      </c>
-      <c r="B53" s="50" t="s">
-        <v>403</v>
-      </c>
-      <c r="D53" s="50" t="s">
-        <v>404</v>
       </c>
       <c r="F53" s="54" t="s">
         <v>43</v>
@@ -14226,13 +14226,13 @@
     </row>
     <row r="54" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="50" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D54" s="50" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F54" s="54" t="s">
         <v>43</v>
@@ -14249,13 +14249,13 @@
     </row>
     <row r="55" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="50" t="s">
+        <v>631</v>
+      </c>
+      <c r="B55" s="50" t="s">
+        <v>631</v>
+      </c>
+      <c r="D55" s="50" t="s">
         <v>632</v>
-      </c>
-      <c r="B55" s="50" t="s">
-        <v>632</v>
-      </c>
-      <c r="D55" s="50" t="s">
-        <v>633</v>
       </c>
       <c r="F55" s="54" t="s">
         <v>43</v>
@@ -14272,13 +14272,13 @@
     </row>
     <row r="56" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="50" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B56" s="50" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D56" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F56" s="54" t="s">
         <v>43</v>
@@ -14295,13 +14295,13 @@
     </row>
     <row r="57" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="50" t="s">
+        <v>410</v>
+      </c>
+      <c r="B57" s="50" t="s">
+        <v>410</v>
+      </c>
+      <c r="D57" s="50" t="s">
         <v>411</v>
-      </c>
-      <c r="B57" s="50" t="s">
-        <v>411</v>
-      </c>
-      <c r="D57" s="50" t="s">
-        <v>412</v>
       </c>
       <c r="F57" s="54" t="s">
         <v>43</v>
@@ -14318,13 +14318,13 @@
     </row>
     <row r="58" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="50" t="s">
+        <v>412</v>
+      </c>
+      <c r="B58" s="50" t="s">
+        <v>412</v>
+      </c>
+      <c r="D58" s="50" t="s">
         <v>413</v>
-      </c>
-      <c r="B58" s="50" t="s">
-        <v>413</v>
-      </c>
-      <c r="D58" s="50" t="s">
-        <v>414</v>
       </c>
       <c r="F58" s="54" t="s">
         <v>43</v>
@@ -14341,13 +14341,13 @@
     </row>
     <row r="59" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="50" t="s">
+        <v>414</v>
+      </c>
+      <c r="B59" s="50" t="s">
+        <v>414</v>
+      </c>
+      <c r="D59" s="50" t="s">
         <v>415</v>
-      </c>
-      <c r="B59" s="50" t="s">
-        <v>415</v>
-      </c>
-      <c r="D59" s="50" t="s">
-        <v>416</v>
       </c>
       <c r="F59" s="54" t="s">
         <v>43</v>
@@ -14364,13 +14364,13 @@
     </row>
     <row r="60" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="50" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B60" s="50" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D60" s="50" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F60" s="54" t="s">
         <v>43</v>
@@ -14387,13 +14387,13 @@
     </row>
     <row r="61" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="50" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D61" s="50" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F61" s="54" t="s">
         <v>43</v>
@@ -14410,13 +14410,13 @@
     </row>
     <row r="62" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="58" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B62" s="58" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D62" s="58" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F62" s="60" t="s">
         <v>43</v>
@@ -14433,13 +14433,13 @@
     </row>
     <row r="63" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="58" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B63" s="58" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D63" s="58" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F63" s="60" t="s">
         <v>43</v>
@@ -14456,13 +14456,13 @@
     </row>
     <row r="64" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="58" t="s">
+        <v>416</v>
+      </c>
+      <c r="B64" s="58" t="s">
+        <v>416</v>
+      </c>
+      <c r="D64" s="58" t="s">
         <v>417</v>
-      </c>
-      <c r="B64" s="58" t="s">
-        <v>417</v>
-      </c>
-      <c r="D64" s="58" t="s">
-        <v>418</v>
       </c>
       <c r="F64" s="60" t="s">
         <v>43</v>
@@ -14479,13 +14479,13 @@
     </row>
     <row r="65" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="58" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B65" s="58" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D65" s="58" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F65" s="60" t="s">
         <v>43</v>
@@ -14502,13 +14502,13 @@
     </row>
     <row r="66" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="58" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B66" s="58" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D66" s="58" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F66" s="60" t="s">
         <v>43</v>
@@ -14525,13 +14525,13 @@
     </row>
     <row r="67" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="58" t="s">
+        <v>419</v>
+      </c>
+      <c r="B67" s="58" t="s">
+        <v>419</v>
+      </c>
+      <c r="D67" s="58" t="s">
         <v>420</v>
-      </c>
-      <c r="B67" s="58" t="s">
-        <v>420</v>
-      </c>
-      <c r="D67" s="58" t="s">
-        <v>421</v>
       </c>
       <c r="F67" s="60" t="s">
         <v>43</v>
@@ -14548,13 +14548,13 @@
     </row>
     <row r="68" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="58" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B68" s="58" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D68" s="58" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F68" s="60" t="s">
         <v>43</v>
@@ -14571,13 +14571,13 @@
     </row>
     <row r="69" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="58" t="s">
+        <v>428</v>
+      </c>
+      <c r="B69" s="58" t="s">
+        <v>428</v>
+      </c>
+      <c r="D69" s="58" t="s">
         <v>429</v>
-      </c>
-      <c r="B69" s="58" t="s">
-        <v>429</v>
-      </c>
-      <c r="D69" s="58" t="s">
-        <v>430</v>
       </c>
       <c r="F69" s="60" t="s">
         <v>43</v>
@@ -14594,13 +14594,13 @@
     </row>
     <row r="70" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="58" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B70" s="58" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D70" s="58" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F70" s="60" t="s">
         <v>43</v>
@@ -14617,13 +14617,13 @@
     </row>
     <row r="71" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="58" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B71" s="58" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D71" s="58" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F71" s="60" t="s">
         <v>43</v>
@@ -14640,13 +14640,13 @@
     </row>
     <row r="72" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="58" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B72" s="58" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D72" s="58" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F72" s="60" t="s">
         <v>43</v>
@@ -14663,13 +14663,13 @@
     </row>
     <row r="73" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="58" t="s">
+        <v>633</v>
+      </c>
+      <c r="B73" s="58" t="s">
+        <v>633</v>
+      </c>
+      <c r="D73" s="58" t="s">
         <v>634</v>
-      </c>
-      <c r="B73" s="58" t="s">
-        <v>634</v>
-      </c>
-      <c r="D73" s="58" t="s">
-        <v>635</v>
       </c>
       <c r="F73" s="60" t="s">
         <v>43</v>
@@ -14686,13 +14686,13 @@
     </row>
     <row r="74" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="58" t="s">
+        <v>430</v>
+      </c>
+      <c r="B74" s="58" t="s">
+        <v>430</v>
+      </c>
+      <c r="D74" s="58" t="s">
         <v>431</v>
-      </c>
-      <c r="B74" s="58" t="s">
-        <v>431</v>
-      </c>
-      <c r="D74" s="58" t="s">
-        <v>432</v>
       </c>
       <c r="F74" s="60" t="s">
         <v>43</v>
@@ -14709,13 +14709,13 @@
     </row>
     <row r="75" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="58" t="s">
+        <v>432</v>
+      </c>
+      <c r="B75" s="58" t="s">
+        <v>432</v>
+      </c>
+      <c r="D75" s="58" t="s">
         <v>433</v>
-      </c>
-      <c r="B75" s="58" t="s">
-        <v>433</v>
-      </c>
-      <c r="D75" s="58" t="s">
-        <v>434</v>
       </c>
       <c r="F75" s="60" t="s">
         <v>43</v>
@@ -14732,13 +14732,13 @@
     </row>
     <row r="76" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="58" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B76" s="58" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D76" s="58" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F76" s="60" t="s">
         <v>43</v>
@@ -14755,13 +14755,13 @@
     </row>
     <row r="77" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="58" t="s">
+        <v>434</v>
+      </c>
+      <c r="B77" s="58" t="s">
+        <v>434</v>
+      </c>
+      <c r="D77" s="58" t="s">
         <v>435</v>
-      </c>
-      <c r="B77" s="58" t="s">
-        <v>435</v>
-      </c>
-      <c r="D77" s="58" t="s">
-        <v>436</v>
       </c>
       <c r="F77" s="60" t="s">
         <v>43</v>
@@ -14778,13 +14778,13 @@
     </row>
     <row r="78" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="58" t="s">
+        <v>436</v>
+      </c>
+      <c r="B78" s="58" t="s">
+        <v>436</v>
+      </c>
+      <c r="D78" s="58" t="s">
         <v>437</v>
-      </c>
-      <c r="B78" s="58" t="s">
-        <v>437</v>
-      </c>
-      <c r="D78" s="58" t="s">
-        <v>438</v>
       </c>
       <c r="F78" s="60" t="s">
         <v>43</v>
@@ -14801,13 +14801,13 @@
     </row>
     <row r="79" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="58" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B79" s="58" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D79" s="58" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F79" s="60" t="s">
         <v>43</v>
@@ -14824,13 +14824,13 @@
     </row>
     <row r="80" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="58" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B80" s="58" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D80" s="58" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F80" s="60" t="s">
         <v>43</v>
@@ -14847,13 +14847,13 @@
     </row>
     <row r="81" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="58" t="s">
+        <v>438</v>
+      </c>
+      <c r="B81" s="58" t="s">
+        <v>438</v>
+      </c>
+      <c r="D81" s="58" t="s">
         <v>439</v>
-      </c>
-      <c r="B81" s="58" t="s">
-        <v>439</v>
-      </c>
-      <c r="D81" s="58" t="s">
-        <v>440</v>
       </c>
       <c r="F81" s="60" t="s">
         <v>43</v>
@@ -14870,13 +14870,13 @@
     </row>
     <row r="82" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="58" t="s">
+        <v>440</v>
+      </c>
+      <c r="B82" s="58" t="s">
+        <v>440</v>
+      </c>
+      <c r="D82" s="58" t="s">
         <v>441</v>
-      </c>
-      <c r="B82" s="58" t="s">
-        <v>441</v>
-      </c>
-      <c r="D82" s="58" t="s">
-        <v>442</v>
       </c>
       <c r="F82" s="60" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Updates the server version being used
</commit_message>
<xml_diff>
--- a/projects/PTool_Full_Analysis.xlsx
+++ b/projects/PTool_Full_Analysis.xlsx
@@ -30,7 +30,7 @@
     <definedName name="TrueFalse">Lookups!$C$12:$C$13</definedName>
     <definedName name="Workflow">Lookups!$E$12:$E$13</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -817,9 +817,6 @@
     <t>../../OpenStudio-PTool/weather/*</t>
   </si>
   <si>
-    <t>../../openstudio-standards/measures</t>
-  </si>
-  <si>
     <t>standard_report_legacy.heating_electricity</t>
   </si>
   <si>
@@ -1948,7 +1945,10 @@
     <t>commercial_lighting_to_et2020_leds.applicable</t>
   </si>
   <si>
-    <t>1.15.18</t>
+    <t>1.21.14</t>
+  </si>
+  <si>
+    <t>../../OpenStudio-Measures/NREL Working Measures</t>
   </si>
 </sst>
 </file>
@@ -6682,8 +6682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6730,7 +6730,7 @@
         <v>81</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>82</v>
@@ -6741,7 +6741,7 @@
         <v>92</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>175</v>
@@ -6752,7 +6752,7 @@
         <v>93</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>95</v>
@@ -6801,7 +6801,7 @@
         <v>83</v>
       </c>
       <c r="B9" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="30"/>
@@ -6823,7 +6823,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>94</v>
@@ -6834,7 +6834,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>260</v>
+        <v>637</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="29" t="s">
@@ -7041,7 +7041,7 @@
         <v>195</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>229</v>
@@ -7095,7 +7095,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7220,7 +7220,7 @@
         <v>8</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="P3" s="16" t="s">
         <v>98</v>
@@ -7289,10 +7289,10 @@
         <v>252</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="P5" s="29" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="R5" s="29" t="s">
         <v>251</v>
@@ -7306,7 +7306,7 @@
         <v>243</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G6" s="29" t="s">
         <v>240</v>
@@ -7330,7 +7330,7 @@
         <v>242</v>
       </c>
       <c r="P6" s="29" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R6" s="29" t="s">
         <v>251</v>
@@ -7368,7 +7368,7 @@
         <v>247</v>
       </c>
       <c r="P7" s="43" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="R7" s="29" t="s">
         <v>251</v>
@@ -7379,13 +7379,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>46</v>
@@ -7438,13 +7438,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>300</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>301</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>46</v>
@@ -7519,7 +7519,7 @@
       </c>
       <c r="C13" s="55"/>
       <c r="D13" s="55" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E13" s="55" t="s">
         <v>50</v>
@@ -7539,7 +7539,7 @@
       </c>
       <c r="C14" s="55"/>
       <c r="D14" s="55" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E14" s="55" t="s">
         <v>51</v>
@@ -7548,7 +7548,7 @@
         <v>44</v>
       </c>
       <c r="H14" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I14" s="55">
         <v>18</v>
@@ -7561,7 +7561,7 @@
       </c>
       <c r="C15" s="55"/>
       <c r="D15" s="55" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E15" s="55" t="s">
         <v>52</v>
@@ -7570,7 +7570,7 @@
         <v>44</v>
       </c>
       <c r="H15" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I15" s="55">
         <v>9</v>
@@ -7583,7 +7583,7 @@
       </c>
       <c r="C16" s="55"/>
       <c r="D16" s="55" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E16" s="55" t="s">
         <v>53</v>
@@ -7603,7 +7603,7 @@
       </c>
       <c r="C17" s="55"/>
       <c r="D17" s="55" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E17" s="55" t="s">
         <v>54</v>
@@ -7612,7 +7612,7 @@
         <v>44</v>
       </c>
       <c r="H17" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I17" s="55">
         <v>18</v>
@@ -7625,7 +7625,7 @@
       </c>
       <c r="C18" s="55"/>
       <c r="D18" s="55" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E18" s="55" t="s">
         <v>55</v>
@@ -7634,7 +7634,7 @@
         <v>44</v>
       </c>
       <c r="H18" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I18" s="55">
         <v>9</v>
@@ -7647,7 +7647,7 @@
       </c>
       <c r="C19" s="55"/>
       <c r="D19" s="55" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E19" s="55" t="s">
         <v>56</v>
@@ -7667,7 +7667,7 @@
       </c>
       <c r="C20" s="55"/>
       <c r="D20" s="55" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E20" s="55" t="s">
         <v>57</v>
@@ -7676,7 +7676,7 @@
         <v>44</v>
       </c>
       <c r="H20" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I20" s="55">
         <v>18</v>
@@ -7689,7 +7689,7 @@
       </c>
       <c r="C21" s="55"/>
       <c r="D21" s="55" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E21" s="55" t="s">
         <v>58</v>
@@ -7698,7 +7698,7 @@
         <v>44</v>
       </c>
       <c r="H21" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I21" s="55">
         <v>9</v>
@@ -7709,13 +7709,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>48</v>
@@ -7768,13 +7768,13 @@
         <v>1</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>442</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>443</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>46</v>
@@ -7829,16 +7829,16 @@
       </c>
       <c r="C26" s="55"/>
       <c r="D26" s="55" t="s">
+        <v>443</v>
+      </c>
+      <c r="E26" s="55" t="s">
         <v>444</v>
-      </c>
-      <c r="E26" s="55" t="s">
-        <v>445</v>
       </c>
       <c r="G26" s="55" t="s">
         <v>44</v>
       </c>
       <c r="H26" s="55" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I26" s="55">
         <v>10</v>
@@ -7851,10 +7851,10 @@
       </c>
       <c r="C27" s="55"/>
       <c r="D27" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="E27" s="55" t="s">
         <v>446</v>
-      </c>
-      <c r="E27" s="55" t="s">
-        <v>447</v>
       </c>
       <c r="G27" s="55" t="s">
         <v>44</v>
@@ -7871,10 +7871,10 @@
       </c>
       <c r="C28" s="55"/>
       <c r="D28" s="55" t="s">
+        <v>447</v>
+      </c>
+      <c r="E28" s="55" t="s">
         <v>448</v>
-      </c>
-      <c r="E28" s="55" t="s">
-        <v>449</v>
       </c>
       <c r="G28" s="55" t="s">
         <v>44</v>
@@ -7889,13 +7889,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>46</v>
@@ -7950,16 +7950,16 @@
       </c>
       <c r="C31" s="55"/>
       <c r="D31" s="55" t="s">
+        <v>302</v>
+      </c>
+      <c r="E31" s="55" t="s">
         <v>303</v>
-      </c>
-      <c r="E31" s="55" t="s">
-        <v>304</v>
       </c>
       <c r="G31" s="55" t="s">
         <v>44</v>
       </c>
       <c r="H31" s="55" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I31" s="55">
         <v>2</v>
@@ -7970,13 +7970,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>450</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>459</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>451</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>46</v>
@@ -8029,13 +8029,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>306</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>46</v>
@@ -8088,13 +8088,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>307</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>308</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>46</v>
@@ -8147,13 +8147,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>310</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>46</v>
@@ -8206,13 +8206,13 @@
         <v>1</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>46</v>
@@ -8265,13 +8265,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>46</v>
@@ -8324,13 +8324,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>454</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>455</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>48</v>
@@ -8383,13 +8383,13 @@
         <v>1</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>311</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>312</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>46</v>
@@ -8464,7 +8464,7 @@
       </c>
       <c r="C49" s="55"/>
       <c r="D49" s="55" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E49" s="55" t="s">
         <v>50</v>
@@ -8484,7 +8484,7 @@
       </c>
       <c r="C50" s="55"/>
       <c r="D50" s="55" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E50" s="55" t="s">
         <v>51</v>
@@ -8493,7 +8493,7 @@
         <v>44</v>
       </c>
       <c r="H50" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I50" s="55">
         <v>18</v>
@@ -8506,7 +8506,7 @@
       </c>
       <c r="C51" s="55"/>
       <c r="D51" s="55" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E51" s="55" t="s">
         <v>52</v>
@@ -8515,7 +8515,7 @@
         <v>44</v>
       </c>
       <c r="H51" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I51" s="55">
         <v>9</v>
@@ -8528,7 +8528,7 @@
       </c>
       <c r="C52" s="55"/>
       <c r="D52" s="55" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E52" s="55" t="s">
         <v>53</v>
@@ -8548,7 +8548,7 @@
       </c>
       <c r="C53" s="55"/>
       <c r="D53" s="55" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E53" s="55" t="s">
         <v>54</v>
@@ -8557,7 +8557,7 @@
         <v>44</v>
       </c>
       <c r="H53" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I53" s="55">
         <v>18</v>
@@ -8570,7 +8570,7 @@
       </c>
       <c r="C54" s="55"/>
       <c r="D54" s="55" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E54" s="55" t="s">
         <v>55</v>
@@ -8579,7 +8579,7 @@
         <v>44</v>
       </c>
       <c r="H54" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I54" s="55">
         <v>9</v>
@@ -8592,7 +8592,7 @@
       </c>
       <c r="C55" s="55"/>
       <c r="D55" s="55" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E55" s="55" t="s">
         <v>56</v>
@@ -8612,7 +8612,7 @@
       </c>
       <c r="C56" s="55"/>
       <c r="D56" s="55" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E56" s="55" t="s">
         <v>57</v>
@@ -8621,7 +8621,7 @@
         <v>44</v>
       </c>
       <c r="H56" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I56" s="55">
         <v>18</v>
@@ -8634,7 +8634,7 @@
       </c>
       <c r="C57" s="55"/>
       <c r="D57" s="55" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E57" s="55" t="s">
         <v>58</v>
@@ -8643,7 +8643,7 @@
         <v>44</v>
       </c>
       <c r="H57" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I57" s="55">
         <v>9</v>
@@ -8654,13 +8654,13 @@
         <v>1</v>
       </c>
       <c r="B58" s="51" t="s">
+        <v>481</v>
+      </c>
+      <c r="C58" s="51" t="s">
+        <v>500</v>
+      </c>
+      <c r="D58" s="51" t="s">
         <v>482</v>
-      </c>
-      <c r="C58" s="51" t="s">
-        <v>501</v>
-      </c>
-      <c r="D58" s="51" t="s">
-        <v>483</v>
       </c>
       <c r="E58" s="51" t="s">
         <v>46</v>
@@ -8715,10 +8715,10 @@
       </c>
       <c r="C60" s="58"/>
       <c r="D60" s="58" t="s">
+        <v>483</v>
+      </c>
+      <c r="E60" s="58" t="s">
         <v>484</v>
-      </c>
-      <c r="E60" s="58" t="s">
-        <v>485</v>
       </c>
       <c r="G60" s="58" t="s">
         <v>44</v>
@@ -8735,10 +8735,10 @@
       </c>
       <c r="C61" s="58"/>
       <c r="D61" s="58" t="s">
+        <v>485</v>
+      </c>
+      <c r="E61" s="58" t="s">
         <v>486</v>
-      </c>
-      <c r="E61" s="58" t="s">
-        <v>487</v>
       </c>
       <c r="G61" s="58" t="s">
         <v>44</v>
@@ -8755,10 +8755,10 @@
       </c>
       <c r="C62" s="58"/>
       <c r="D62" s="58" t="s">
+        <v>487</v>
+      </c>
+      <c r="E62" s="58" t="s">
         <v>488</v>
-      </c>
-      <c r="E62" s="58" t="s">
-        <v>489</v>
       </c>
       <c r="G62" s="58" t="s">
         <v>44</v>
@@ -8773,13 +8773,13 @@
         <v>1</v>
       </c>
       <c r="B63" s="51" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C63" s="51" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D63" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E63" s="51" t="s">
         <v>46</v>
@@ -8832,13 +8832,13 @@
         <v>1</v>
       </c>
       <c r="B65" s="51" t="s">
+        <v>489</v>
+      </c>
+      <c r="C65" s="51" t="s">
+        <v>501</v>
+      </c>
+      <c r="D65" s="51" t="s">
         <v>490</v>
-      </c>
-      <c r="C65" s="51" t="s">
-        <v>502</v>
-      </c>
-      <c r="D65" s="51" t="s">
-        <v>491</v>
       </c>
       <c r="E65" s="51" t="s">
         <v>46</v>
@@ -8891,13 +8891,13 @@
         <v>1</v>
       </c>
       <c r="B67" s="51" t="s">
+        <v>491</v>
+      </c>
+      <c r="C67" s="51" t="s">
+        <v>502</v>
+      </c>
+      <c r="D67" s="51" t="s">
         <v>492</v>
-      </c>
-      <c r="C67" s="51" t="s">
-        <v>503</v>
-      </c>
-      <c r="D67" s="51" t="s">
-        <v>493</v>
       </c>
       <c r="E67" s="51" t="s">
         <v>46</v>
@@ -8950,13 +8950,13 @@
         <v>1</v>
       </c>
       <c r="B69" s="51" t="s">
+        <v>493</v>
+      </c>
+      <c r="C69" s="51" t="s">
+        <v>503</v>
+      </c>
+      <c r="D69" s="51" t="s">
         <v>494</v>
-      </c>
-      <c r="C69" s="51" t="s">
-        <v>504</v>
-      </c>
-      <c r="D69" s="51" t="s">
-        <v>495</v>
       </c>
       <c r="E69" s="51" t="s">
         <v>46</v>
@@ -9009,13 +9009,13 @@
         <v>1</v>
       </c>
       <c r="B71" s="51" t="s">
+        <v>495</v>
+      </c>
+      <c r="C71" s="51" t="s">
+        <v>504</v>
+      </c>
+      <c r="D71" s="51" t="s">
         <v>496</v>
-      </c>
-      <c r="C71" s="51" t="s">
-        <v>505</v>
-      </c>
-      <c r="D71" s="51" t="s">
-        <v>497</v>
       </c>
       <c r="E71" s="51" t="s">
         <v>46</v>
@@ -9068,13 +9068,13 @@
         <v>1</v>
       </c>
       <c r="B73" s="51" t="s">
+        <v>497</v>
+      </c>
+      <c r="C73" s="51" t="s">
+        <v>505</v>
+      </c>
+      <c r="D73" s="51" t="s">
         <v>498</v>
-      </c>
-      <c r="C73" s="51" t="s">
-        <v>506</v>
-      </c>
-      <c r="D73" s="51" t="s">
-        <v>499</v>
       </c>
       <c r="E73" s="51" t="s">
         <v>46</v>
@@ -9127,13 +9127,13 @@
         <v>1</v>
       </c>
       <c r="B75" s="51" t="s">
+        <v>506</v>
+      </c>
+      <c r="C75" s="51" t="s">
         <v>507</v>
       </c>
-      <c r="C75" s="51" t="s">
-        <v>508</v>
-      </c>
       <c r="D75" s="51" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E75" s="51" t="s">
         <v>46</v>
@@ -9186,13 +9186,13 @@
         <v>1</v>
       </c>
       <c r="B77" s="51" t="s">
+        <v>313</v>
+      </c>
+      <c r="C77" s="51" t="s">
+        <v>376</v>
+      </c>
+      <c r="D77" s="51" t="s">
         <v>314</v>
-      </c>
-      <c r="C77" s="51" t="s">
-        <v>377</v>
-      </c>
-      <c r="D77" s="51" t="s">
-        <v>315</v>
       </c>
       <c r="E77" s="51" t="s">
         <v>46</v>
@@ -9267,7 +9267,7 @@
       </c>
       <c r="C80" s="58"/>
       <c r="D80" s="58" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E80" s="58" t="s">
         <v>50</v>
@@ -9287,7 +9287,7 @@
       </c>
       <c r="C81" s="58"/>
       <c r="D81" s="58" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E81" s="58" t="s">
         <v>51</v>
@@ -9296,7 +9296,7 @@
         <v>44</v>
       </c>
       <c r="H81" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I81" s="58">
         <v>18</v>
@@ -9309,7 +9309,7 @@
       </c>
       <c r="C82" s="58"/>
       <c r="D82" s="58" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E82" s="58" t="s">
         <v>52</v>
@@ -9318,7 +9318,7 @@
         <v>44</v>
       </c>
       <c r="H82" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I82" s="58">
         <v>9</v>
@@ -9331,7 +9331,7 @@
       </c>
       <c r="C83" s="58"/>
       <c r="D83" s="58" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E83" s="58" t="s">
         <v>53</v>
@@ -9351,7 +9351,7 @@
       </c>
       <c r="C84" s="58"/>
       <c r="D84" s="58" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E84" s="58" t="s">
         <v>54</v>
@@ -9360,7 +9360,7 @@
         <v>44</v>
       </c>
       <c r="H84" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I84" s="58">
         <v>18</v>
@@ -9373,7 +9373,7 @@
       </c>
       <c r="C85" s="58"/>
       <c r="D85" s="58" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E85" s="58" t="s">
         <v>55</v>
@@ -9382,7 +9382,7 @@
         <v>44</v>
       </c>
       <c r="H85" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I85" s="58">
         <v>9</v>
@@ -9395,7 +9395,7 @@
       </c>
       <c r="C86" s="58"/>
       <c r="D86" s="58" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E86" s="58" t="s">
         <v>56</v>
@@ -9415,7 +9415,7 @@
       </c>
       <c r="C87" s="58"/>
       <c r="D87" s="58" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E87" s="58" t="s">
         <v>57</v>
@@ -9424,7 +9424,7 @@
         <v>44</v>
       </c>
       <c r="H87" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I87" s="58">
         <v>18</v>
@@ -9437,7 +9437,7 @@
       </c>
       <c r="C88" s="58"/>
       <c r="D88" s="58" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E88" s="58" t="s">
         <v>58</v>
@@ -9446,7 +9446,7 @@
         <v>44</v>
       </c>
       <c r="H88" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I88" s="58">
         <v>9</v>
@@ -9457,13 +9457,13 @@
         <v>1</v>
       </c>
       <c r="B89" s="51" t="s">
+        <v>315</v>
+      </c>
+      <c r="C89" s="51" t="s">
+        <v>377</v>
+      </c>
+      <c r="D89" s="51" t="s">
         <v>316</v>
-      </c>
-      <c r="C89" s="51" t="s">
-        <v>378</v>
-      </c>
-      <c r="D89" s="51" t="s">
-        <v>317</v>
       </c>
       <c r="E89" s="51" t="s">
         <v>46</v>
@@ -9538,7 +9538,7 @@
       </c>
       <c r="C92" s="58"/>
       <c r="D92" s="58" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E92" s="58" t="s">
         <v>50</v>
@@ -9558,7 +9558,7 @@
       </c>
       <c r="C93" s="58"/>
       <c r="D93" s="58" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E93" s="58" t="s">
         <v>51</v>
@@ -9567,7 +9567,7 @@
         <v>44</v>
       </c>
       <c r="H93" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I93" s="58">
         <v>18</v>
@@ -9580,7 +9580,7 @@
       </c>
       <c r="C94" s="58"/>
       <c r="D94" s="58" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E94" s="58" t="s">
         <v>52</v>
@@ -9589,7 +9589,7 @@
         <v>44</v>
       </c>
       <c r="H94" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I94" s="58">
         <v>9</v>
@@ -9602,7 +9602,7 @@
       </c>
       <c r="C95" s="58"/>
       <c r="D95" s="58" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E95" s="58" t="s">
         <v>53</v>
@@ -9622,7 +9622,7 @@
       </c>
       <c r="C96" s="58"/>
       <c r="D96" s="58" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E96" s="58" t="s">
         <v>54</v>
@@ -9631,7 +9631,7 @@
         <v>44</v>
       </c>
       <c r="H96" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I96" s="58">
         <v>18</v>
@@ -9644,7 +9644,7 @@
       </c>
       <c r="C97" s="58"/>
       <c r="D97" s="58" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E97" s="58" t="s">
         <v>55</v>
@@ -9653,7 +9653,7 @@
         <v>44</v>
       </c>
       <c r="H97" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I97" s="58">
         <v>9</v>
@@ -9666,7 +9666,7 @@
       </c>
       <c r="C98" s="58"/>
       <c r="D98" s="58" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E98" s="58" t="s">
         <v>56</v>
@@ -9686,7 +9686,7 @@
       </c>
       <c r="C99" s="58"/>
       <c r="D99" s="58" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E99" s="58" t="s">
         <v>57</v>
@@ -9695,7 +9695,7 @@
         <v>44</v>
       </c>
       <c r="H99" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I99" s="58">
         <v>18</v>
@@ -9708,7 +9708,7 @@
       </c>
       <c r="C100" s="58"/>
       <c r="D100" s="58" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E100" s="58" t="s">
         <v>58</v>
@@ -9717,7 +9717,7 @@
         <v>44</v>
       </c>
       <c r="H100" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I100" s="58">
         <v>9</v>
@@ -9728,13 +9728,13 @@
         <v>1</v>
       </c>
       <c r="B101" s="49" t="s">
+        <v>523</v>
+      </c>
+      <c r="C101" s="49" t="s">
+        <v>539</v>
+      </c>
+      <c r="D101" s="49" t="s">
         <v>524</v>
-      </c>
-      <c r="C101" s="49" t="s">
-        <v>540</v>
-      </c>
-      <c r="D101" s="49" t="s">
-        <v>525</v>
       </c>
       <c r="E101" s="49" t="s">
         <v>46</v>
@@ -9787,13 +9787,13 @@
         <v>1</v>
       </c>
       <c r="B103" s="49" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C103" s="49" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D103" s="49" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E103" s="49" t="s">
         <v>46</v>
@@ -9848,16 +9848,16 @@
       </c>
       <c r="C105" s="60"/>
       <c r="D105" s="60" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E105" s="60" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G105" s="60" t="s">
         <v>44</v>
       </c>
       <c r="H105" s="60" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I105" s="60">
         <v>30</v>
@@ -9868,13 +9868,13 @@
         <v>1</v>
       </c>
       <c r="B106" s="49" t="s">
+        <v>526</v>
+      </c>
+      <c r="C106" s="49" t="s">
+        <v>542</v>
+      </c>
+      <c r="D106" s="49" t="s">
         <v>527</v>
-      </c>
-      <c r="C106" s="49" t="s">
-        <v>543</v>
-      </c>
-      <c r="D106" s="49" t="s">
-        <v>528</v>
       </c>
       <c r="E106" s="49" t="s">
         <v>48</v>
@@ -9927,13 +9927,13 @@
         <v>1</v>
       </c>
       <c r="B108" s="49" t="s">
+        <v>317</v>
+      </c>
+      <c r="C108" s="49" t="s">
+        <v>378</v>
+      </c>
+      <c r="D108" s="49" t="s">
         <v>318</v>
-      </c>
-      <c r="C108" s="49" t="s">
-        <v>379</v>
-      </c>
-      <c r="D108" s="49" t="s">
-        <v>319</v>
       </c>
       <c r="E108" s="49" t="s">
         <v>46</v>
@@ -9986,13 +9986,13 @@
         <v>1</v>
       </c>
       <c r="B110" s="49" t="s">
+        <v>528</v>
+      </c>
+      <c r="C110" s="49" t="s">
+        <v>543</v>
+      </c>
+      <c r="D110" s="49" t="s">
         <v>529</v>
-      </c>
-      <c r="C110" s="49" t="s">
-        <v>544</v>
-      </c>
-      <c r="D110" s="49" t="s">
-        <v>530</v>
       </c>
       <c r="E110" s="49" t="s">
         <v>46</v>
@@ -10047,16 +10047,16 @@
       </c>
       <c r="C112" s="60"/>
       <c r="D112" s="60" t="s">
+        <v>296</v>
+      </c>
+      <c r="E112" s="60" t="s">
         <v>297</v>
-      </c>
-      <c r="E112" s="60" t="s">
-        <v>298</v>
       </c>
       <c r="G112" s="60" t="s">
         <v>44</v>
       </c>
       <c r="H112" s="60" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I112" s="60">
         <v>1</v>
@@ -10069,10 +10069,10 @@
       </c>
       <c r="C113" s="60"/>
       <c r="D113" s="60" t="s">
+        <v>266</v>
+      </c>
+      <c r="E113" s="60" t="s">
         <v>267</v>
-      </c>
-      <c r="E113" s="60" t="s">
-        <v>268</v>
       </c>
       <c r="G113" s="60" t="s">
         <v>44</v>
@@ -10089,10 +10089,10 @@
       </c>
       <c r="C114" s="60"/>
       <c r="D114" s="60" t="s">
+        <v>268</v>
+      </c>
+      <c r="E114" s="60" t="s">
         <v>269</v>
-      </c>
-      <c r="E114" s="60" t="s">
-        <v>270</v>
       </c>
       <c r="G114" s="60" t="s">
         <v>44</v>
@@ -10109,10 +10109,10 @@
       </c>
       <c r="C115" s="60"/>
       <c r="D115" s="60" t="s">
+        <v>270</v>
+      </c>
+      <c r="E115" s="60" t="s">
         <v>271</v>
-      </c>
-      <c r="E115" s="60" t="s">
-        <v>272</v>
       </c>
       <c r="G115" s="60" t="s">
         <v>44</v>
@@ -10129,10 +10129,10 @@
       </c>
       <c r="C116" s="60"/>
       <c r="D116" s="60" t="s">
+        <v>272</v>
+      </c>
+      <c r="E116" s="60" t="s">
         <v>273</v>
-      </c>
-      <c r="E116" s="60" t="s">
-        <v>274</v>
       </c>
       <c r="G116" s="60" t="s">
         <v>44</v>
@@ -10149,10 +10149,10 @@
       </c>
       <c r="C117" s="60"/>
       <c r="D117" s="60" t="s">
+        <v>274</v>
+      </c>
+      <c r="E117" s="60" t="s">
         <v>275</v>
-      </c>
-      <c r="E117" s="60" t="s">
-        <v>276</v>
       </c>
       <c r="G117" s="60" t="s">
         <v>44</v>
@@ -10169,10 +10169,10 @@
       </c>
       <c r="C118" s="60"/>
       <c r="D118" s="60" t="s">
+        <v>276</v>
+      </c>
+      <c r="E118" s="60" t="s">
         <v>277</v>
-      </c>
-      <c r="E118" s="60" t="s">
-        <v>278</v>
       </c>
       <c r="G118" s="60" t="s">
         <v>44</v>
@@ -10189,10 +10189,10 @@
       </c>
       <c r="C119" s="60"/>
       <c r="D119" s="60" t="s">
+        <v>278</v>
+      </c>
+      <c r="E119" s="60" t="s">
         <v>279</v>
-      </c>
-      <c r="E119" s="60" t="s">
-        <v>280</v>
       </c>
       <c r="G119" s="60" t="s">
         <v>44</v>
@@ -10209,10 +10209,10 @@
       </c>
       <c r="C120" s="60"/>
       <c r="D120" s="60" t="s">
+        <v>280</v>
+      </c>
+      <c r="E120" s="60" t="s">
         <v>281</v>
-      </c>
-      <c r="E120" s="60" t="s">
-        <v>282</v>
       </c>
       <c r="G120" s="60" t="s">
         <v>44</v>
@@ -10227,13 +10227,13 @@
         <v>1</v>
       </c>
       <c r="B121" s="49" t="s">
+        <v>319</v>
+      </c>
+      <c r="C121" s="49" t="s">
+        <v>379</v>
+      </c>
+      <c r="D121" s="49" t="s">
         <v>320</v>
-      </c>
-      <c r="C121" s="49" t="s">
-        <v>380</v>
-      </c>
-      <c r="D121" s="49" t="s">
-        <v>321</v>
       </c>
       <c r="E121" s="49" t="s">
         <v>46</v>
@@ -10286,13 +10286,13 @@
         <v>1</v>
       </c>
       <c r="B123" s="49" t="s">
+        <v>321</v>
+      </c>
+      <c r="C123" s="49" t="s">
+        <v>380</v>
+      </c>
+      <c r="D123" s="49" t="s">
         <v>322</v>
-      </c>
-      <c r="C123" s="49" t="s">
-        <v>381</v>
-      </c>
-      <c r="D123" s="49" t="s">
-        <v>323</v>
       </c>
       <c r="E123" s="49" t="s">
         <v>46</v>
@@ -10345,13 +10345,13 @@
         <v>1</v>
       </c>
       <c r="B125" s="49" t="s">
+        <v>530</v>
+      </c>
+      <c r="C125" s="49" t="s">
+        <v>544</v>
+      </c>
+      <c r="D125" s="49" t="s">
         <v>531</v>
-      </c>
-      <c r="C125" s="49" t="s">
-        <v>545</v>
-      </c>
-      <c r="D125" s="49" t="s">
-        <v>532</v>
       </c>
       <c r="E125" s="49" t="s">
         <v>48</v>
@@ -10404,13 +10404,13 @@
         <v>1</v>
       </c>
       <c r="B127" s="49" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C127" s="49" t="s">
+        <v>545</v>
+      </c>
+      <c r="D127" s="49" t="s">
         <v>546</v>
-      </c>
-      <c r="D127" s="49" t="s">
-        <v>547</v>
       </c>
       <c r="E127" s="49" t="s">
         <v>46</v>
@@ -10463,13 +10463,13 @@
         <v>1</v>
       </c>
       <c r="B129" s="49" t="s">
+        <v>323</v>
+      </c>
+      <c r="C129" s="49" t="s">
+        <v>400</v>
+      </c>
+      <c r="D129" s="49" t="s">
         <v>324</v>
-      </c>
-      <c r="C129" s="49" t="s">
-        <v>401</v>
-      </c>
-      <c r="D129" s="49" t="s">
-        <v>325</v>
       </c>
       <c r="E129" s="49" t="s">
         <v>46</v>
@@ -10522,13 +10522,13 @@
         <v>1</v>
       </c>
       <c r="B131" s="49" t="s">
+        <v>325</v>
+      </c>
+      <c r="C131" s="49" t="s">
+        <v>401</v>
+      </c>
+      <c r="D131" s="49" t="s">
         <v>326</v>
-      </c>
-      <c r="C131" s="49" t="s">
-        <v>402</v>
-      </c>
-      <c r="D131" s="49" t="s">
-        <v>327</v>
       </c>
       <c r="E131" s="49" t="s">
         <v>46</v>
@@ -10583,16 +10583,16 @@
       </c>
       <c r="C133" s="60"/>
       <c r="D133" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="E133" s="60" t="s">
         <v>328</v>
-      </c>
-      <c r="E133" s="60" t="s">
-        <v>329</v>
       </c>
       <c r="G133" s="60" t="s">
         <v>44</v>
       </c>
       <c r="H133" s="60" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I133" s="60">
         <v>10</v>
@@ -10603,13 +10603,13 @@
         <v>1</v>
       </c>
       <c r="B134" s="49" t="s">
+        <v>329</v>
+      </c>
+      <c r="C134" s="49" t="s">
+        <v>402</v>
+      </c>
+      <c r="D134" s="49" t="s">
         <v>330</v>
-      </c>
-      <c r="C134" s="49" t="s">
-        <v>403</v>
-      </c>
-      <c r="D134" s="49" t="s">
-        <v>331</v>
       </c>
       <c r="E134" s="49" t="s">
         <v>46</v>
@@ -10664,16 +10664,16 @@
       </c>
       <c r="C136" s="60"/>
       <c r="D136" s="60" t="s">
+        <v>331</v>
+      </c>
+      <c r="E136" s="60" t="s">
         <v>332</v>
-      </c>
-      <c r="E136" s="60" t="s">
-        <v>333</v>
       </c>
       <c r="G136" s="60" t="s">
         <v>44</v>
       </c>
       <c r="H136" s="60" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I136" s="60">
         <v>0.5</v>
@@ -10684,13 +10684,13 @@
         <v>1</v>
       </c>
       <c r="B137" s="49" t="s">
+        <v>532</v>
+      </c>
+      <c r="C137" s="49" t="s">
+        <v>547</v>
+      </c>
+      <c r="D137" s="49" t="s">
         <v>533</v>
-      </c>
-      <c r="C137" s="49" t="s">
-        <v>548</v>
-      </c>
-      <c r="D137" s="49" t="s">
-        <v>534</v>
       </c>
       <c r="E137" s="49" t="s">
         <v>48</v>
@@ -10743,13 +10743,13 @@
         <v>1</v>
       </c>
       <c r="B139" s="57" t="s">
+        <v>555</v>
+      </c>
+      <c r="C139" s="57" t="s">
+        <v>586</v>
+      </c>
+      <c r="D139" s="57" t="s">
         <v>556</v>
-      </c>
-      <c r="C139" s="57" t="s">
-        <v>587</v>
-      </c>
-      <c r="D139" s="57" t="s">
-        <v>557</v>
       </c>
       <c r="E139" s="57" t="s">
         <v>46</v>
@@ -10802,13 +10802,13 @@
         <v>1</v>
       </c>
       <c r="B141" s="57" t="s">
+        <v>557</v>
+      </c>
+      <c r="C141" s="57" t="s">
+        <v>587</v>
+      </c>
+      <c r="D141" s="57" t="s">
         <v>558</v>
-      </c>
-      <c r="C141" s="57" t="s">
-        <v>588</v>
-      </c>
-      <c r="D141" s="57" t="s">
-        <v>559</v>
       </c>
       <c r="E141" s="57" t="s">
         <v>48</v>
@@ -10861,13 +10861,13 @@
         <v>1</v>
       </c>
       <c r="B143" s="57" t="s">
+        <v>334</v>
+      </c>
+      <c r="C143" s="57" t="s">
+        <v>403</v>
+      </c>
+      <c r="D143" s="57" t="s">
         <v>335</v>
-      </c>
-      <c r="C143" s="57" t="s">
-        <v>404</v>
-      </c>
-      <c r="D143" s="57" t="s">
-        <v>336</v>
       </c>
       <c r="E143" s="57" t="s">
         <v>46</v>
@@ -10942,7 +10942,7 @@
       </c>
       <c r="C146" s="61"/>
       <c r="D146" s="61" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E146" s="61" t="s">
         <v>50</v>
@@ -10962,7 +10962,7 @@
       </c>
       <c r="C147" s="61"/>
       <c r="D147" s="61" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E147" s="61" t="s">
         <v>51</v>
@@ -10971,7 +10971,7 @@
         <v>44</v>
       </c>
       <c r="H147" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I147" s="61">
         <v>18</v>
@@ -10984,7 +10984,7 @@
       </c>
       <c r="C148" s="61"/>
       <c r="D148" s="61" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E148" s="61" t="s">
         <v>52</v>
@@ -10993,7 +10993,7 @@
         <v>44</v>
       </c>
       <c r="H148" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I148" s="61">
         <v>9</v>
@@ -11006,7 +11006,7 @@
       </c>
       <c r="C149" s="61"/>
       <c r="D149" s="61" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E149" s="61" t="s">
         <v>53</v>
@@ -11026,7 +11026,7 @@
       </c>
       <c r="C150" s="61"/>
       <c r="D150" s="61" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E150" s="61" t="s">
         <v>54</v>
@@ -11035,7 +11035,7 @@
         <v>44</v>
       </c>
       <c r="H150" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I150" s="61">
         <v>18</v>
@@ -11048,7 +11048,7 @@
       </c>
       <c r="C151" s="61"/>
       <c r="D151" s="61" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E151" s="61" t="s">
         <v>55</v>
@@ -11057,7 +11057,7 @@
         <v>44</v>
       </c>
       <c r="H151" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I151" s="61">
         <v>9</v>
@@ -11070,7 +11070,7 @@
       </c>
       <c r="C152" s="61"/>
       <c r="D152" s="61" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E152" s="61" t="s">
         <v>56</v>
@@ -11090,7 +11090,7 @@
       </c>
       <c r="C153" s="61"/>
       <c r="D153" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E153" s="61" t="s">
         <v>57</v>
@@ -11099,7 +11099,7 @@
         <v>44</v>
       </c>
       <c r="H153" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I153" s="61">
         <v>18</v>
@@ -11112,7 +11112,7 @@
       </c>
       <c r="C154" s="61"/>
       <c r="D154" s="61" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E154" s="61" t="s">
         <v>58</v>
@@ -11121,7 +11121,7 @@
         <v>44</v>
       </c>
       <c r="H154" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I154" s="61">
         <v>9</v>
@@ -11132,13 +11132,13 @@
         <v>1</v>
       </c>
       <c r="B155" s="57" t="s">
+        <v>559</v>
+      </c>
+      <c r="C155" s="57" t="s">
+        <v>588</v>
+      </c>
+      <c r="D155" s="57" t="s">
         <v>560</v>
-      </c>
-      <c r="C155" s="57" t="s">
-        <v>589</v>
-      </c>
-      <c r="D155" s="57" t="s">
-        <v>561</v>
       </c>
       <c r="E155" s="57" t="s">
         <v>48</v>
@@ -11191,13 +11191,13 @@
         <v>1</v>
       </c>
       <c r="B157" s="57" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C157" s="57" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D157" s="57" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E157" s="57" t="s">
         <v>46</v>
@@ -11211,7 +11211,7 @@
       </c>
       <c r="C158" s="61"/>
       <c r="D158" s="61" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E158" s="61" t="s">
         <v>254</v>
@@ -11271,7 +11271,7 @@
       </c>
       <c r="C160" s="61"/>
       <c r="D160" s="61" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E160" s="61" t="s">
         <v>50</v>
@@ -11291,7 +11291,7 @@
       </c>
       <c r="C161" s="61"/>
       <c r="D161" s="61" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E161" s="61" t="s">
         <v>51</v>
@@ -11300,7 +11300,7 @@
         <v>44</v>
       </c>
       <c r="H161" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I161" s="61">
         <v>18</v>
@@ -11313,7 +11313,7 @@
       </c>
       <c r="C162" s="61"/>
       <c r="D162" s="61" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E162" s="61" t="s">
         <v>52</v>
@@ -11322,7 +11322,7 @@
         <v>44</v>
       </c>
       <c r="H162" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I162" s="61">
         <v>9</v>
@@ -11335,7 +11335,7 @@
       </c>
       <c r="C163" s="61"/>
       <c r="D163" s="61" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E163" s="61" t="s">
         <v>53</v>
@@ -11355,7 +11355,7 @@
       </c>
       <c r="C164" s="61"/>
       <c r="D164" s="61" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E164" s="61" t="s">
         <v>54</v>
@@ -11364,7 +11364,7 @@
         <v>44</v>
       </c>
       <c r="H164" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I164" s="61">
         <v>18</v>
@@ -11377,7 +11377,7 @@
       </c>
       <c r="C165" s="61"/>
       <c r="D165" s="61" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E165" s="61" t="s">
         <v>55</v>
@@ -11386,7 +11386,7 @@
         <v>44</v>
       </c>
       <c r="H165" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I165" s="61">
         <v>9</v>
@@ -11399,7 +11399,7 @@
       </c>
       <c r="C166" s="61"/>
       <c r="D166" s="61" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E166" s="61" t="s">
         <v>56</v>
@@ -11419,7 +11419,7 @@
       </c>
       <c r="C167" s="61"/>
       <c r="D167" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E167" s="61" t="s">
         <v>57</v>
@@ -11428,7 +11428,7 @@
         <v>44</v>
       </c>
       <c r="H167" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I167" s="61">
         <v>18</v>
@@ -11441,7 +11441,7 @@
       </c>
       <c r="C168" s="61"/>
       <c r="D168" s="61" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E168" s="61" t="s">
         <v>58</v>
@@ -11450,7 +11450,7 @@
         <v>44</v>
       </c>
       <c r="H168" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I168" s="61">
         <v>9</v>
@@ -11461,13 +11461,13 @@
         <v>1</v>
       </c>
       <c r="B169" s="57" t="s">
+        <v>337</v>
+      </c>
+      <c r="C169" s="57" t="s">
+        <v>405</v>
+      </c>
+      <c r="D169" s="57" t="s">
         <v>338</v>
-      </c>
-      <c r="C169" s="57" t="s">
-        <v>406</v>
-      </c>
-      <c r="D169" s="57" t="s">
-        <v>339</v>
       </c>
       <c r="E169" s="57" t="s">
         <v>46</v>
@@ -11520,13 +11520,13 @@
         <v>1</v>
       </c>
       <c r="B171" s="57" t="s">
+        <v>561</v>
+      </c>
+      <c r="C171" s="57" t="s">
+        <v>589</v>
+      </c>
+      <c r="D171" s="57" t="s">
         <v>562</v>
-      </c>
-      <c r="C171" s="57" t="s">
-        <v>590</v>
-      </c>
-      <c r="D171" s="57" t="s">
-        <v>563</v>
       </c>
       <c r="E171" s="57" t="s">
         <v>46</v>
@@ -11581,10 +11581,10 @@
       </c>
       <c r="C173" s="61"/>
       <c r="D173" s="61" t="s">
+        <v>563</v>
+      </c>
+      <c r="E173" s="61" t="s">
         <v>564</v>
-      </c>
-      <c r="E173" s="61" t="s">
-        <v>565</v>
       </c>
       <c r="G173" s="61" t="s">
         <v>44</v>
@@ -11601,10 +11601,10 @@
       </c>
       <c r="C174" s="61"/>
       <c r="D174" s="61" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E174" s="61" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G174" s="61" t="s">
         <v>44</v>
@@ -11621,7 +11621,7 @@
       </c>
       <c r="C175" s="61"/>
       <c r="D175" s="61" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E175" s="61" t="s">
         <v>50</v>
@@ -11641,7 +11641,7 @@
       </c>
       <c r="C176" s="61"/>
       <c r="D176" s="61" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E176" s="61" t="s">
         <v>51</v>
@@ -11650,7 +11650,7 @@
         <v>44</v>
       </c>
       <c r="H176" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I176" s="61">
         <v>18</v>
@@ -11663,7 +11663,7 @@
       </c>
       <c r="C177" s="61"/>
       <c r="D177" s="61" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E177" s="61" t="s">
         <v>52</v>
@@ -11672,7 +11672,7 @@
         <v>44</v>
       </c>
       <c r="H177" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I177" s="61">
         <v>9</v>
@@ -11685,7 +11685,7 @@
       </c>
       <c r="C178" s="61"/>
       <c r="D178" s="61" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E178" s="61" t="s">
         <v>53</v>
@@ -11705,7 +11705,7 @@
       </c>
       <c r="C179" s="61"/>
       <c r="D179" s="61" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E179" s="61" t="s">
         <v>54</v>
@@ -11714,7 +11714,7 @@
         <v>44</v>
       </c>
       <c r="H179" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I179" s="61">
         <v>18</v>
@@ -11727,7 +11727,7 @@
       </c>
       <c r="C180" s="61"/>
       <c r="D180" s="61" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E180" s="61" t="s">
         <v>55</v>
@@ -11736,7 +11736,7 @@
         <v>44</v>
       </c>
       <c r="H180" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I180" s="61">
         <v>9</v>
@@ -11749,7 +11749,7 @@
       </c>
       <c r="C181" s="61"/>
       <c r="D181" s="61" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E181" s="61" t="s">
         <v>56</v>
@@ -11769,7 +11769,7 @@
       </c>
       <c r="C182" s="61"/>
       <c r="D182" s="61" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E182" s="61" t="s">
         <v>57</v>
@@ -11778,7 +11778,7 @@
         <v>44</v>
       </c>
       <c r="H182" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I182" s="61">
         <v>18</v>
@@ -11791,7 +11791,7 @@
       </c>
       <c r="C183" s="61"/>
       <c r="D183" s="61" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E183" s="61" t="s">
         <v>58</v>
@@ -11800,7 +11800,7 @@
         <v>44</v>
       </c>
       <c r="H183" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I183" s="61">
         <v>9</v>
@@ -11811,13 +11811,13 @@
         <v>1</v>
       </c>
       <c r="B184" s="57" t="s">
+        <v>339</v>
+      </c>
+      <c r="C184" s="57" t="s">
+        <v>417</v>
+      </c>
+      <c r="D184" s="57" t="s">
         <v>340</v>
-      </c>
-      <c r="C184" s="57" t="s">
-        <v>418</v>
-      </c>
-      <c r="D184" s="57" t="s">
-        <v>341</v>
       </c>
       <c r="E184" s="57" t="s">
         <v>46</v>
@@ -11872,16 +11872,16 @@
       </c>
       <c r="C186" s="61"/>
       <c r="D186" s="61" t="s">
+        <v>341</v>
+      </c>
+      <c r="E186" s="61" t="s">
         <v>342</v>
-      </c>
-      <c r="E186" s="61" t="s">
-        <v>343</v>
       </c>
       <c r="G186" s="61" t="s">
         <v>44</v>
       </c>
       <c r="H186" s="61" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I186" s="61">
         <v>20</v>
@@ -11892,13 +11892,13 @@
         <v>1</v>
       </c>
       <c r="B187" s="57" t="s">
+        <v>572</v>
+      </c>
+      <c r="C187" s="57" t="s">
+        <v>590</v>
+      </c>
+      <c r="D187" s="57" t="s">
         <v>573</v>
-      </c>
-      <c r="C187" s="57" t="s">
-        <v>591</v>
-      </c>
-      <c r="D187" s="57" t="s">
-        <v>574</v>
       </c>
       <c r="E187" s="57" t="s">
         <v>46</v>
@@ -11951,13 +11951,13 @@
         <v>1</v>
       </c>
       <c r="B189" s="57" t="s">
+        <v>574</v>
+      </c>
+      <c r="C189" s="57" t="s">
+        <v>591</v>
+      </c>
+      <c r="D189" s="57" t="s">
         <v>575</v>
-      </c>
-      <c r="C189" s="57" t="s">
-        <v>592</v>
-      </c>
-      <c r="D189" s="57" t="s">
-        <v>576</v>
       </c>
       <c r="E189" s="57" t="s">
         <v>46</v>
@@ -12012,16 +12012,16 @@
       </c>
       <c r="C191" s="61"/>
       <c r="D191" s="61" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E191" s="61" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G191" s="61" t="s">
         <v>44</v>
       </c>
       <c r="H191" s="61" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I191" s="61">
         <v>30</v>
@@ -12032,13 +12032,13 @@
         <v>1</v>
       </c>
       <c r="B192" s="57" t="s">
+        <v>577</v>
+      </c>
+      <c r="C192" s="57" t="s">
+        <v>592</v>
+      </c>
+      <c r="D192" s="57" t="s">
         <v>578</v>
-      </c>
-      <c r="C192" s="57" t="s">
-        <v>593</v>
-      </c>
-      <c r="D192" s="57" t="s">
-        <v>579</v>
       </c>
       <c r="E192" s="57" t="s">
         <v>48</v>
@@ -12091,13 +12091,13 @@
         <v>1</v>
       </c>
       <c r="B194" s="57" t="s">
+        <v>343</v>
+      </c>
+      <c r="C194" s="57" t="s">
+        <v>418</v>
+      </c>
+      <c r="D194" s="57" t="s">
         <v>344</v>
-      </c>
-      <c r="C194" s="57" t="s">
-        <v>419</v>
-      </c>
-      <c r="D194" s="57" t="s">
-        <v>345</v>
       </c>
       <c r="E194" s="57" t="s">
         <v>46</v>
@@ -12152,10 +12152,10 @@
       </c>
       <c r="C196" s="61"/>
       <c r="D196" s="61" t="s">
+        <v>345</v>
+      </c>
+      <c r="E196" s="61" t="s">
         <v>346</v>
-      </c>
-      <c r="E196" s="61" t="s">
-        <v>347</v>
       </c>
       <c r="G196" s="61" t="s">
         <v>44</v>
@@ -12172,16 +12172,16 @@
       </c>
       <c r="C197" s="61"/>
       <c r="D197" s="61" t="s">
+        <v>347</v>
+      </c>
+      <c r="E197" s="61" t="s">
         <v>348</v>
-      </c>
-      <c r="E197" s="61" t="s">
-        <v>349</v>
       </c>
       <c r="G197" s="61" t="s">
         <v>44</v>
       </c>
       <c r="H197" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I197" s="61">
         <v>9</v>
@@ -12194,16 +12194,16 @@
       </c>
       <c r="C198" s="61"/>
       <c r="D198" s="61" t="s">
+        <v>349</v>
+      </c>
+      <c r="E198" s="61" t="s">
         <v>350</v>
-      </c>
-      <c r="E198" s="61" t="s">
-        <v>351</v>
       </c>
       <c r="G198" s="61" t="s">
         <v>44</v>
       </c>
       <c r="H198" s="61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I198" s="61">
         <v>16</v>
@@ -12214,13 +12214,13 @@
         <v>1</v>
       </c>
       <c r="B199" s="57" t="s">
+        <v>351</v>
+      </c>
+      <c r="C199" s="57" t="s">
+        <v>419</v>
+      </c>
+      <c r="D199" s="57" t="s">
         <v>352</v>
-      </c>
-      <c r="C199" s="57" t="s">
-        <v>420</v>
-      </c>
-      <c r="D199" s="57" t="s">
-        <v>353</v>
       </c>
       <c r="E199" s="57" t="s">
         <v>46</v>
@@ -12275,7 +12275,7 @@
       </c>
       <c r="C201" s="61"/>
       <c r="D201" s="61" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E201" s="61" t="s">
         <v>41</v>
@@ -12284,7 +12284,7 @@
         <v>44</v>
       </c>
       <c r="H201" s="61" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I201" s="61">
         <v>20</v>
@@ -12295,13 +12295,13 @@
         <v>1</v>
       </c>
       <c r="B202" s="57" t="s">
+        <v>579</v>
+      </c>
+      <c r="C202" s="57" t="s">
+        <v>593</v>
+      </c>
+      <c r="D202" s="57" t="s">
         <v>580</v>
-      </c>
-      <c r="C202" s="57" t="s">
-        <v>594</v>
-      </c>
-      <c r="D202" s="57" t="s">
-        <v>581</v>
       </c>
       <c r="E202" s="57" t="s">
         <v>48</v>
@@ -12354,13 +12354,13 @@
         <v>1</v>
       </c>
       <c r="B204" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="C204" s="57" t="s">
+        <v>420</v>
+      </c>
+      <c r="D204" s="57" t="s">
         <v>355</v>
-      </c>
-      <c r="C204" s="57" t="s">
-        <v>421</v>
-      </c>
-      <c r="D204" s="57" t="s">
-        <v>356</v>
       </c>
       <c r="E204" s="57" t="s">
         <v>46</v>
@@ -12413,13 +12413,13 @@
         <v>1</v>
       </c>
       <c r="B206" s="57" t="s">
+        <v>356</v>
+      </c>
+      <c r="C206" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="D206" s="57" t="s">
         <v>357</v>
-      </c>
-      <c r="C206" s="57" t="s">
-        <v>422</v>
-      </c>
-      <c r="D206" s="57" t="s">
-        <v>358</v>
       </c>
       <c r="E206" s="57" t="s">
         <v>46</v>
@@ -12472,13 +12472,13 @@
         <v>1</v>
       </c>
       <c r="B208" s="57" t="s">
+        <v>581</v>
+      </c>
+      <c r="C208" s="57" t="s">
+        <v>594</v>
+      </c>
+      <c r="D208" s="57" t="s">
         <v>582</v>
-      </c>
-      <c r="C208" s="57" t="s">
-        <v>595</v>
-      </c>
-      <c r="D208" s="57" t="s">
-        <v>583</v>
       </c>
       <c r="E208" s="57" t="s">
         <v>46</v>
@@ -12531,13 +12531,13 @@
         <v>1</v>
       </c>
       <c r="B210" s="57" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C210" s="57" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D210" s="57" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E210" s="57" t="s">
         <v>46</v>
@@ -12590,13 +12590,13 @@
         <v>1</v>
       </c>
       <c r="B212" s="57" t="s">
+        <v>358</v>
+      </c>
+      <c r="C212" s="57" t="s">
+        <v>422</v>
+      </c>
+      <c r="D212" s="57" t="s">
         <v>359</v>
-      </c>
-      <c r="C212" s="57" t="s">
-        <v>423</v>
-      </c>
-      <c r="D212" s="57" t="s">
-        <v>360</v>
       </c>
       <c r="E212" s="57" t="s">
         <v>46</v>
@@ -12649,13 +12649,13 @@
         <v>1</v>
       </c>
       <c r="B214" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="C214" s="57" t="s">
+        <v>423</v>
+      </c>
+      <c r="D214" s="57" t="s">
         <v>361</v>
-      </c>
-      <c r="C214" s="57" t="s">
-        <v>424</v>
-      </c>
-      <c r="D214" s="57" t="s">
-        <v>362</v>
       </c>
       <c r="E214" s="57" t="s">
         <v>46</v>
@@ -12710,16 +12710,16 @@
       </c>
       <c r="C216" s="61"/>
       <c r="D216" s="61" t="s">
+        <v>362</v>
+      </c>
+      <c r="E216" s="61" t="s">
         <v>363</v>
-      </c>
-      <c r="E216" s="61" t="s">
-        <v>364</v>
       </c>
       <c r="G216" s="61" t="s">
         <v>44</v>
       </c>
       <c r="H216" s="61" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I216" s="61">
         <v>15</v>
@@ -12947,12 +12947,12 @@
     </row>
     <row r="7" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E7" s="34" t="s">
         <v>91</v>
@@ -13353,14 +13353,14 @@
     </row>
     <row r="21" spans="1:13" s="44" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="45" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C21" s="45"/>
       <c r="D21" s="45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E21" s="45"/>
       <c r="F21" s="45" t="s">
@@ -13382,13 +13382,13 @@
     </row>
     <row r="22" spans="1:13" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F22" s="46" t="s">
         <v>43</v>
@@ -13405,13 +13405,13 @@
     </row>
     <row r="23" spans="1:13" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>369</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>370</v>
       </c>
       <c r="F23" s="46" t="s">
         <v>43</v>
@@ -13428,13 +13428,13 @@
     </row>
     <row r="24" spans="1:13" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F24" s="46" t="s">
         <v>43</v>
@@ -13451,13 +13451,13 @@
     </row>
     <row r="25" spans="1:13" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F25" s="46" t="s">
         <v>43</v>
@@ -13474,13 +13474,13 @@
     </row>
     <row r="26" spans="1:13" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F26" s="46" t="s">
         <v>43</v>
@@ -13497,13 +13497,13 @@
     </row>
     <row r="27" spans="1:13" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F27" s="46" t="s">
         <v>43</v>
@@ -13520,13 +13520,13 @@
     </row>
     <row r="28" spans="1:13" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>382</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>383</v>
       </c>
       <c r="F28" s="46" t="s">
         <v>43</v>
@@ -13543,13 +13543,13 @@
     </row>
     <row r="29" spans="1:13" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>384</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>385</v>
       </c>
       <c r="F29" s="46" t="s">
         <v>43</v>
@@ -13566,13 +13566,13 @@
     </row>
     <row r="30" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>386</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>387</v>
       </c>
       <c r="F30" s="46" t="s">
         <v>43</v>
@@ -13589,13 +13589,13 @@
     </row>
     <row r="31" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F31" s="46" t="s">
         <v>43</v>
@@ -13612,13 +13612,13 @@
     </row>
     <row r="32" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F32" s="46" t="s">
         <v>43</v>
@@ -13635,13 +13635,13 @@
     </row>
     <row r="33" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F33" s="46" t="s">
         <v>43</v>
@@ -13658,13 +13658,13 @@
     </row>
     <row r="34" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>388</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>389</v>
       </c>
       <c r="F34" s="46" t="s">
         <v>43</v>
@@ -13681,13 +13681,13 @@
     </row>
     <row r="35" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="51" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D35" s="51" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F35" s="54" t="s">
         <v>43</v>
@@ -13704,13 +13704,13 @@
     </row>
     <row r="36" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="51" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B36" s="51" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D36" s="51" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F36" s="54" t="s">
         <v>43</v>
@@ -13727,13 +13727,13 @@
     </row>
     <row r="37" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="51" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B37" s="51" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D37" s="51" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F37" s="54" t="s">
         <v>43</v>
@@ -13750,13 +13750,13 @@
     </row>
     <row r="38" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="51" t="s">
+        <v>619</v>
+      </c>
+      <c r="B38" s="51" t="s">
+        <v>619</v>
+      </c>
+      <c r="D38" s="51" t="s">
         <v>620</v>
-      </c>
-      <c r="B38" s="51" t="s">
-        <v>620</v>
-      </c>
-      <c r="D38" s="51" t="s">
-        <v>621</v>
       </c>
       <c r="F38" s="54" t="s">
         <v>43</v>
@@ -13773,13 +13773,13 @@
     </row>
     <row r="39" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="51" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B39" s="51" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D39" s="51" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F39" s="54" t="s">
         <v>43</v>
@@ -13796,13 +13796,13 @@
     </row>
     <row r="40" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="51" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B40" s="51" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D40" s="51" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F40" s="54" t="s">
         <v>43</v>
@@ -13819,13 +13819,13 @@
     </row>
     <row r="41" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="51" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B41" s="51" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D41" s="51" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F41" s="54" t="s">
         <v>43</v>
@@ -13842,13 +13842,13 @@
     </row>
     <row r="42" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="51" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B42" s="51" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D42" s="51" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F42" s="54" t="s">
         <v>43</v>
@@ -13865,13 +13865,13 @@
     </row>
     <row r="43" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="51" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B43" s="51" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D43" s="51" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F43" s="54" t="s">
         <v>43</v>
@@ -13888,13 +13888,13 @@
     </row>
     <row r="44" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="51" t="s">
+        <v>390</v>
+      </c>
+      <c r="B44" s="51" t="s">
+        <v>390</v>
+      </c>
+      <c r="D44" s="51" t="s">
         <v>391</v>
-      </c>
-      <c r="B44" s="51" t="s">
-        <v>391</v>
-      </c>
-      <c r="D44" s="51" t="s">
-        <v>392</v>
       </c>
       <c r="F44" s="54" t="s">
         <v>43</v>
@@ -13911,13 +13911,13 @@
     </row>
     <row r="45" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="51" t="s">
+        <v>392</v>
+      </c>
+      <c r="B45" s="51" t="s">
+        <v>392</v>
+      </c>
+      <c r="D45" s="51" t="s">
         <v>393</v>
-      </c>
-      <c r="B45" s="51" t="s">
-        <v>393</v>
-      </c>
-      <c r="D45" s="51" t="s">
-        <v>394</v>
       </c>
       <c r="F45" s="54" t="s">
         <v>43</v>
@@ -13934,13 +13934,13 @@
     </row>
     <row r="46" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="49" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B46" s="49" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D46" s="49" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F46" s="53" t="s">
         <v>43</v>
@@ -13957,13 +13957,13 @@
     </row>
     <row r="47" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="49" t="s">
+        <v>617</v>
+      </c>
+      <c r="B47" s="49" t="s">
+        <v>617</v>
+      </c>
+      <c r="D47" s="49" t="s">
         <v>618</v>
-      </c>
-      <c r="B47" s="49" t="s">
-        <v>618</v>
-      </c>
-      <c r="D47" s="49" t="s">
-        <v>619</v>
       </c>
       <c r="F47" s="53" t="s">
         <v>43</v>
@@ -13980,13 +13980,13 @@
     </row>
     <row r="48" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="49" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B48" s="49" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D48" s="49" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F48" s="53" t="s">
         <v>43</v>
@@ -14003,13 +14003,13 @@
     </row>
     <row r="49" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="49" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B49" s="49" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D49" s="49" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F49" s="53" t="s">
         <v>43</v>
@@ -14026,13 +14026,13 @@
     </row>
     <row r="50" spans="1:9" s="49" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="49" t="s">
+        <v>394</v>
+      </c>
+      <c r="B50" s="49" t="s">
+        <v>394</v>
+      </c>
+      <c r="D50" s="49" t="s">
         <v>395</v>
-      </c>
-      <c r="B50" s="49" t="s">
-        <v>395</v>
-      </c>
-      <c r="D50" s="49" t="s">
-        <v>396</v>
       </c>
       <c r="F50" s="53" t="s">
         <v>43</v>
@@ -14049,13 +14049,13 @@
     </row>
     <row r="51" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="49" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B51" s="49" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D51" s="49" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F51" s="53" t="s">
         <v>43</v>
@@ -14072,13 +14072,13 @@
     </row>
     <row r="52" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="49" t="s">
+        <v>396</v>
+      </c>
+      <c r="B52" s="49" t="s">
+        <v>396</v>
+      </c>
+      <c r="D52" s="49" t="s">
         <v>397</v>
-      </c>
-      <c r="B52" s="49" t="s">
-        <v>397</v>
-      </c>
-      <c r="D52" s="49" t="s">
-        <v>398</v>
       </c>
       <c r="F52" s="53" t="s">
         <v>43</v>
@@ -14095,13 +14095,13 @@
     </row>
     <row r="53" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="49" t="s">
+        <v>398</v>
+      </c>
+      <c r="B53" s="49" t="s">
+        <v>398</v>
+      </c>
+      <c r="D53" s="49" t="s">
         <v>399</v>
-      </c>
-      <c r="B53" s="49" t="s">
-        <v>399</v>
-      </c>
-      <c r="D53" s="49" t="s">
-        <v>400</v>
       </c>
       <c r="F53" s="53" t="s">
         <v>43</v>
@@ -14118,13 +14118,13 @@
     </row>
     <row r="54" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="49" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B54" s="49" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D54" s="49" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F54" s="53" t="s">
         <v>43</v>
@@ -14141,13 +14141,13 @@
     </row>
     <row r="55" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49" t="s">
+        <v>621</v>
+      </c>
+      <c r="B55" s="49" t="s">
+        <v>621</v>
+      </c>
+      <c r="D55" s="49" t="s">
         <v>622</v>
-      </c>
-      <c r="B55" s="49" t="s">
-        <v>622</v>
-      </c>
-      <c r="D55" s="49" t="s">
-        <v>623</v>
       </c>
       <c r="F55" s="53" t="s">
         <v>43</v>
@@ -14164,13 +14164,13 @@
     </row>
     <row r="56" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="49" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B56" s="49" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D56" s="49" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F56" s="53" t="s">
         <v>43</v>
@@ -14187,13 +14187,13 @@
     </row>
     <row r="57" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="49" t="s">
+        <v>406</v>
+      </c>
+      <c r="B57" s="49" t="s">
+        <v>406</v>
+      </c>
+      <c r="D57" s="49" t="s">
         <v>407</v>
-      </c>
-      <c r="B57" s="49" t="s">
-        <v>407</v>
-      </c>
-      <c r="D57" s="49" t="s">
-        <v>408</v>
       </c>
       <c r="F57" s="53" t="s">
         <v>43</v>
@@ -14210,13 +14210,13 @@
     </row>
     <row r="58" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="49" t="s">
+        <v>408</v>
+      </c>
+      <c r="B58" s="49" t="s">
+        <v>408</v>
+      </c>
+      <c r="D58" s="49" t="s">
         <v>409</v>
-      </c>
-      <c r="B58" s="49" t="s">
-        <v>409</v>
-      </c>
-      <c r="D58" s="49" t="s">
-        <v>410</v>
       </c>
       <c r="F58" s="53" t="s">
         <v>43</v>
@@ -14233,13 +14233,13 @@
     </row>
     <row r="59" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="49" t="s">
+        <v>410</v>
+      </c>
+      <c r="B59" s="49" t="s">
+        <v>410</v>
+      </c>
+      <c r="D59" s="49" t="s">
         <v>411</v>
-      </c>
-      <c r="B59" s="49" t="s">
-        <v>411</v>
-      </c>
-      <c r="D59" s="49" t="s">
-        <v>412</v>
       </c>
       <c r="F59" s="53" t="s">
         <v>43</v>
@@ -14256,13 +14256,13 @@
     </row>
     <row r="60" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="49" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B60" s="49" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D60" s="49" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F60" s="53" t="s">
         <v>43</v>
@@ -14279,13 +14279,13 @@
     </row>
     <row r="61" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="57" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B61" s="57" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D61" s="57" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F61" s="59" t="s">
         <v>43</v>
@@ -14302,13 +14302,13 @@
     </row>
     <row r="62" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="57" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B62" s="57" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D62" s="57" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F62" s="59" t="s">
         <v>43</v>
@@ -14325,13 +14325,13 @@
     </row>
     <row r="63" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="57" t="s">
+        <v>412</v>
+      </c>
+      <c r="B63" s="57" t="s">
+        <v>412</v>
+      </c>
+      <c r="D63" s="57" t="s">
         <v>413</v>
-      </c>
-      <c r="B63" s="57" t="s">
-        <v>413</v>
-      </c>
-      <c r="D63" s="57" t="s">
-        <v>414</v>
       </c>
       <c r="F63" s="59" t="s">
         <v>43</v>
@@ -14348,13 +14348,13 @@
     </row>
     <row r="64" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="57" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B64" s="57" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D64" s="57" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F64" s="59" t="s">
         <v>43</v>
@@ -14371,13 +14371,13 @@
     </row>
     <row r="65" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="57" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B65" s="57" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D65" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F65" s="59" t="s">
         <v>43</v>
@@ -14394,13 +14394,13 @@
     </row>
     <row r="66" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="57" t="s">
+        <v>415</v>
+      </c>
+      <c r="B66" s="57" t="s">
+        <v>415</v>
+      </c>
+      <c r="D66" s="57" t="s">
         <v>416</v>
-      </c>
-      <c r="B66" s="57" t="s">
-        <v>416</v>
-      </c>
-      <c r="D66" s="57" t="s">
-        <v>417</v>
       </c>
       <c r="F66" s="59" t="s">
         <v>43</v>
@@ -14417,13 +14417,13 @@
     </row>
     <row r="67" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="57" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B67" s="57" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D67" s="57" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F67" s="59" t="s">
         <v>43</v>
@@ -14440,13 +14440,13 @@
     </row>
     <row r="68" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="57" t="s">
+        <v>424</v>
+      </c>
+      <c r="B68" s="57" t="s">
+        <v>424</v>
+      </c>
+      <c r="D68" s="57" t="s">
         <v>425</v>
-      </c>
-      <c r="B68" s="57" t="s">
-        <v>425</v>
-      </c>
-      <c r="D68" s="57" t="s">
-        <v>426</v>
       </c>
       <c r="F68" s="59" t="s">
         <v>43</v>
@@ -14463,13 +14463,13 @@
     </row>
     <row r="69" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="57" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B69" s="57" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D69" s="57" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F69" s="59" t="s">
         <v>43</v>
@@ -14486,13 +14486,13 @@
     </row>
     <row r="70" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="57" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B70" s="57" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D70" s="57" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F70" s="59" t="s">
         <v>43</v>
@@ -14509,13 +14509,13 @@
     </row>
     <row r="71" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="57" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B71" s="57" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D71" s="57" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F71" s="59" t="s">
         <v>43</v>
@@ -14532,13 +14532,13 @@
     </row>
     <row r="72" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="57" t="s">
+        <v>623</v>
+      </c>
+      <c r="B72" s="57" t="s">
+        <v>623</v>
+      </c>
+      <c r="D72" s="57" t="s">
         <v>624</v>
-      </c>
-      <c r="B72" s="57" t="s">
-        <v>624</v>
-      </c>
-      <c r="D72" s="57" t="s">
-        <v>625</v>
       </c>
       <c r="F72" s="59" t="s">
         <v>43</v>
@@ -14555,13 +14555,13 @@
     </row>
     <row r="73" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="57" t="s">
+        <v>426</v>
+      </c>
+      <c r="B73" s="57" t="s">
+        <v>426</v>
+      </c>
+      <c r="D73" s="57" t="s">
         <v>427</v>
-      </c>
-      <c r="B73" s="57" t="s">
-        <v>427</v>
-      </c>
-      <c r="D73" s="57" t="s">
-        <v>428</v>
       </c>
       <c r="F73" s="59" t="s">
         <v>43</v>
@@ -14578,13 +14578,13 @@
     </row>
     <row r="74" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="57" t="s">
+        <v>428</v>
+      </c>
+      <c r="B74" s="57" t="s">
+        <v>428</v>
+      </c>
+      <c r="D74" s="57" t="s">
         <v>429</v>
-      </c>
-      <c r="B74" s="57" t="s">
-        <v>429</v>
-      </c>
-      <c r="D74" s="57" t="s">
-        <v>430</v>
       </c>
       <c r="F74" s="59" t="s">
         <v>43</v>
@@ -14601,13 +14601,13 @@
     </row>
     <row r="75" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="57" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B75" s="57" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D75" s="57" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F75" s="59" t="s">
         <v>43</v>
@@ -14624,13 +14624,13 @@
     </row>
     <row r="76" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="57" t="s">
+        <v>430</v>
+      </c>
+      <c r="B76" s="57" t="s">
+        <v>430</v>
+      </c>
+      <c r="D76" s="57" t="s">
         <v>431</v>
-      </c>
-      <c r="B76" s="57" t="s">
-        <v>431</v>
-      </c>
-      <c r="D76" s="57" t="s">
-        <v>432</v>
       </c>
       <c r="F76" s="59" t="s">
         <v>43</v>
@@ -14647,13 +14647,13 @@
     </row>
     <row r="77" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="57" t="s">
+        <v>432</v>
+      </c>
+      <c r="B77" s="57" t="s">
+        <v>432</v>
+      </c>
+      <c r="D77" s="57" t="s">
         <v>433</v>
-      </c>
-      <c r="B77" s="57" t="s">
-        <v>433</v>
-      </c>
-      <c r="D77" s="57" t="s">
-        <v>434</v>
       </c>
       <c r="F77" s="59" t="s">
         <v>43</v>
@@ -14670,13 +14670,13 @@
     </row>
     <row r="78" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="57" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B78" s="57" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D78" s="57" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F78" s="59" t="s">
         <v>43</v>
@@ -14693,13 +14693,13 @@
     </row>
     <row r="79" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="57" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B79" s="57" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D79" s="57" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F79" s="59" t="s">
         <v>43</v>
@@ -14716,13 +14716,13 @@
     </row>
     <row r="80" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="57" t="s">
+        <v>434</v>
+      </c>
+      <c r="B80" s="57" t="s">
+        <v>434</v>
+      </c>
+      <c r="D80" s="57" t="s">
         <v>435</v>
-      </c>
-      <c r="B80" s="57" t="s">
-        <v>435</v>
-      </c>
-      <c r="D80" s="57" t="s">
-        <v>436</v>
       </c>
       <c r="F80" s="59" t="s">
         <v>43</v>
@@ -14739,13 +14739,13 @@
     </row>
     <row r="81" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="57" t="s">
+        <v>436</v>
+      </c>
+      <c r="B81" s="57" t="s">
+        <v>436</v>
+      </c>
+      <c r="D81" s="57" t="s">
         <v>437</v>
-      </c>
-      <c r="B81" s="57" t="s">
-        <v>437</v>
-      </c>
-      <c r="D81" s="57" t="s">
-        <v>438</v>
       </c>
       <c r="F81" s="59" t="s">
         <v>43</v>

</xml_diff>